<commit_message>
Fin du Crud Mysql
  - Pour la suite, Il va falloir Apprendre la base de Express
  - Faire une appli CRUD Mongoose qui utilise, Debug, colors, et autres modules
</commit_message>
<xml_diff>
--- a/Cahier des charges/Organisation Projet Nodejs.xlsx
+++ b/Cahier des charges/Organisation Projet Nodejs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z2j9457\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\MyEnv\NodeJs\Cahier des charges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4E92B6-3CD2-42DD-B071-9733733741B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D14DD30-0FFA-4991-A7A9-997F9B750E6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{D1074EF0-41CD-437C-83BE-5015162961C9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="3" xr2:uid="{D1074EF0-41CD-437C-83BE-5015162961C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="423">
   <si>
     <t>Check bin sheet for more informations</t>
     <phoneticPr fontId="1"/>
@@ -2616,6 +2616,111 @@
   </si>
   <si>
     <t>every</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Importance</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>realisation avant le</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Avec L'xp ca viendra</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>tuto plus solo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>EJS + MONGOOSE a test
+Creer une rest API avec ca</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>tracking + Excel</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Generator</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mysql</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>generator + tracking</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;= faire ca avec une database Mongoose et transformer le tout en rest API</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Essayer de refaire le CRUD avec Joi/ejs/validator/Mongoose</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Essayer maintenant !!!</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>revoir une doc vite fait</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Le prochain projet de Mongoose se fera sous PM2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CRUD_Mongoose</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>generator</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>security</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Pas tout de suite</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Aujourd'hui</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Plus tard</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Mongoose CRUD </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>pas tout de suite</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mongoose/generator/etc..</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3241,7 +3346,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3413,60 +3518,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -3531,6 +3582,75 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -8319,7 +8439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471BD040-1E5E-4739-AB8B-4F419BB83EB3}">
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A109" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
@@ -8396,95 +8516,95 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="25.5" x14ac:dyDescent="0.4">
-      <c r="A10" s="95"/>
-      <c r="B10" s="96" t="s">
+      <c r="A10" s="77"/>
+      <c r="B10" s="78" t="s">
         <v>380</v>
       </c>
-      <c r="C10" s="95"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="95"/>
-      <c r="F10" s="95"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="95"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="77"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="77"/>
     </row>
     <row r="14" spans="1:8" ht="25.5" x14ac:dyDescent="0.4">
-      <c r="A14" s="94">
+      <c r="A14" s="76">
         <v>1</v>
       </c>
-      <c r="B14" s="94" t="s">
+      <c r="B14" s="76" t="s">
         <v>379</v>
       </c>
-      <c r="C14" s="93"/>
-      <c r="D14" s="90" t="s">
+      <c r="C14" s="75"/>
+      <c r="D14" s="72" t="s">
         <v>378</v>
       </c>
-      <c r="E14" s="92" t="s">
+      <c r="E14" s="74" t="s">
         <v>377</v>
       </c>
-      <c r="F14" s="90"/>
-      <c r="G14" s="90"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="72"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B15" s="88" t="s">
+      <c r="B15" s="70" t="s">
         <v>376</v>
       </c>
-      <c r="D15" s="90"/>
-      <c r="E15" s="91" t="s">
+      <c r="D15" s="72"/>
+      <c r="E15" s="73" t="s">
         <v>375</v>
       </c>
-      <c r="F15" s="90"/>
-      <c r="G15" s="90"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="72"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B16" s="89"/>
+      <c r="B16" s="71"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B17" s="87" t="s">
+      <c r="B17" s="69" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B18" s="88" t="s">
+      <c r="B18" s="70" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B19" s="87" t="s">
+      <c r="B19" s="69" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B20" s="87" t="s">
+      <c r="B20" s="69" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B21" s="87" t="s">
+      <c r="B21" s="69" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B22" s="87" t="s">
+      <c r="B22" s="69" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B23" s="87" t="s">
+      <c r="B23" s="69" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B24" s="87" t="s">
+      <c r="B24" s="69" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B25" s="87" t="s">
+      <c r="B25" s="69" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B26" s="86" t="s">
+      <c r="B26" s="68" t="s">
         <v>365</v>
       </c>
     </row>
@@ -8549,17 +8669,17 @@
       </c>
     </row>
     <row r="42" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="85" t="s">
+      <c r="A42" s="67" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="82" t="s">
+      <c r="A43" s="64" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A44" s="84"/>
+      <c r="A44" s="66"/>
     </row>
     <row r="45" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
@@ -8567,22 +8687,22 @@
       </c>
     </row>
     <row r="46" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="83" t="s">
+      <c r="A46" s="65" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="82" t="s">
+      <c r="A47" s="64" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="81" t="s">
+      <c r="A48" s="63" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="81" t="s">
+      <c r="A49" s="63" t="s">
         <v>346</v>
       </c>
     </row>
@@ -8607,223 +8727,223 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A67" s="75" t="s">
+      <c r="A67" s="57" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A68" s="75" t="s">
+      <c r="A68" s="57" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A69" s="75" t="s">
+      <c r="A69" s="57" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A70" s="75" t="s">
+      <c r="A70" s="57" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="71" spans="1:7" s="79" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="80" t="s">
+    <row r="71" spans="1:7" s="61" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A71" s="62" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A72" s="75" t="s">
+      <c r="A72" s="57" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A73" s="75" t="s">
+      <c r="A73" s="57" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A74" s="75" t="s">
+      <c r="A74" s="57" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A75" s="75" t="s">
+      <c r="A75" s="57" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A76" s="75" t="s">
+      <c r="A76" s="57" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="77" spans="1:7" s="79" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A77" s="80" t="s">
+    <row r="77" spans="1:7" s="61" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A77" s="62" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="78" spans="1:7" s="79" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="80" t="s">
+    <row r="78" spans="1:7" s="61" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="62" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="79" spans="1:7" s="79" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="80" t="s">
+    <row r="79" spans="1:7" s="61" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="62" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="80" spans="1:7" s="79" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="80" t="s">
+    <row r="80" spans="1:7" s="61" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A80" s="62" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="81" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="80" t="s">
+    <row r="81" spans="1:1" s="61" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A81" s="62" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="82" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="80" t="s">
+    <row r="82" spans="1:1" s="61" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="62" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="83" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="80" t="s">
+    <row r="83" spans="1:1" s="61" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A83" s="62" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="84" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="80" t="s">
+    <row r="84" spans="1:1" s="61" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="62" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="85" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="80" t="s">
+    <row r="85" spans="1:1" s="61" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A85" s="62" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A86" s="75" t="s">
+      <c r="A86" s="57" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A87" s="75" t="s">
+      <c r="A87" s="57" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A88" s="75" t="s">
+      <c r="A88" s="57" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A89" s="75" t="s">
+      <c r="A89" s="57" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A90" s="75" t="s">
+      <c r="A90" s="57" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A91" s="75" t="s">
+      <c r="A91" s="57" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A92" s="75" t="s">
+      <c r="A92" s="57" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A93" s="75" t="s">
+      <c r="A93" s="57" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A94" s="75" t="s">
+      <c r="A94" s="57" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A95" s="75" t="s">
+      <c r="A95" s="57" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A96" s="75" t="s">
+      <c r="A96" s="57" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A97" s="75" t="s">
+      <c r="A97" s="57" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A98" s="77"/>
+      <c r="A98" s="59"/>
     </row>
     <row r="99" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A99" s="78" t="s">
+      <c r="A99" s="60" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A100" s="75" t="s">
+      <c r="A100" s="57" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A101" s="75" t="s">
+      <c r="A101" s="57" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A102" s="75" t="s">
+      <c r="A102" s="57" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="103" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A103" s="77"/>
+      <c r="A103" s="59"/>
     </row>
     <row r="104" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A104" s="76" t="s">
+      <c r="A104" s="58" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A105" s="75" t="s">
+      <c r="A105" s="57" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A106" s="75" t="s">
+      <c r="A106" s="57" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A107" s="75" t="s">
+      <c r="A107" s="57" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A108" s="75" t="s">
+      <c r="A108" s="57" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A109" s="75" t="s">
+      <c r="A109" s="57" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A110" s="75" t="s">
+      <c r="A110" s="57" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A111" s="75" t="s">
+      <c r="A111" s="57" t="s">
         <v>299</v>
       </c>
     </row>
@@ -8888,276 +9008,276 @@
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="2" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K2" s="57" t="s">
+      <c r="K2" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="58"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="58"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="58"/>
-      <c r="W2" s="58"/>
-      <c r="X2" s="59"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="80"/>
+      <c r="T2" s="80"/>
+      <c r="U2" s="80"/>
+      <c r="V2" s="80"/>
+      <c r="W2" s="80"/>
+      <c r="X2" s="81"/>
     </row>
     <row r="3" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K3" s="60"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
-      <c r="P3" s="61"/>
-      <c r="Q3" s="61"/>
-      <c r="R3" s="61"/>
-      <c r="S3" s="61"/>
-      <c r="T3" s="61"/>
-      <c r="U3" s="61"/>
-      <c r="V3" s="61"/>
-      <c r="W3" s="61"/>
-      <c r="X3" s="62"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="83"/>
+      <c r="P3" s="83"/>
+      <c r="Q3" s="83"/>
+      <c r="R3" s="83"/>
+      <c r="S3" s="83"/>
+      <c r="T3" s="83"/>
+      <c r="U3" s="83"/>
+      <c r="V3" s="83"/>
+      <c r="W3" s="83"/>
+      <c r="X3" s="84"/>
     </row>
     <row r="6" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K6" s="57" t="s">
+      <c r="K6" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="58"/>
-      <c r="O6" s="58"/>
-      <c r="P6" s="58"/>
-      <c r="Q6" s="58"/>
-      <c r="R6" s="58"/>
-      <c r="S6" s="58"/>
-      <c r="T6" s="58"/>
-      <c r="U6" s="58"/>
-      <c r="V6" s="58"/>
-      <c r="W6" s="58"/>
-      <c r="X6" s="59"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="80"/>
+      <c r="N6" s="80"/>
+      <c r="O6" s="80"/>
+      <c r="P6" s="80"/>
+      <c r="Q6" s="80"/>
+      <c r="R6" s="80"/>
+      <c r="S6" s="80"/>
+      <c r="T6" s="80"/>
+      <c r="U6" s="80"/>
+      <c r="V6" s="80"/>
+      <c r="W6" s="80"/>
+      <c r="X6" s="81"/>
     </row>
     <row r="7" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K7" s="60"/>
-      <c r="L7" s="61"/>
-      <c r="M7" s="61"/>
-      <c r="N7" s="61"/>
-      <c r="O7" s="61"/>
-      <c r="P7" s="61"/>
-      <c r="Q7" s="61"/>
-      <c r="R7" s="61"/>
-      <c r="S7" s="61"/>
-      <c r="T7" s="61"/>
-      <c r="U7" s="61"/>
-      <c r="V7" s="61"/>
-      <c r="W7" s="61"/>
-      <c r="X7" s="62"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="83"/>
+      <c r="M7" s="83"/>
+      <c r="N7" s="83"/>
+      <c r="O7" s="83"/>
+      <c r="P7" s="83"/>
+      <c r="Q7" s="83"/>
+      <c r="R7" s="83"/>
+      <c r="S7" s="83"/>
+      <c r="T7" s="83"/>
+      <c r="U7" s="83"/>
+      <c r="V7" s="83"/>
+      <c r="W7" s="83"/>
+      <c r="X7" s="84"/>
     </row>
     <row r="10" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K10" s="63" t="s">
+      <c r="K10" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="L10" s="64"/>
-      <c r="M10" s="64"/>
-      <c r="N10" s="64"/>
-      <c r="O10" s="64"/>
-      <c r="P10" s="64"/>
-      <c r="Q10" s="64"/>
-      <c r="R10" s="64"/>
-      <c r="S10" s="64"/>
-      <c r="T10" s="64"/>
-      <c r="U10" s="64"/>
-      <c r="V10" s="64"/>
-      <c r="W10" s="64"/>
-      <c r="X10" s="65"/>
+      <c r="L10" s="86"/>
+      <c r="M10" s="86"/>
+      <c r="N10" s="86"/>
+      <c r="O10" s="86"/>
+      <c r="P10" s="86"/>
+      <c r="Q10" s="86"/>
+      <c r="R10" s="86"/>
+      <c r="S10" s="86"/>
+      <c r="T10" s="86"/>
+      <c r="U10" s="86"/>
+      <c r="V10" s="86"/>
+      <c r="W10" s="86"/>
+      <c r="X10" s="87"/>
     </row>
     <row r="11" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K11" s="66"/>
-      <c r="L11" s="67"/>
-      <c r="M11" s="67"/>
-      <c r="N11" s="67"/>
-      <c r="O11" s="67"/>
-      <c r="P11" s="67"/>
-      <c r="Q11" s="67"/>
-      <c r="R11" s="67"/>
-      <c r="S11" s="67"/>
-      <c r="T11" s="67"/>
-      <c r="U11" s="67"/>
-      <c r="V11" s="67"/>
-      <c r="W11" s="67"/>
-      <c r="X11" s="68"/>
+      <c r="K11" s="88"/>
+      <c r="L11" s="89"/>
+      <c r="M11" s="89"/>
+      <c r="N11" s="89"/>
+      <c r="O11" s="89"/>
+      <c r="P11" s="89"/>
+      <c r="Q11" s="89"/>
+      <c r="R11" s="89"/>
+      <c r="S11" s="89"/>
+      <c r="T11" s="89"/>
+      <c r="U11" s="89"/>
+      <c r="V11" s="89"/>
+      <c r="W11" s="89"/>
+      <c r="X11" s="90"/>
     </row>
     <row r="14" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K14" s="57" t="s">
+      <c r="K14" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="L14" s="58"/>
-      <c r="M14" s="58"/>
-      <c r="N14" s="58"/>
-      <c r="O14" s="58"/>
-      <c r="P14" s="58"/>
-      <c r="Q14" s="58"/>
-      <c r="R14" s="58"/>
-      <c r="S14" s="58"/>
-      <c r="T14" s="58"/>
-      <c r="U14" s="58"/>
-      <c r="V14" s="58"/>
-      <c r="W14" s="58"/>
-      <c r="X14" s="59"/>
+      <c r="L14" s="80"/>
+      <c r="M14" s="80"/>
+      <c r="N14" s="80"/>
+      <c r="O14" s="80"/>
+      <c r="P14" s="80"/>
+      <c r="Q14" s="80"/>
+      <c r="R14" s="80"/>
+      <c r="S14" s="80"/>
+      <c r="T14" s="80"/>
+      <c r="U14" s="80"/>
+      <c r="V14" s="80"/>
+      <c r="W14" s="80"/>
+      <c r="X14" s="81"/>
     </row>
     <row r="15" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K15" s="60"/>
-      <c r="L15" s="61"/>
-      <c r="M15" s="61"/>
-      <c r="N15" s="61"/>
-      <c r="O15" s="61"/>
-      <c r="P15" s="61"/>
-      <c r="Q15" s="61"/>
-      <c r="R15" s="61"/>
-      <c r="S15" s="61"/>
-      <c r="T15" s="61"/>
-      <c r="U15" s="61"/>
-      <c r="V15" s="61"/>
-      <c r="W15" s="61"/>
-      <c r="X15" s="62"/>
+      <c r="K15" s="82"/>
+      <c r="L15" s="83"/>
+      <c r="M15" s="83"/>
+      <c r="N15" s="83"/>
+      <c r="O15" s="83"/>
+      <c r="P15" s="83"/>
+      <c r="Q15" s="83"/>
+      <c r="R15" s="83"/>
+      <c r="S15" s="83"/>
+      <c r="T15" s="83"/>
+      <c r="U15" s="83"/>
+      <c r="V15" s="83"/>
+      <c r="W15" s="83"/>
+      <c r="X15" s="84"/>
     </row>
     <row r="18" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K18" s="57" t="s">
+      <c r="K18" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="L18" s="58"/>
-      <c r="M18" s="58"/>
-      <c r="N18" s="58"/>
-      <c r="O18" s="58"/>
-      <c r="P18" s="58"/>
-      <c r="Q18" s="58"/>
-      <c r="R18" s="58"/>
-      <c r="S18" s="58"/>
-      <c r="T18" s="58"/>
-      <c r="U18" s="58"/>
-      <c r="V18" s="58"/>
-      <c r="W18" s="58"/>
-      <c r="X18" s="59"/>
+      <c r="L18" s="80"/>
+      <c r="M18" s="80"/>
+      <c r="N18" s="80"/>
+      <c r="O18" s="80"/>
+      <c r="P18" s="80"/>
+      <c r="Q18" s="80"/>
+      <c r="R18" s="80"/>
+      <c r="S18" s="80"/>
+      <c r="T18" s="80"/>
+      <c r="U18" s="80"/>
+      <c r="V18" s="80"/>
+      <c r="W18" s="80"/>
+      <c r="X18" s="81"/>
     </row>
     <row r="19" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K19" s="60"/>
-      <c r="L19" s="61"/>
-      <c r="M19" s="61"/>
-      <c r="N19" s="61"/>
-      <c r="O19" s="61"/>
-      <c r="P19" s="61"/>
-      <c r="Q19" s="61"/>
-      <c r="R19" s="61"/>
-      <c r="S19" s="61"/>
-      <c r="T19" s="61"/>
-      <c r="U19" s="61"/>
-      <c r="V19" s="61"/>
-      <c r="W19" s="61"/>
-      <c r="X19" s="62"/>
+      <c r="K19" s="82"/>
+      <c r="L19" s="83"/>
+      <c r="M19" s="83"/>
+      <c r="N19" s="83"/>
+      <c r="O19" s="83"/>
+      <c r="P19" s="83"/>
+      <c r="Q19" s="83"/>
+      <c r="R19" s="83"/>
+      <c r="S19" s="83"/>
+      <c r="T19" s="83"/>
+      <c r="U19" s="83"/>
+      <c r="V19" s="83"/>
+      <c r="W19" s="83"/>
+      <c r="X19" s="84"/>
     </row>
     <row r="22" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K22" s="57" t="s">
+      <c r="K22" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="L22" s="58"/>
-      <c r="M22" s="58"/>
-      <c r="N22" s="58"/>
-      <c r="O22" s="58"/>
-      <c r="P22" s="58"/>
-      <c r="Q22" s="58"/>
-      <c r="R22" s="58"/>
-      <c r="S22" s="58"/>
-      <c r="T22" s="58"/>
-      <c r="U22" s="58"/>
-      <c r="V22" s="58"/>
-      <c r="W22" s="58"/>
-      <c r="X22" s="59"/>
+      <c r="L22" s="80"/>
+      <c r="M22" s="80"/>
+      <c r="N22" s="80"/>
+      <c r="O22" s="80"/>
+      <c r="P22" s="80"/>
+      <c r="Q22" s="80"/>
+      <c r="R22" s="80"/>
+      <c r="S22" s="80"/>
+      <c r="T22" s="80"/>
+      <c r="U22" s="80"/>
+      <c r="V22" s="80"/>
+      <c r="W22" s="80"/>
+      <c r="X22" s="81"/>
     </row>
     <row r="23" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K23" s="60"/>
-      <c r="L23" s="61"/>
-      <c r="M23" s="61"/>
-      <c r="N23" s="61"/>
-      <c r="O23" s="61"/>
-      <c r="P23" s="61"/>
-      <c r="Q23" s="61"/>
-      <c r="R23" s="61"/>
-      <c r="S23" s="61"/>
-      <c r="T23" s="61"/>
-      <c r="U23" s="61"/>
-      <c r="V23" s="61"/>
-      <c r="W23" s="61"/>
-      <c r="X23" s="62"/>
+      <c r="K23" s="82"/>
+      <c r="L23" s="83"/>
+      <c r="M23" s="83"/>
+      <c r="N23" s="83"/>
+      <c r="O23" s="83"/>
+      <c r="P23" s="83"/>
+      <c r="Q23" s="83"/>
+      <c r="R23" s="83"/>
+      <c r="S23" s="83"/>
+      <c r="T23" s="83"/>
+      <c r="U23" s="83"/>
+      <c r="V23" s="83"/>
+      <c r="W23" s="83"/>
+      <c r="X23" s="84"/>
     </row>
     <row r="26" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K26" s="57" t="s">
+      <c r="K26" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="L26" s="58"/>
-      <c r="M26" s="58"/>
-      <c r="N26" s="58"/>
-      <c r="O26" s="58"/>
-      <c r="P26" s="58"/>
-      <c r="Q26" s="58"/>
-      <c r="R26" s="58"/>
-      <c r="S26" s="58"/>
-      <c r="T26" s="58"/>
-      <c r="U26" s="58"/>
-      <c r="V26" s="58"/>
-      <c r="W26" s="58"/>
-      <c r="X26" s="59"/>
+      <c r="L26" s="80"/>
+      <c r="M26" s="80"/>
+      <c r="N26" s="80"/>
+      <c r="O26" s="80"/>
+      <c r="P26" s="80"/>
+      <c r="Q26" s="80"/>
+      <c r="R26" s="80"/>
+      <c r="S26" s="80"/>
+      <c r="T26" s="80"/>
+      <c r="U26" s="80"/>
+      <c r="V26" s="80"/>
+      <c r="W26" s="80"/>
+      <c r="X26" s="81"/>
     </row>
     <row r="27" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K27" s="60"/>
-      <c r="L27" s="61"/>
-      <c r="M27" s="61"/>
-      <c r="N27" s="61"/>
-      <c r="O27" s="61"/>
-      <c r="P27" s="61"/>
-      <c r="Q27" s="61"/>
-      <c r="R27" s="61"/>
-      <c r="S27" s="61"/>
-      <c r="T27" s="61"/>
-      <c r="U27" s="61"/>
-      <c r="V27" s="61"/>
-      <c r="W27" s="61"/>
-      <c r="X27" s="62"/>
+      <c r="K27" s="82"/>
+      <c r="L27" s="83"/>
+      <c r="M27" s="83"/>
+      <c r="N27" s="83"/>
+      <c r="O27" s="83"/>
+      <c r="P27" s="83"/>
+      <c r="Q27" s="83"/>
+      <c r="R27" s="83"/>
+      <c r="S27" s="83"/>
+      <c r="T27" s="83"/>
+      <c r="U27" s="83"/>
+      <c r="V27" s="83"/>
+      <c r="W27" s="83"/>
+      <c r="X27" s="84"/>
     </row>
     <row r="30" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K30" s="57" t="s">
+      <c r="K30" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="L30" s="58"/>
-      <c r="M30" s="58"/>
-      <c r="N30" s="58"/>
-      <c r="O30" s="58"/>
-      <c r="P30" s="58"/>
-      <c r="Q30" s="58"/>
-      <c r="R30" s="58"/>
-      <c r="S30" s="58"/>
-      <c r="T30" s="58"/>
-      <c r="U30" s="58"/>
-      <c r="V30" s="58"/>
-      <c r="W30" s="58"/>
-      <c r="X30" s="59"/>
+      <c r="L30" s="80"/>
+      <c r="M30" s="80"/>
+      <c r="N30" s="80"/>
+      <c r="O30" s="80"/>
+      <c r="P30" s="80"/>
+      <c r="Q30" s="80"/>
+      <c r="R30" s="80"/>
+      <c r="S30" s="80"/>
+      <c r="T30" s="80"/>
+      <c r="U30" s="80"/>
+      <c r="V30" s="80"/>
+      <c r="W30" s="80"/>
+      <c r="X30" s="81"/>
     </row>
     <row r="31" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K31" s="60"/>
-      <c r="L31" s="61"/>
-      <c r="M31" s="61"/>
-      <c r="N31" s="61"/>
-      <c r="O31" s="61"/>
-      <c r="P31" s="61"/>
-      <c r="Q31" s="61"/>
-      <c r="R31" s="61"/>
-      <c r="S31" s="61"/>
-      <c r="T31" s="61"/>
-      <c r="U31" s="61"/>
-      <c r="V31" s="61"/>
-      <c r="W31" s="61"/>
-      <c r="X31" s="62"/>
+      <c r="K31" s="82"/>
+      <c r="L31" s="83"/>
+      <c r="M31" s="83"/>
+      <c r="N31" s="83"/>
+      <c r="O31" s="83"/>
+      <c r="P31" s="83"/>
+      <c r="Q31" s="83"/>
+      <c r="R31" s="83"/>
+      <c r="S31" s="83"/>
+      <c r="T31" s="83"/>
+      <c r="U31" s="83"/>
+      <c r="V31" s="83"/>
+      <c r="W31" s="83"/>
+      <c r="X31" s="84"/>
     </row>
     <row r="38" spans="11:11" x14ac:dyDescent="0.4">
       <c r="K38" t="s">
@@ -9211,10 +9331,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1494C983-D6B3-4A8C-AA9C-1AD533947069}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J85"/>
+  <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G53"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -9225,10 +9345,12 @@
     <col min="4" max="4" width="17.875" customWidth="1"/>
     <col min="5" max="5" width="11.75" style="1" customWidth="1"/>
     <col min="6" max="6" width="25.125" customWidth="1"/>
-    <col min="8" max="8" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" customWidth="1"/>
+    <col min="8" max="8" width="17.625" style="99" customWidth="1"/>
+    <col min="9" max="9" width="9" style="101"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>140</v>
       </c>
@@ -9247,16 +9369,24 @@
       <c r="F1" s="15" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="72" t="s">
+      <c r="G1" s="97" t="s">
+        <v>397</v>
+      </c>
+      <c r="H1" s="98" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="94" t="s">
         <v>188</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="74"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="96"/>
       <c r="E2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H2"/>
+      <c r="I2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3" s="24" t="str">
         <f>COUNTA(E$3:E3)&amp;"."</f>
         <v>1.</v>
@@ -9277,8 +9407,14 @@
       <c r="G3" s="28" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="H3" s="99">
+        <v>43623</v>
+      </c>
+      <c r="I3" s="101" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A4" s="29" t="str">
         <f>COUNTA(E$3:E4)&amp;"."</f>
         <v>2.</v>
@@ -9301,8 +9437,14 @@
       <c r="G4" s="34" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H4" s="99">
+        <v>43630</v>
+      </c>
+      <c r="I4" s="101" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A5" s="29" t="str">
         <f>COUNTA(E$3:E5)&amp;"."</f>
         <v>3.</v>
@@ -9323,8 +9465,14 @@
       <c r="G5" s="34" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H5" s="99">
+        <v>43630</v>
+      </c>
+      <c r="I5" s="101" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="38.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="29" t="str">
         <f>COUNTA(E$3:E6)&amp;"."</f>
         <v>4.</v>
@@ -9347,16 +9495,24 @@
       <c r="G6" s="36" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="69" t="s">
+      <c r="H6" s="99">
+        <v>43630</v>
+      </c>
+      <c r="I6" s="101" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="91" t="s">
         <v>190</v>
       </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="71"/>
+      <c r="B7" s="92"/>
+      <c r="C7" s="93"/>
       <c r="E7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H7"/>
+      <c r="I7"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A8" s="24" t="str">
         <f>COUNTA(E$3:E8)&amp;"."</f>
         <v>5.</v>
@@ -9377,8 +9533,14 @@
       <c r="G8" s="38" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H8" s="99" t="s">
+        <v>403</v>
+      </c>
+      <c r="I8" s="100" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A9" s="29" t="str">
         <f>COUNTA(E$3:E9)&amp;"."</f>
         <v>6.</v>
@@ -9401,8 +9563,17 @@
       <c r="G9" s="38" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H9" s="99">
+        <v>43637</v>
+      </c>
+      <c r="I9" s="100" t="s">
+        <v>404</v>
+      </c>
+      <c r="K9" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A10" s="29" t="str">
         <f>COUNTA(E$3:E10)&amp;"."</f>
         <v>7.</v>
@@ -9423,8 +9594,11 @@
       <c r="G10" s="28" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I10" s="100" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A11" s="29" t="str">
         <f>COUNTA(E$3:E11)&amp;"."</f>
         <v>8.</v>
@@ -9445,8 +9619,14 @@
       <c r="G11" s="28" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="H11" s="99">
+        <v>43677</v>
+      </c>
+      <c r="I11" s="100" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A12" s="29" t="str">
         <f>COUNTA(E$3:E12)&amp;"."</f>
         <v>9.</v>
@@ -9469,8 +9649,17 @@
       <c r="G12" s="28" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H12" s="99">
+        <v>43616</v>
+      </c>
+      <c r="I12" s="100" t="s">
+        <v>402</v>
+      </c>
+      <c r="N12" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A13" s="29" t="str">
         <f>COUNTA(E$3:E13)&amp;"."</f>
         <v>10.</v>
@@ -9491,8 +9680,17 @@
       <c r="G13" s="28" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+      <c r="H13" s="99">
+        <v>43612</v>
+      </c>
+      <c r="I13" s="101" t="s">
+        <v>414</v>
+      </c>
+      <c r="N13" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A14" s="16" t="str">
         <f>COUNTA(E$3:E14)&amp;"."</f>
         <v>11.</v>
@@ -9513,14 +9711,16 @@
       <c r="G14" s="22" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H14"/>
+      <c r="I14"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15" s="29" t="str">
         <f>COUNTA(E$3:E15)&amp;"."</f>
         <v>12.</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>148</v>
+        <v>406</v>
       </c>
       <c r="C15" s="31" t="s">
         <v>84</v>
@@ -9535,8 +9735,14 @@
       <c r="G15" s="38" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="31.5" hidden="1" x14ac:dyDescent="0.4">
+      <c r="H15" s="99">
+        <v>43612</v>
+      </c>
+      <c r="I15" s="101" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="31.5" hidden="1" x14ac:dyDescent="0.4">
       <c r="A16" s="16" t="str">
         <f>COUNTA(E$3:E16)&amp;"."</f>
         <v>13.</v>
@@ -9559,8 +9765,10 @@
       <c r="G16" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="H16"/>
+      <c r="I16"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A17" s="29" t="str">
         <f>COUNTA(E$3:E17)&amp;"."</f>
         <v>14.</v>
@@ -9581,8 +9789,11 @@
       <c r="G17" s="38" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="I17" s="101" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A18" s="29" t="str">
         <f>COUNTA(E$3:E18)&amp;"."</f>
         <v>15.</v>
@@ -9605,8 +9816,14 @@
       <c r="G18" s="38" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I18" s="101" t="s">
+        <v>409</v>
+      </c>
+      <c r="N18" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A19" s="29" t="str">
         <f>COUNTA(E$3:E19)&amp;"."</f>
         <v>16.</v>
@@ -9627,8 +9844,14 @@
       <c r="G19" s="28" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+      <c r="I19" s="101" t="s">
+        <v>422</v>
+      </c>
+      <c r="N19" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A20" s="16" t="str">
         <f>COUNTA(E$3:E20)&amp;"."</f>
         <v>17.</v>
@@ -9651,8 +9874,10 @@
       <c r="G20" s="22" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+      <c r="H20"/>
+      <c r="I20"/>
+    </row>
+    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A21" s="16" t="str">
         <f>COUNTA(E$3:E21)&amp;"."</f>
         <v>18.</v>
@@ -9675,8 +9900,10 @@
       <c r="G21" s="22" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="H21"/>
+      <c r="I21"/>
+    </row>
+    <row r="22" spans="1:14" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A22" s="29" t="str">
         <f>COUNTA(E$3:E22)&amp;"."</f>
         <v>19.</v>
@@ -9699,9 +9926,15 @@
       <c r="G22" s="28" t="s">
         <v>220</v>
       </c>
+      <c r="I22" s="101" t="s">
+        <v>409</v>
+      </c>
       <c r="J22" s="18"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="N22" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A23" s="29" t="str">
         <f>COUNTA(E$3:E23)&amp;"."</f>
         <v>20.</v>
@@ -9724,8 +9957,14 @@
       <c r="G23" s="28" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="56.25" hidden="1" x14ac:dyDescent="0.4">
+      <c r="I23" s="101" t="s">
+        <v>415</v>
+      </c>
+      <c r="J23" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="56.25" hidden="1" x14ac:dyDescent="0.4">
       <c r="A24" s="16" t="str">
         <f>COUNTA(E$3:E24)&amp;"."</f>
         <v>21.</v>
@@ -9748,8 +9987,10 @@
       <c r="G24" s="22" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+      <c r="H24"/>
+      <c r="I24"/>
+    </row>
+    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A25" s="16" t="str">
         <f>COUNTA(E$3:E25)&amp;"."</f>
         <v>22.</v>
@@ -9772,8 +10013,10 @@
       <c r="G25" s="22" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+      <c r="H25"/>
+      <c r="I25"/>
+    </row>
+    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A26" s="16" t="str">
         <f>COUNTA(E$3:E26)&amp;"."</f>
         <v>23.</v>
@@ -9796,8 +10039,10 @@
       <c r="G26" s="22" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+      <c r="H26"/>
+      <c r="I26"/>
+    </row>
+    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A27" s="16" t="str">
         <f>COUNTA(E$3:E27)&amp;"."</f>
         <v>24.</v>
@@ -9820,8 +10065,10 @@
       <c r="G27" s="22" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+      <c r="H27"/>
+      <c r="I27"/>
+    </row>
+    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A28" s="16" t="str">
         <f>COUNTA(E$3:E28)&amp;"."</f>
         <v>25.</v>
@@ -9842,8 +10089,10 @@
       <c r="G28" s="22" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+      <c r="H28"/>
+      <c r="I28"/>
+    </row>
+    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A29" s="16" t="str">
         <f>COUNTA(E$3:E29)&amp;"."</f>
         <v>26.</v>
@@ -9866,8 +10115,10 @@
       <c r="G29" s="23" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="H29"/>
+      <c r="I29"/>
+    </row>
+    <row r="30" spans="1:14" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A30" s="29" t="str">
         <f>COUNTA(E$3:E30)&amp;"."</f>
         <v>27.</v>
@@ -9890,8 +10141,11 @@
       <c r="G30" s="28" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="56.25" hidden="1" x14ac:dyDescent="0.4">
+      <c r="I30" s="101" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="56.25" hidden="1" x14ac:dyDescent="0.4">
       <c r="A31" s="16" t="str">
         <f>COUNTA(E$3:E31)&amp;"."</f>
         <v>28.</v>
@@ -9914,8 +10168,10 @@
       <c r="G31" s="22" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+      <c r="H31"/>
+      <c r="I31"/>
+    </row>
+    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A32" s="16" t="str">
         <f>COUNTA(E$3:E32)&amp;"."</f>
         <v>29.</v>
@@ -9938,8 +10194,10 @@
       <c r="G32" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="37.5" hidden="1" x14ac:dyDescent="0.4">
+      <c r="H32"/>
+      <c r="I32"/>
+    </row>
+    <row r="33" spans="1:14" ht="37.5" hidden="1" x14ac:dyDescent="0.4">
       <c r="A33" s="16" t="str">
         <f>COUNTA(E$3:E33)&amp;"."</f>
         <v>30.</v>
@@ -9960,8 +10218,10 @@
       <c r="G33" s="23" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="57" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H33"/>
+      <c r="I33"/>
+    </row>
+    <row r="34" spans="1:14" ht="57" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A34" s="17" t="str">
         <f>COUNTA(E$3:E34)&amp;"."</f>
         <v>31.</v>
@@ -9984,16 +10244,20 @@
       <c r="G34" s="23" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="69" t="s">
+      <c r="H34"/>
+      <c r="I34"/>
+    </row>
+    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="91" t="s">
         <v>195</v>
       </c>
-      <c r="B35" s="70"/>
-      <c r="C35" s="71"/>
+      <c r="B35" s="92"/>
+      <c r="C35" s="93"/>
       <c r="E35"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H35"/>
+      <c r="I35"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A36" s="29" t="str">
         <f>COUNTA(E$3:E36)&amp;"."</f>
         <v>32.</v>
@@ -10014,8 +10278,14 @@
       <c r="G36" s="38" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H36" s="99">
+        <v>43612</v>
+      </c>
+      <c r="I36" s="101" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A37" s="29" t="str">
         <f>COUNTA(E$3:E37)&amp;"."</f>
         <v>33.</v>
@@ -10036,8 +10306,11 @@
       <c r="G37" s="34" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I37" s="101" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A38" s="29" t="str">
         <f>COUNTA(E$3:E38)&amp;"."</f>
         <v>34.</v>
@@ -10060,16 +10333,24 @@
       <c r="G38" s="40" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="69" t="s">
+      <c r="I38" s="101" t="s">
+        <v>412</v>
+      </c>
+      <c r="N38" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="91" t="s">
         <v>198</v>
       </c>
-      <c r="B39" s="70"/>
-      <c r="C39" s="71"/>
+      <c r="B39" s="92"/>
+      <c r="C39" s="93"/>
       <c r="E39"/>
-    </row>
-    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+      <c r="H39"/>
+      <c r="I39"/>
+    </row>
+    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A40" s="16" t="str">
         <f>COUNTA(E$3:E40)&amp;"."</f>
         <v>35.</v>
@@ -10090,8 +10371,10 @@
       <c r="G40" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="37.5" hidden="1" x14ac:dyDescent="0.4">
+      <c r="H40"/>
+      <c r="I40"/>
+    </row>
+    <row r="41" spans="1:14" ht="37.5" hidden="1" x14ac:dyDescent="0.4">
       <c r="A41" s="16" t="str">
         <f>COUNTA(E$3:E41)&amp;"."</f>
         <v>36.</v>
@@ -10111,16 +10394,20 @@
       <c r="F41" s="7" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="69" t="s">
+      <c r="H41"/>
+      <c r="I41"/>
+    </row>
+    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="91" t="s">
         <v>189</v>
       </c>
-      <c r="B42" s="70"/>
-      <c r="C42" s="71"/>
+      <c r="B42" s="92"/>
+      <c r="C42" s="93"/>
       <c r="E42"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H42"/>
+      <c r="I42"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A43" s="29" t="str">
         <f>COUNTA(E$3:E43)&amp;"."</f>
         <v>37.</v>
@@ -10143,8 +10430,11 @@
       <c r="G43" s="28" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.4">
+      <c r="I43" s="101" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="75" hidden="1" x14ac:dyDescent="0.4">
       <c r="A44" s="16" t="str">
         <f>COUNTA(E$3:E44)&amp;"."</f>
         <v>38.</v>
@@ -10167,8 +10457,10 @@
       <c r="G44" s="23" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="93.75" hidden="1" x14ac:dyDescent="0.4">
+      <c r="H44"/>
+      <c r="I44"/>
+    </row>
+    <row r="45" spans="1:14" ht="93.75" hidden="1" x14ac:dyDescent="0.4">
       <c r="A45" s="16" t="str">
         <f>COUNTA(E$3:E45)&amp;"."</f>
         <v>39.</v>
@@ -10191,8 +10483,10 @@
       <c r="G45" s="22" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="75" x14ac:dyDescent="0.4">
+      <c r="H45"/>
+      <c r="I45"/>
+    </row>
+    <row r="46" spans="1:14" ht="75" x14ac:dyDescent="0.4">
       <c r="A46" s="29" t="str">
         <f>COUNTA(E$3:E46)&amp;"."</f>
         <v>40.</v>
@@ -10215,8 +10509,11 @@
       <c r="G46" s="34" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="I46" s="101" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A47" s="29" t="str">
         <f>COUNTA(E$3:E47)&amp;"."</f>
         <v>41.</v>
@@ -10239,8 +10536,11 @@
       <c r="G47" s="34" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="56.25" hidden="1" x14ac:dyDescent="0.4">
+      <c r="I47" s="101" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="56.25" hidden="1" x14ac:dyDescent="0.4">
       <c r="A48" s="16" t="str">
         <f>COUNTA(E$3:E48)&amp;"."</f>
         <v>42.</v>
@@ -10263,16 +10563,20 @@
       <c r="G48" s="23" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="69" t="s">
+      <c r="H48"/>
+      <c r="I48"/>
+    </row>
+    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="91" t="s">
         <v>196</v>
       </c>
-      <c r="B49" s="70"/>
-      <c r="C49" s="71"/>
+      <c r="B49" s="92"/>
+      <c r="C49" s="93"/>
       <c r="E49"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H49"/>
+      <c r="I49"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A50" s="29" t="str">
         <f>COUNTA(E$3:E50)&amp;"."</f>
         <v>43.</v>
@@ -10295,8 +10599,14 @@
       <c r="G50" s="40" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H50" s="99">
+        <v>43612</v>
+      </c>
+      <c r="I50" s="101" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A51" s="29" t="str">
         <f>COUNTA(E$3:E51)&amp;"."</f>
         <v>44.</v>
@@ -10317,8 +10627,14 @@
       <c r="G51" s="40" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="I51" s="101" t="s">
+        <v>420</v>
+      </c>
+      <c r="N51" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A52" s="29" t="str">
         <f>COUNTA(E$3:E52)&amp;"."</f>
         <v>45.</v>
@@ -10341,8 +10657,14 @@
       <c r="G52" s="40" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H52" s="99">
+        <v>43612</v>
+      </c>
+      <c r="I52" s="101" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A53" s="29" t="str">
         <f>COUNTA(E$3:E53)&amp;"."</f>
         <v>46.</v>
@@ -10365,17 +10687,21 @@
       <c r="G53" s="40" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="69" t="s">
+      <c r="I53" s="101" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="91" t="s">
         <v>197</v>
       </c>
-      <c r="B54" s="70"/>
-      <c r="C54" s="71"/>
+      <c r="B54" s="92"/>
+      <c r="C54" s="93"/>
       <c r="E54"/>
       <c r="H54" s="19"/>
-    </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
+      <c r="I54"/>
+    </row>
+    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A55" s="16" t="str">
         <f>COUNTA(E$3:E55)&amp;"."</f>
         <v>47.</v>
@@ -10396,8 +10722,9 @@
         <v>159</v>
       </c>
       <c r="H55" s="19"/>
-    </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
+      <c r="I55"/>
+    </row>
+    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A56" s="16" t="str">
         <f>COUNTA(E$3:E56)&amp;"."</f>
         <v>48.</v>
@@ -10418,8 +10745,9 @@
         <v>13</v>
       </c>
       <c r="H56" s="19"/>
-    </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
+      <c r="I56"/>
+    </row>
+    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A57" s="16" t="str">
         <f>COUNTA(E$3:E57)&amp;"."</f>
         <v>49.</v>
@@ -10440,8 +10768,9 @@
         <v>16</v>
       </c>
       <c r="H57" s="19"/>
-    </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
+      <c r="I57"/>
+    </row>
+    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A58" s="16" t="str">
         <f>COUNTA(E$3:E58)&amp;"."</f>
         <v>50.</v>
@@ -10462,8 +10791,9 @@
         <v>25</v>
       </c>
       <c r="H58" s="19"/>
-    </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
+      <c r="I58"/>
+    </row>
+    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A59" s="16" t="str">
         <f>COUNTA(E$3:E59)&amp;"."</f>
         <v>51.</v>
@@ -10483,8 +10813,10 @@
       <c r="F59" s="7" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
+      <c r="H59"/>
+      <c r="I59"/>
+    </row>
+    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A60" s="16" t="str">
         <f>COUNTA(E$3:E60)&amp;"."</f>
         <v>52.</v>
@@ -10504,8 +10836,10 @@
       <c r="F60" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
+      <c r="H60"/>
+      <c r="I60"/>
+    </row>
+    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A61" s="16" t="str">
         <f>COUNTA(E$3:E61)&amp;"."</f>
         <v>53.</v>
@@ -10523,8 +10857,10 @@
         <v>63</v>
       </c>
       <c r="F61" s="7"/>
-    </row>
-    <row r="62" spans="1:8" ht="75" hidden="1" x14ac:dyDescent="0.4">
+      <c r="H61"/>
+      <c r="I61"/>
+    </row>
+    <row r="62" spans="1:14" ht="75" hidden="1" x14ac:dyDescent="0.4">
       <c r="A62" s="16" t="str">
         <f>COUNTA(E$3:E62)&amp;"."</f>
         <v>54.</v>
@@ -10544,8 +10880,10 @@
       <c r="F62" s="7" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
+      <c r="H62"/>
+      <c r="I62"/>
+    </row>
+    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A63" s="16" t="str">
         <f>COUNTA(E$3:E63)&amp;"."</f>
         <v>55.</v>
@@ -10563,8 +10901,10 @@
         <v>63</v>
       </c>
       <c r="F63" s="7"/>
-    </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
+      <c r="H63"/>
+      <c r="I63"/>
+    </row>
+    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A64" s="16" t="str">
         <f>COUNTA(E$3:E64)&amp;"."</f>
         <v>56.</v>
@@ -10582,8 +10922,10 @@
         <v>63</v>
       </c>
       <c r="F64" s="7"/>
-    </row>
-    <row r="65" spans="1:6" ht="56.25" hidden="1" x14ac:dyDescent="0.4">
+      <c r="H64"/>
+      <c r="I64"/>
+    </row>
+    <row r="65" spans="1:6" customFormat="1" ht="56.25" hidden="1" x14ac:dyDescent="0.4">
       <c r="A65" s="16" t="str">
         <f>COUNTA(E$3:E65)&amp;"."</f>
         <v>57.</v>
@@ -10604,7 +10946,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="56.25" hidden="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:6" customFormat="1" ht="56.25" hidden="1" x14ac:dyDescent="0.4">
       <c r="A66" s="16" t="str">
         <f>COUNTA(E$3:E66)&amp;"."</f>
         <v>58.</v>
@@ -10625,7 +10967,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A67" s="16" t="str">
         <f>COUNTA(E$3:E67)&amp;"."</f>
         <v>59.</v>
@@ -10644,7 +10986,7 @@
       </c>
       <c r="F67" s="7"/>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A68" s="16" t="str">
         <f>COUNTA(E$3:E68)&amp;"."</f>
         <v>60.</v>
@@ -10663,7 +11005,7 @@
       </c>
       <c r="F68" s="7"/>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A69" s="16" t="str">
         <f>COUNTA(E$3:E69)&amp;"."</f>
         <v>61.</v>
@@ -10682,7 +11024,7 @@
       </c>
       <c r="F69" s="7"/>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A70" s="16" t="str">
         <f>COUNTA(E$3:E70)&amp;"."</f>
         <v>62.</v>
@@ -10701,7 +11043,7 @@
       </c>
       <c r="F70" s="7"/>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A71" s="16" t="str">
         <f>COUNTA(E$3:E71)&amp;"."</f>
         <v>63.</v>
@@ -10720,7 +11062,7 @@
       </c>
       <c r="F71" s="7"/>
     </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A72" s="16" t="str">
         <f>COUNTA(E$3:E72)&amp;"."</f>
         <v>64.</v>
@@ -10739,7 +11081,7 @@
       </c>
       <c r="F72" s="7"/>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A73" s="16" t="str">
         <f>COUNTA(E$3:E73)&amp;"."</f>
         <v>65.</v>
@@ -10758,7 +11100,7 @@
       </c>
       <c r="F73" s="7"/>
     </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A74" s="16" t="str">
         <f>COUNTA(E$3:E74)&amp;"."</f>
         <v>66.</v>
@@ -10777,7 +11119,7 @@
       </c>
       <c r="F74" s="7"/>
     </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A75" s="16" t="str">
         <f>COUNTA(E$3:E75)&amp;"."</f>
         <v>67.</v>
@@ -10796,7 +11138,7 @@
       </c>
       <c r="F75" s="7"/>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A76" s="16" t="str">
         <f>COUNTA(E$3:E76)&amp;"."</f>
         <v>68.</v>
@@ -10815,7 +11157,7 @@
       </c>
       <c r="F76" s="7"/>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A77" s="16" t="str">
         <f>COUNTA(E$3:E77)&amp;"."</f>
         <v>69.</v>
@@ -10834,7 +11176,7 @@
       </c>
       <c r="F77" s="8"/>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A78" s="16" t="str">
         <f>COUNTA(E$3:E78)&amp;"."</f>
         <v>70.</v>
@@ -10853,7 +11195,7 @@
       </c>
       <c r="F78" s="8"/>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A79" s="16" t="str">
         <f>COUNTA(E$3:E79)&amp;"."</f>
         <v>71.</v>
@@ -10872,7 +11214,7 @@
       </c>
       <c r="F79" s="8"/>
     </row>
-    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A80" s="16" t="str">
         <f>COUNTA(E$3:E80)&amp;"."</f>
         <v>72.</v>
@@ -10891,7 +11233,7 @@
       </c>
       <c r="F80" s="8"/>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A81" s="16" t="str">
         <f>COUNTA(E$3:E81)&amp;"."</f>
         <v>73.</v>
@@ -10910,7 +11252,7 @@
       </c>
       <c r="F81" s="8"/>
     </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A82" s="16" t="str">
         <f>COUNTA(E$3:E82)&amp;"."</f>
         <v>74.</v>
@@ -10929,7 +11271,7 @@
       </c>
       <c r="F82" s="8"/>
     </row>
-    <row r="83" spans="1:6" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6" customFormat="1" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A83" s="17" t="str">
         <f>COUNTA(E$3:E83)&amp;"."</f>
         <v>75.</v>
@@ -10948,8 +11290,14 @@
       </c>
       <c r="F83" s="10"/>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.4"/>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="84" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="1"/>
+      <c r="E84" s="1"/>
+    </row>
+    <row r="85" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A85" s="1"/>
+      <c r="E85" s="1"/>
+    </row>
   </sheetData>
   <autoFilter ref="G1:G85" xr:uid="{729D066D-B44E-46AC-81FA-7975A774CA00}">
     <filterColumn colId="0">

</xml_diff>

<commit_message>
Un petit start avec mongoose CRUD
Ce soir Commencer par utiliser mozilla pour avoir la structure et c'est de part cette structure qu'on va creer la sienne
</commit_message>
<xml_diff>
--- a/Cahier des charges/Organisation Projet Nodejs.xlsx
+++ b/Cahier des charges/Organisation Projet Nodejs.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\MyEnv\NodeJs\Cahier des charges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D14DD30-0FFA-4991-A7A9-997F9B750E6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0E2E13-CBC6-477D-B8E0-BA393A4D4C7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="3" xr2:uid="{D1074EF0-41CD-437C-83BE-5015162961C9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="4" xr2:uid="{D1074EF0-41CD-437C-83BE-5015162961C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="6" r:id="rId1"/>
     <sheet name="Organisation Projet node.js" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="5" r:id="rId4"/>
-    <sheet name="bin" sheetId="2" r:id="rId5"/>
-    <sheet name="Model Generator" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="7" r:id="rId5"/>
+    <sheet name="bin" sheetId="2" r:id="rId6"/>
+    <sheet name="Model Generator" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet2!$G$1:$G$85</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="441">
   <si>
     <t>Check bin sheet for more informations</t>
     <phoneticPr fontId="1"/>
@@ -2721,6 +2722,78 @@
   </si>
   <si>
     <t>Mongoose/generator/etc..</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1 comprendre comment marche app.js et www</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Commencer sans aucun support un projet express </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Recap des new technos a utiliser:
+ - ejs
+ - lodash/joi/validator
+ - Morgan
+ - PM2
+ - moment
+ - jQuery
+ - debug
+ - color
+ - faker
+ - mongoose
+ - express
+ - bodyparser</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Recap des new technos a utiliser:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - ejs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - lodash/joi/validator</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Morgan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - PM2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - moment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - debug</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - color</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - faker</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - mongoose</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - express</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - bodyparser</t>
+  </si>
+  <si>
+    <t>Utilisation</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>cookie-parser</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2951,7 +3024,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3000,8 +3073,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="27">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -3337,6 +3416,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -3346,7 +3455,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3584,6 +3693,21 @@
     <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3638,19 +3762,31 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -9008,276 +9144,276 @@
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="2" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K2" s="79" t="s">
+      <c r="K2" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
-      <c r="Q2" s="80"/>
-      <c r="R2" s="80"/>
-      <c r="S2" s="80"/>
-      <c r="T2" s="80"/>
-      <c r="U2" s="80"/>
-      <c r="V2" s="80"/>
-      <c r="W2" s="80"/>
-      <c r="X2" s="81"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="85"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="85"/>
+      <c r="U2" s="85"/>
+      <c r="V2" s="85"/>
+      <c r="W2" s="85"/>
+      <c r="X2" s="86"/>
     </row>
     <row r="3" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K3" s="82"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="83"/>
-      <c r="N3" s="83"/>
-      <c r="O3" s="83"/>
-      <c r="P3" s="83"/>
-      <c r="Q3" s="83"/>
-      <c r="R3" s="83"/>
-      <c r="S3" s="83"/>
-      <c r="T3" s="83"/>
-      <c r="U3" s="83"/>
-      <c r="V3" s="83"/>
-      <c r="W3" s="83"/>
-      <c r="X3" s="84"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="88"/>
+      <c r="M3" s="88"/>
+      <c r="N3" s="88"/>
+      <c r="O3" s="88"/>
+      <c r="P3" s="88"/>
+      <c r="Q3" s="88"/>
+      <c r="R3" s="88"/>
+      <c r="S3" s="88"/>
+      <c r="T3" s="88"/>
+      <c r="U3" s="88"/>
+      <c r="V3" s="88"/>
+      <c r="W3" s="88"/>
+      <c r="X3" s="89"/>
     </row>
     <row r="6" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K6" s="79" t="s">
+      <c r="K6" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="80"/>
-      <c r="M6" s="80"/>
-      <c r="N6" s="80"/>
-      <c r="O6" s="80"/>
-      <c r="P6" s="80"/>
-      <c r="Q6" s="80"/>
-      <c r="R6" s="80"/>
-      <c r="S6" s="80"/>
-      <c r="T6" s="80"/>
-      <c r="U6" s="80"/>
-      <c r="V6" s="80"/>
-      <c r="W6" s="80"/>
-      <c r="X6" s="81"/>
+      <c r="L6" s="85"/>
+      <c r="M6" s="85"/>
+      <c r="N6" s="85"/>
+      <c r="O6" s="85"/>
+      <c r="P6" s="85"/>
+      <c r="Q6" s="85"/>
+      <c r="R6" s="85"/>
+      <c r="S6" s="85"/>
+      <c r="T6" s="85"/>
+      <c r="U6" s="85"/>
+      <c r="V6" s="85"/>
+      <c r="W6" s="85"/>
+      <c r="X6" s="86"/>
     </row>
     <row r="7" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K7" s="82"/>
-      <c r="L7" s="83"/>
-      <c r="M7" s="83"/>
-      <c r="N7" s="83"/>
-      <c r="O7" s="83"/>
-      <c r="P7" s="83"/>
-      <c r="Q7" s="83"/>
-      <c r="R7" s="83"/>
-      <c r="S7" s="83"/>
-      <c r="T7" s="83"/>
-      <c r="U7" s="83"/>
-      <c r="V7" s="83"/>
-      <c r="W7" s="83"/>
-      <c r="X7" s="84"/>
+      <c r="K7" s="87"/>
+      <c r="L7" s="88"/>
+      <c r="M7" s="88"/>
+      <c r="N7" s="88"/>
+      <c r="O7" s="88"/>
+      <c r="P7" s="88"/>
+      <c r="Q7" s="88"/>
+      <c r="R7" s="88"/>
+      <c r="S7" s="88"/>
+      <c r="T7" s="88"/>
+      <c r="U7" s="88"/>
+      <c r="V7" s="88"/>
+      <c r="W7" s="88"/>
+      <c r="X7" s="89"/>
     </row>
     <row r="10" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K10" s="85" t="s">
+      <c r="K10" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="L10" s="86"/>
-      <c r="M10" s="86"/>
-      <c r="N10" s="86"/>
-      <c r="O10" s="86"/>
-      <c r="P10" s="86"/>
-      <c r="Q10" s="86"/>
-      <c r="R10" s="86"/>
-      <c r="S10" s="86"/>
-      <c r="T10" s="86"/>
-      <c r="U10" s="86"/>
-      <c r="V10" s="86"/>
-      <c r="W10" s="86"/>
-      <c r="X10" s="87"/>
+      <c r="L10" s="91"/>
+      <c r="M10" s="91"/>
+      <c r="N10" s="91"/>
+      <c r="O10" s="91"/>
+      <c r="P10" s="91"/>
+      <c r="Q10" s="91"/>
+      <c r="R10" s="91"/>
+      <c r="S10" s="91"/>
+      <c r="T10" s="91"/>
+      <c r="U10" s="91"/>
+      <c r="V10" s="91"/>
+      <c r="W10" s="91"/>
+      <c r="X10" s="92"/>
     </row>
     <row r="11" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K11" s="88"/>
-      <c r="L11" s="89"/>
-      <c r="M11" s="89"/>
-      <c r="N11" s="89"/>
-      <c r="O11" s="89"/>
-      <c r="P11" s="89"/>
-      <c r="Q11" s="89"/>
-      <c r="R11" s="89"/>
-      <c r="S11" s="89"/>
-      <c r="T11" s="89"/>
-      <c r="U11" s="89"/>
-      <c r="V11" s="89"/>
-      <c r="W11" s="89"/>
-      <c r="X11" s="90"/>
+      <c r="K11" s="93"/>
+      <c r="L11" s="94"/>
+      <c r="M11" s="94"/>
+      <c r="N11" s="94"/>
+      <c r="O11" s="94"/>
+      <c r="P11" s="94"/>
+      <c r="Q11" s="94"/>
+      <c r="R11" s="94"/>
+      <c r="S11" s="94"/>
+      <c r="T11" s="94"/>
+      <c r="U11" s="94"/>
+      <c r="V11" s="94"/>
+      <c r="W11" s="94"/>
+      <c r="X11" s="95"/>
     </row>
     <row r="14" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K14" s="79" t="s">
+      <c r="K14" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="L14" s="80"/>
-      <c r="M14" s="80"/>
-      <c r="N14" s="80"/>
-      <c r="O14" s="80"/>
-      <c r="P14" s="80"/>
-      <c r="Q14" s="80"/>
-      <c r="R14" s="80"/>
-      <c r="S14" s="80"/>
-      <c r="T14" s="80"/>
-      <c r="U14" s="80"/>
-      <c r="V14" s="80"/>
-      <c r="W14" s="80"/>
-      <c r="X14" s="81"/>
+      <c r="L14" s="85"/>
+      <c r="M14" s="85"/>
+      <c r="N14" s="85"/>
+      <c r="O14" s="85"/>
+      <c r="P14" s="85"/>
+      <c r="Q14" s="85"/>
+      <c r="R14" s="85"/>
+      <c r="S14" s="85"/>
+      <c r="T14" s="85"/>
+      <c r="U14" s="85"/>
+      <c r="V14" s="85"/>
+      <c r="W14" s="85"/>
+      <c r="X14" s="86"/>
     </row>
     <row r="15" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K15" s="82"/>
-      <c r="L15" s="83"/>
-      <c r="M15" s="83"/>
-      <c r="N15" s="83"/>
-      <c r="O15" s="83"/>
-      <c r="P15" s="83"/>
-      <c r="Q15" s="83"/>
-      <c r="R15" s="83"/>
-      <c r="S15" s="83"/>
-      <c r="T15" s="83"/>
-      <c r="U15" s="83"/>
-      <c r="V15" s="83"/>
-      <c r="W15" s="83"/>
-      <c r="X15" s="84"/>
+      <c r="K15" s="87"/>
+      <c r="L15" s="88"/>
+      <c r="M15" s="88"/>
+      <c r="N15" s="88"/>
+      <c r="O15" s="88"/>
+      <c r="P15" s="88"/>
+      <c r="Q15" s="88"/>
+      <c r="R15" s="88"/>
+      <c r="S15" s="88"/>
+      <c r="T15" s="88"/>
+      <c r="U15" s="88"/>
+      <c r="V15" s="88"/>
+      <c r="W15" s="88"/>
+      <c r="X15" s="89"/>
     </row>
     <row r="18" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K18" s="79" t="s">
+      <c r="K18" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="L18" s="80"/>
-      <c r="M18" s="80"/>
-      <c r="N18" s="80"/>
-      <c r="O18" s="80"/>
-      <c r="P18" s="80"/>
-      <c r="Q18" s="80"/>
-      <c r="R18" s="80"/>
-      <c r="S18" s="80"/>
-      <c r="T18" s="80"/>
-      <c r="U18" s="80"/>
-      <c r="V18" s="80"/>
-      <c r="W18" s="80"/>
-      <c r="X18" s="81"/>
+      <c r="L18" s="85"/>
+      <c r="M18" s="85"/>
+      <c r="N18" s="85"/>
+      <c r="O18" s="85"/>
+      <c r="P18" s="85"/>
+      <c r="Q18" s="85"/>
+      <c r="R18" s="85"/>
+      <c r="S18" s="85"/>
+      <c r="T18" s="85"/>
+      <c r="U18" s="85"/>
+      <c r="V18" s="85"/>
+      <c r="W18" s="85"/>
+      <c r="X18" s="86"/>
     </row>
     <row r="19" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K19" s="82"/>
-      <c r="L19" s="83"/>
-      <c r="M19" s="83"/>
-      <c r="N19" s="83"/>
-      <c r="O19" s="83"/>
-      <c r="P19" s="83"/>
-      <c r="Q19" s="83"/>
-      <c r="R19" s="83"/>
-      <c r="S19" s="83"/>
-      <c r="T19" s="83"/>
-      <c r="U19" s="83"/>
-      <c r="V19" s="83"/>
-      <c r="W19" s="83"/>
-      <c r="X19" s="84"/>
+      <c r="K19" s="87"/>
+      <c r="L19" s="88"/>
+      <c r="M19" s="88"/>
+      <c r="N19" s="88"/>
+      <c r="O19" s="88"/>
+      <c r="P19" s="88"/>
+      <c r="Q19" s="88"/>
+      <c r="R19" s="88"/>
+      <c r="S19" s="88"/>
+      <c r="T19" s="88"/>
+      <c r="U19" s="88"/>
+      <c r="V19" s="88"/>
+      <c r="W19" s="88"/>
+      <c r="X19" s="89"/>
     </row>
     <row r="22" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K22" s="79" t="s">
+      <c r="K22" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="L22" s="80"/>
-      <c r="M22" s="80"/>
-      <c r="N22" s="80"/>
-      <c r="O22" s="80"/>
-      <c r="P22" s="80"/>
-      <c r="Q22" s="80"/>
-      <c r="R22" s="80"/>
-      <c r="S22" s="80"/>
-      <c r="T22" s="80"/>
-      <c r="U22" s="80"/>
-      <c r="V22" s="80"/>
-      <c r="W22" s="80"/>
-      <c r="X22" s="81"/>
+      <c r="L22" s="85"/>
+      <c r="M22" s="85"/>
+      <c r="N22" s="85"/>
+      <c r="O22" s="85"/>
+      <c r="P22" s="85"/>
+      <c r="Q22" s="85"/>
+      <c r="R22" s="85"/>
+      <c r="S22" s="85"/>
+      <c r="T22" s="85"/>
+      <c r="U22" s="85"/>
+      <c r="V22" s="85"/>
+      <c r="W22" s="85"/>
+      <c r="X22" s="86"/>
     </row>
     <row r="23" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K23" s="82"/>
-      <c r="L23" s="83"/>
-      <c r="M23" s="83"/>
-      <c r="N23" s="83"/>
-      <c r="O23" s="83"/>
-      <c r="P23" s="83"/>
-      <c r="Q23" s="83"/>
-      <c r="R23" s="83"/>
-      <c r="S23" s="83"/>
-      <c r="T23" s="83"/>
-      <c r="U23" s="83"/>
-      <c r="V23" s="83"/>
-      <c r="W23" s="83"/>
-      <c r="X23" s="84"/>
+      <c r="K23" s="87"/>
+      <c r="L23" s="88"/>
+      <c r="M23" s="88"/>
+      <c r="N23" s="88"/>
+      <c r="O23" s="88"/>
+      <c r="P23" s="88"/>
+      <c r="Q23" s="88"/>
+      <c r="R23" s="88"/>
+      <c r="S23" s="88"/>
+      <c r="T23" s="88"/>
+      <c r="U23" s="88"/>
+      <c r="V23" s="88"/>
+      <c r="W23" s="88"/>
+      <c r="X23" s="89"/>
     </row>
     <row r="26" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K26" s="79" t="s">
+      <c r="K26" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="L26" s="80"/>
-      <c r="M26" s="80"/>
-      <c r="N26" s="80"/>
-      <c r="O26" s="80"/>
-      <c r="P26" s="80"/>
-      <c r="Q26" s="80"/>
-      <c r="R26" s="80"/>
-      <c r="S26" s="80"/>
-      <c r="T26" s="80"/>
-      <c r="U26" s="80"/>
-      <c r="V26" s="80"/>
-      <c r="W26" s="80"/>
-      <c r="X26" s="81"/>
+      <c r="L26" s="85"/>
+      <c r="M26" s="85"/>
+      <c r="N26" s="85"/>
+      <c r="O26" s="85"/>
+      <c r="P26" s="85"/>
+      <c r="Q26" s="85"/>
+      <c r="R26" s="85"/>
+      <c r="S26" s="85"/>
+      <c r="T26" s="85"/>
+      <c r="U26" s="85"/>
+      <c r="V26" s="85"/>
+      <c r="W26" s="85"/>
+      <c r="X26" s="86"/>
     </row>
     <row r="27" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K27" s="82"/>
-      <c r="L27" s="83"/>
-      <c r="M27" s="83"/>
-      <c r="N27" s="83"/>
-      <c r="O27" s="83"/>
-      <c r="P27" s="83"/>
-      <c r="Q27" s="83"/>
-      <c r="R27" s="83"/>
-      <c r="S27" s="83"/>
-      <c r="T27" s="83"/>
-      <c r="U27" s="83"/>
-      <c r="V27" s="83"/>
-      <c r="W27" s="83"/>
-      <c r="X27" s="84"/>
+      <c r="K27" s="87"/>
+      <c r="L27" s="88"/>
+      <c r="M27" s="88"/>
+      <c r="N27" s="88"/>
+      <c r="O27" s="88"/>
+      <c r="P27" s="88"/>
+      <c r="Q27" s="88"/>
+      <c r="R27" s="88"/>
+      <c r="S27" s="88"/>
+      <c r="T27" s="88"/>
+      <c r="U27" s="88"/>
+      <c r="V27" s="88"/>
+      <c r="W27" s="88"/>
+      <c r="X27" s="89"/>
     </row>
     <row r="30" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K30" s="79" t="s">
+      <c r="K30" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="L30" s="80"/>
-      <c r="M30" s="80"/>
-      <c r="N30" s="80"/>
-      <c r="O30" s="80"/>
-      <c r="P30" s="80"/>
-      <c r="Q30" s="80"/>
-      <c r="R30" s="80"/>
-      <c r="S30" s="80"/>
-      <c r="T30" s="80"/>
-      <c r="U30" s="80"/>
-      <c r="V30" s="80"/>
-      <c r="W30" s="80"/>
-      <c r="X30" s="81"/>
+      <c r="L30" s="85"/>
+      <c r="M30" s="85"/>
+      <c r="N30" s="85"/>
+      <c r="O30" s="85"/>
+      <c r="P30" s="85"/>
+      <c r="Q30" s="85"/>
+      <c r="R30" s="85"/>
+      <c r="S30" s="85"/>
+      <c r="T30" s="85"/>
+      <c r="U30" s="85"/>
+      <c r="V30" s="85"/>
+      <c r="W30" s="85"/>
+      <c r="X30" s="86"/>
     </row>
     <row r="31" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K31" s="82"/>
-      <c r="L31" s="83"/>
-      <c r="M31" s="83"/>
-      <c r="N31" s="83"/>
-      <c r="O31" s="83"/>
-      <c r="P31" s="83"/>
-      <c r="Q31" s="83"/>
-      <c r="R31" s="83"/>
-      <c r="S31" s="83"/>
-      <c r="T31" s="83"/>
-      <c r="U31" s="83"/>
-      <c r="V31" s="83"/>
-      <c r="W31" s="83"/>
-      <c r="X31" s="84"/>
+      <c r="K31" s="87"/>
+      <c r="L31" s="88"/>
+      <c r="M31" s="88"/>
+      <c r="N31" s="88"/>
+      <c r="O31" s="88"/>
+      <c r="P31" s="88"/>
+      <c r="Q31" s="88"/>
+      <c r="R31" s="88"/>
+      <c r="S31" s="88"/>
+      <c r="T31" s="88"/>
+      <c r="U31" s="88"/>
+      <c r="V31" s="88"/>
+      <c r="W31" s="88"/>
+      <c r="X31" s="89"/>
     </row>
     <row r="38" spans="11:11" x14ac:dyDescent="0.4">
       <c r="K38" t="s">
@@ -9331,10 +9467,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1494C983-D6B3-4A8C-AA9C-1AD533947069}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:N85"/>
+  <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -9344,10 +9480,10 @@
     <col min="3" max="3" width="62.75" customWidth="1"/>
     <col min="4" max="4" width="17.875" customWidth="1"/>
     <col min="5" max="5" width="11.75" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.125" customWidth="1"/>
+    <col min="6" max="6" width="31.625" customWidth="1"/>
     <col min="7" max="7" width="11.5" customWidth="1"/>
-    <col min="8" max="8" width="17.625" style="99" customWidth="1"/>
-    <col min="9" max="9" width="9" style="101"/>
+    <col min="8" max="8" width="17.625" style="81" customWidth="1"/>
+    <col min="9" max="9" width="9" style="83"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
@@ -9369,19 +9505,19 @@
       <c r="F1" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="G1" s="97" t="s">
+      <c r="G1" s="79" t="s">
         <v>397</v>
       </c>
-      <c r="H1" s="98" t="s">
+      <c r="H1" s="80" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="99" t="s">
         <v>188</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="96"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="101"/>
       <c r="E2"/>
       <c r="H2"/>
       <c r="I2"/>
@@ -9407,10 +9543,10 @@
       <c r="G3" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="H3" s="99">
+      <c r="H3" s="81">
         <v>43623</v>
       </c>
-      <c r="I3" s="101" t="s">
+      <c r="I3" s="83" t="s">
         <v>401</v>
       </c>
     </row>
@@ -9437,10 +9573,10 @@
       <c r="G4" s="34" t="s">
         <v>220</v>
       </c>
-      <c r="H4" s="99">
+      <c r="H4" s="81">
         <v>43630</v>
       </c>
-      <c r="I4" s="101" t="s">
+      <c r="I4" s="83" t="s">
         <v>401</v>
       </c>
     </row>
@@ -9465,10 +9601,10 @@
       <c r="G5" s="34" t="s">
         <v>220</v>
       </c>
-      <c r="H5" s="99">
+      <c r="H5" s="81">
         <v>43630</v>
       </c>
-      <c r="I5" s="101" t="s">
+      <c r="I5" s="83" t="s">
         <v>401</v>
       </c>
     </row>
@@ -9495,19 +9631,19 @@
       <c r="G6" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="H6" s="99">
+      <c r="H6" s="81">
         <v>43630</v>
       </c>
-      <c r="I6" s="101" t="s">
+      <c r="I6" s="83" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="91" t="s">
+      <c r="A7" s="96" t="s">
         <v>190</v>
       </c>
-      <c r="B7" s="92"/>
-      <c r="C7" s="93"/>
+      <c r="B7" s="97"/>
+      <c r="C7" s="98"/>
       <c r="E7"/>
       <c r="H7"/>
       <c r="I7"/>
@@ -9533,10 +9669,10 @@
       <c r="G8" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="H8" s="99" t="s">
+      <c r="H8" s="81" t="s">
         <v>403</v>
       </c>
-      <c r="I8" s="100" t="s">
+      <c r="I8" s="82" t="s">
         <v>399</v>
       </c>
     </row>
@@ -9563,10 +9699,10 @@
       <c r="G9" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="H9" s="99">
+      <c r="H9" s="81">
         <v>43637</v>
       </c>
-      <c r="I9" s="100" t="s">
+      <c r="I9" s="82" t="s">
         <v>404</v>
       </c>
       <c r="K9" t="s">
@@ -9594,7 +9730,7 @@
       <c r="G10" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="I10" s="100" t="s">
+      <c r="I10" s="82" t="s">
         <v>400</v>
       </c>
     </row>
@@ -9619,10 +9755,10 @@
       <c r="G11" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="H11" s="99">
+      <c r="H11" s="81">
         <v>43677</v>
       </c>
-      <c r="I11" s="100" t="s">
+      <c r="I11" s="82" t="s">
         <v>405</v>
       </c>
     </row>
@@ -9649,10 +9785,10 @@
       <c r="G12" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="H12" s="99">
+      <c r="H12" s="81">
         <v>43616</v>
       </c>
-      <c r="I12" s="100" t="s">
+      <c r="I12" s="82" t="s">
         <v>402</v>
       </c>
       <c r="N12" t="s">
@@ -9680,10 +9816,10 @@
       <c r="G13" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="H13" s="99">
+      <c r="H13" s="81">
         <v>43612</v>
       </c>
-      <c r="I13" s="101" t="s">
+      <c r="I13" s="83" t="s">
         <v>414</v>
       </c>
       <c r="N13" t="s">
@@ -9735,10 +9871,10 @@
       <c r="G15" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="H15" s="99">
+      <c r="H15" s="81">
         <v>43612</v>
       </c>
-      <c r="I15" s="101" t="s">
+      <c r="I15" s="83" t="s">
         <v>400</v>
       </c>
     </row>
@@ -9789,7 +9925,7 @@
       <c r="G17" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="I17" s="101" t="s">
+      <c r="I17" s="83" t="s">
         <v>407</v>
       </c>
     </row>
@@ -9816,7 +9952,7 @@
       <c r="G18" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="I18" s="101" t="s">
+      <c r="I18" s="83" t="s">
         <v>409</v>
       </c>
       <c r="N18" t="s">
@@ -9844,7 +9980,7 @@
       <c r="G19" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="I19" s="101" t="s">
+      <c r="I19" s="83" t="s">
         <v>422</v>
       </c>
       <c r="N19" t="s">
@@ -9926,7 +10062,7 @@
       <c r="G22" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="I22" s="101" t="s">
+      <c r="I22" s="83" t="s">
         <v>409</v>
       </c>
       <c r="J22" s="18"/>
@@ -9957,7 +10093,7 @@
       <c r="G23" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="I23" s="101" t="s">
+      <c r="I23" s="83" t="s">
         <v>415</v>
       </c>
       <c r="J23" t="s">
@@ -10141,7 +10277,7 @@
       <c r="G30" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="I30" s="101" t="s">
+      <c r="I30" s="83" t="s">
         <v>417</v>
       </c>
     </row>
@@ -10248,11 +10384,11 @@
       <c r="I34"/>
     </row>
     <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="91" t="s">
+      <c r="A35" s="96" t="s">
         <v>195</v>
       </c>
-      <c r="B35" s="92"/>
-      <c r="C35" s="93"/>
+      <c r="B35" s="97"/>
+      <c r="C35" s="98"/>
       <c r="E35"/>
       <c r="H35"/>
       <c r="I35"/>
@@ -10278,10 +10414,10 @@
       <c r="G36" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="H36" s="99">
+      <c r="H36" s="81">
         <v>43612</v>
       </c>
-      <c r="I36" s="101" t="s">
+      <c r="I36" s="83" t="s">
         <v>410</v>
       </c>
     </row>
@@ -10306,7 +10442,7 @@
       <c r="G37" s="34" t="s">
         <v>220</v>
       </c>
-      <c r="I37" s="101" t="s">
+      <c r="I37" s="83" t="s">
         <v>411</v>
       </c>
     </row>
@@ -10333,7 +10469,7 @@
       <c r="G38" s="40" t="s">
         <v>220</v>
       </c>
-      <c r="I38" s="101" t="s">
+      <c r="I38" s="83" t="s">
         <v>412</v>
       </c>
       <c r="N38" t="s">
@@ -10341,11 +10477,11 @@
       </c>
     </row>
     <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="91" t="s">
+      <c r="A39" s="96" t="s">
         <v>198</v>
       </c>
-      <c r="B39" s="92"/>
-      <c r="C39" s="93"/>
+      <c r="B39" s="97"/>
+      <c r="C39" s="98"/>
       <c r="E39"/>
       <c r="H39"/>
       <c r="I39"/>
@@ -10398,11 +10534,11 @@
       <c r="I41"/>
     </row>
     <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="91" t="s">
+      <c r="A42" s="96" t="s">
         <v>189</v>
       </c>
-      <c r="B42" s="92"/>
-      <c r="C42" s="93"/>
+      <c r="B42" s="97"/>
+      <c r="C42" s="98"/>
       <c r="E42"/>
       <c r="H42"/>
       <c r="I42"/>
@@ -10430,7 +10566,7 @@
       <c r="G43" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="I43" s="101" t="s">
+      <c r="I43" s="83" t="s">
         <v>405</v>
       </c>
     </row>
@@ -10509,7 +10645,7 @@
       <c r="G46" s="34" t="s">
         <v>220</v>
       </c>
-      <c r="I46" s="101" t="s">
+      <c r="I46" s="83" t="s">
         <v>419</v>
       </c>
     </row>
@@ -10536,7 +10672,7 @@
       <c r="G47" s="34" t="s">
         <v>220</v>
       </c>
-      <c r="I47" s="101" t="s">
+      <c r="I47" s="83" t="s">
         <v>405</v>
       </c>
     </row>
@@ -10567,11 +10703,11 @@
       <c r="I48"/>
     </row>
     <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="91" t="s">
+      <c r="A49" s="96" t="s">
         <v>196</v>
       </c>
-      <c r="B49" s="92"/>
-      <c r="C49" s="93"/>
+      <c r="B49" s="97"/>
+      <c r="C49" s="98"/>
       <c r="E49"/>
       <c r="H49"/>
       <c r="I49"/>
@@ -10599,10 +10735,10 @@
       <c r="G50" s="40" t="s">
         <v>220</v>
       </c>
-      <c r="H50" s="99">
+      <c r="H50" s="81">
         <v>43612</v>
       </c>
-      <c r="I50" s="101" t="s">
+      <c r="I50" s="83" t="s">
         <v>418</v>
       </c>
     </row>
@@ -10627,7 +10763,7 @@
       <c r="G51" s="40" t="s">
         <v>220</v>
       </c>
-      <c r="I51" s="101" t="s">
+      <c r="I51" s="83" t="s">
         <v>420</v>
       </c>
       <c r="N51" t="s">
@@ -10657,10 +10793,10 @@
       <c r="G52" s="40" t="s">
         <v>220</v>
       </c>
-      <c r="H52" s="99">
+      <c r="H52" s="81">
         <v>43612</v>
       </c>
-      <c r="I52" s="101" t="s">
+      <c r="I52" s="83" t="s">
         <v>418</v>
       </c>
     </row>
@@ -10687,16 +10823,16 @@
       <c r="G53" s="40" t="s">
         <v>220</v>
       </c>
-      <c r="I53" s="101" t="s">
+      <c r="I53" s="83" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="91" t="s">
+      <c r="A54" s="96" t="s">
         <v>197</v>
       </c>
-      <c r="B54" s="92"/>
-      <c r="C54" s="93"/>
+      <c r="B54" s="97"/>
+      <c r="C54" s="98"/>
       <c r="E54"/>
       <c r="H54" s="19"/>
       <c r="I54"/>
@@ -11233,7 +11369,7 @@
       </c>
       <c r="F80" s="8"/>
     </row>
-    <row r="81" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.4">
       <c r="A81" s="16" t="str">
         <f>COUNTA(E$3:E81)&amp;"."</f>
         <v>73.</v>
@@ -11251,8 +11387,10 @@
         <v>63</v>
       </c>
       <c r="F81" s="8"/>
-    </row>
-    <row r="82" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+      <c r="H81"/>
+      <c r="I81"/>
+    </row>
+    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.4">
       <c r="A82" s="16" t="str">
         <f>COUNTA(E$3:E82)&amp;"."</f>
         <v>74.</v>
@@ -11270,8 +11408,10 @@
         <v>63</v>
       </c>
       <c r="F82" s="8"/>
-    </row>
-    <row r="83" spans="1:6" customFormat="1" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H82"/>
+      <c r="I82"/>
+    </row>
+    <row r="83" spans="1:9" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A83" s="17" t="str">
         <f>COUNTA(E$3:E83)&amp;"."</f>
         <v>75.</v>
@@ -11289,14 +11429,31 @@
         <v>63</v>
       </c>
       <c r="F83" s="10"/>
-    </row>
-    <row r="84" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="1"/>
-      <c r="E84" s="1"/>
-    </row>
-    <row r="85" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="1"/>
-      <c r="E85" s="1"/>
+      <c r="H83"/>
+      <c r="I83"/>
+    </row>
+    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.4">
+      <c r="H84"/>
+      <c r="I84"/>
+    </row>
+    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.4">
+      <c r="H85"/>
+      <c r="I85"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F89" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F90" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="243.75" x14ac:dyDescent="0.4">
+      <c r="F91" s="102" t="s">
+        <v>425</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="G1:G85" xr:uid="{729D066D-B44E-46AC-81FA-7975A774CA00}">
@@ -11325,6 +11482,130 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6511554B-3B83-477E-8F82-CB1DA06B1302}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="109" t="s">
+        <v>426</v>
+      </c>
+      <c r="B1" s="110" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="107" t="s">
+        <v>427</v>
+      </c>
+      <c r="B2" s="108" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" s="103" t="s">
+        <v>428</v>
+      </c>
+      <c r="B3" s="104" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" s="103" t="s">
+        <v>429</v>
+      </c>
+      <c r="B4" s="104" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" s="103" t="s">
+        <v>430</v>
+      </c>
+      <c r="B5" s="104" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" s="103" t="s">
+        <v>431</v>
+      </c>
+      <c r="B6" s="104" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" s="103" t="s">
+        <v>432</v>
+      </c>
+      <c r="B7" s="104" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8" s="103" t="s">
+        <v>433</v>
+      </c>
+      <c r="B8" s="104" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A9" s="103" t="s">
+        <v>434</v>
+      </c>
+      <c r="B9" s="104" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A10" s="103" t="s">
+        <v>435</v>
+      </c>
+      <c r="B10" s="104" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A11" s="103" t="s">
+        <v>440</v>
+      </c>
+      <c r="B11" s="104" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12" s="103" t="s">
+        <v>436</v>
+      </c>
+      <c r="B12" s="104" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="105" t="s">
+        <v>437</v>
+      </c>
+      <c r="B13" s="106" t="s">
+        <v>439</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A53464A6-95CF-4320-84CC-75B433BA2AF9}">
   <dimension ref="A1:G27"/>
   <sheetViews>
@@ -11948,7 +12229,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36417535-E656-49C5-B1CE-46E62C58C912}">
   <dimension ref="B3:E34"/>
   <sheetViews>

</xml_diff>

<commit_message>
CRUD MONGOOSE : Pas fini mais tant pis!
J'ai vu ce que j'ai voulu voir avec ces 2 cruds.
Je passe maintenant au projet tracking
</commit_message>
<xml_diff>
--- a/Cahier des charges/Organisation Projet Nodejs.xlsx
+++ b/Cahier des charges/Organisation Projet Nodejs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\MyEnv\NodeJs\Cahier des charges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0E2E13-CBC6-477D-B8E0-BA393A4D4C7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D136CCE-6EF9-4207-8940-1E936216AC1B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="4" xr2:uid="{D1074EF0-41CD-437C-83BE-5015162961C9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="5" xr2:uid="{D1074EF0-41CD-437C-83BE-5015162961C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="6" r:id="rId1"/>
@@ -18,8 +18,9 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="5" r:id="rId4"/>
     <sheet name="Sheet3" sheetId="7" r:id="rId5"/>
-    <sheet name="bin" sheetId="2" r:id="rId6"/>
-    <sheet name="Model Generator" sheetId="3" r:id="rId7"/>
+    <sheet name="Tracking application Recap" sheetId="8" r:id="rId6"/>
+    <sheet name="bin" sheetId="2" r:id="rId7"/>
+    <sheet name="Model Generator" sheetId="3" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet2!$G$1:$G$85</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="478">
   <si>
     <t>Check bin sheet for more informations</t>
     <phoneticPr fontId="1"/>
@@ -2794,6 +2795,154 @@
   </si>
   <si>
     <t>cookie-parser</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>On le fait en mongoose parce que l'insert est plus rapide</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Collection</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>200/401/402/403/404/500</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>connection_status</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Changing Site path point</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>path</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>connection_time</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>response_time</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>user_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>country</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>error_message</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>promotion</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>promotion_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Long</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>from</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>to</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>uniquement si erreur de navigation</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Boolean</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Uniquement si timed_out</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Uniquement si</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Et avec ces Datas je veux pouvoir repondre a :</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>est-ce que user x est dangereux</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>D'ou vient l'utilisateur en premier</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Une promotion ca donne envie d'acheter?</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Combien ya d'erreur sur le site</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Combien de User en meme temps</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Je veux que le tracking soit independent du site. C'est a dire qu'il n'ai aucun impact sur le code du site a l'exception de l'mport</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Ya t'il des attacks et ca proviendrai d'ou</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>req</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mixed</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Voir ce que les utilisateurs rentrent dans les formulaires</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>crud</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>enum : {'get','post','put','delete'}</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3455,7 +3604,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3708,6 +3857,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3762,32 +3938,11 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9144,276 +9299,276 @@
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="2" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K2" s="84" t="s">
+      <c r="K2" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
-      <c r="R2" s="85"/>
-      <c r="S2" s="85"/>
-      <c r="T2" s="85"/>
-      <c r="U2" s="85"/>
-      <c r="V2" s="85"/>
-      <c r="W2" s="85"/>
-      <c r="X2" s="86"/>
+      <c r="L2" s="94"/>
+      <c r="M2" s="94"/>
+      <c r="N2" s="94"/>
+      <c r="O2" s="94"/>
+      <c r="P2" s="94"/>
+      <c r="Q2" s="94"/>
+      <c r="R2" s="94"/>
+      <c r="S2" s="94"/>
+      <c r="T2" s="94"/>
+      <c r="U2" s="94"/>
+      <c r="V2" s="94"/>
+      <c r="W2" s="94"/>
+      <c r="X2" s="95"/>
     </row>
     <row r="3" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K3" s="87"/>
-      <c r="L3" s="88"/>
-      <c r="M3" s="88"/>
-      <c r="N3" s="88"/>
-      <c r="O3" s="88"/>
-      <c r="P3" s="88"/>
-      <c r="Q3" s="88"/>
-      <c r="R3" s="88"/>
-      <c r="S3" s="88"/>
-      <c r="T3" s="88"/>
-      <c r="U3" s="88"/>
-      <c r="V3" s="88"/>
-      <c r="W3" s="88"/>
-      <c r="X3" s="89"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="97"/>
+      <c r="P3" s="97"/>
+      <c r="Q3" s="97"/>
+      <c r="R3" s="97"/>
+      <c r="S3" s="97"/>
+      <c r="T3" s="97"/>
+      <c r="U3" s="97"/>
+      <c r="V3" s="97"/>
+      <c r="W3" s="97"/>
+      <c r="X3" s="98"/>
     </row>
     <row r="6" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K6" s="84" t="s">
+      <c r="K6" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="85"/>
-      <c r="M6" s="85"/>
-      <c r="N6" s="85"/>
-      <c r="O6" s="85"/>
-      <c r="P6" s="85"/>
-      <c r="Q6" s="85"/>
-      <c r="R6" s="85"/>
-      <c r="S6" s="85"/>
-      <c r="T6" s="85"/>
-      <c r="U6" s="85"/>
-      <c r="V6" s="85"/>
-      <c r="W6" s="85"/>
-      <c r="X6" s="86"/>
+      <c r="L6" s="94"/>
+      <c r="M6" s="94"/>
+      <c r="N6" s="94"/>
+      <c r="O6" s="94"/>
+      <c r="P6" s="94"/>
+      <c r="Q6" s="94"/>
+      <c r="R6" s="94"/>
+      <c r="S6" s="94"/>
+      <c r="T6" s="94"/>
+      <c r="U6" s="94"/>
+      <c r="V6" s="94"/>
+      <c r="W6" s="94"/>
+      <c r="X6" s="95"/>
     </row>
     <row r="7" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K7" s="87"/>
-      <c r="L7" s="88"/>
-      <c r="M7" s="88"/>
-      <c r="N7" s="88"/>
-      <c r="O7" s="88"/>
-      <c r="P7" s="88"/>
-      <c r="Q7" s="88"/>
-      <c r="R7" s="88"/>
-      <c r="S7" s="88"/>
-      <c r="T7" s="88"/>
-      <c r="U7" s="88"/>
-      <c r="V7" s="88"/>
-      <c r="W7" s="88"/>
-      <c r="X7" s="89"/>
+      <c r="K7" s="96"/>
+      <c r="L7" s="97"/>
+      <c r="M7" s="97"/>
+      <c r="N7" s="97"/>
+      <c r="O7" s="97"/>
+      <c r="P7" s="97"/>
+      <c r="Q7" s="97"/>
+      <c r="R7" s="97"/>
+      <c r="S7" s="97"/>
+      <c r="T7" s="97"/>
+      <c r="U7" s="97"/>
+      <c r="V7" s="97"/>
+      <c r="W7" s="97"/>
+      <c r="X7" s="98"/>
     </row>
     <row r="10" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K10" s="90" t="s">
+      <c r="K10" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="L10" s="91"/>
-      <c r="M10" s="91"/>
-      <c r="N10" s="91"/>
-      <c r="O10" s="91"/>
-      <c r="P10" s="91"/>
-      <c r="Q10" s="91"/>
-      <c r="R10" s="91"/>
-      <c r="S10" s="91"/>
-      <c r="T10" s="91"/>
-      <c r="U10" s="91"/>
-      <c r="V10" s="91"/>
-      <c r="W10" s="91"/>
-      <c r="X10" s="92"/>
+      <c r="L10" s="100"/>
+      <c r="M10" s="100"/>
+      <c r="N10" s="100"/>
+      <c r="O10" s="100"/>
+      <c r="P10" s="100"/>
+      <c r="Q10" s="100"/>
+      <c r="R10" s="100"/>
+      <c r="S10" s="100"/>
+      <c r="T10" s="100"/>
+      <c r="U10" s="100"/>
+      <c r="V10" s="100"/>
+      <c r="W10" s="100"/>
+      <c r="X10" s="101"/>
     </row>
     <row r="11" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K11" s="93"/>
-      <c r="L11" s="94"/>
-      <c r="M11" s="94"/>
-      <c r="N11" s="94"/>
-      <c r="O11" s="94"/>
-      <c r="P11" s="94"/>
-      <c r="Q11" s="94"/>
-      <c r="R11" s="94"/>
-      <c r="S11" s="94"/>
-      <c r="T11" s="94"/>
-      <c r="U11" s="94"/>
-      <c r="V11" s="94"/>
-      <c r="W11" s="94"/>
-      <c r="X11" s="95"/>
+      <c r="K11" s="102"/>
+      <c r="L11" s="103"/>
+      <c r="M11" s="103"/>
+      <c r="N11" s="103"/>
+      <c r="O11" s="103"/>
+      <c r="P11" s="103"/>
+      <c r="Q11" s="103"/>
+      <c r="R11" s="103"/>
+      <c r="S11" s="103"/>
+      <c r="T11" s="103"/>
+      <c r="U11" s="103"/>
+      <c r="V11" s="103"/>
+      <c r="W11" s="103"/>
+      <c r="X11" s="104"/>
     </row>
     <row r="14" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K14" s="84" t="s">
+      <c r="K14" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="L14" s="85"/>
-      <c r="M14" s="85"/>
-      <c r="N14" s="85"/>
-      <c r="O14" s="85"/>
-      <c r="P14" s="85"/>
-      <c r="Q14" s="85"/>
-      <c r="R14" s="85"/>
-      <c r="S14" s="85"/>
-      <c r="T14" s="85"/>
-      <c r="U14" s="85"/>
-      <c r="V14" s="85"/>
-      <c r="W14" s="85"/>
-      <c r="X14" s="86"/>
+      <c r="L14" s="94"/>
+      <c r="M14" s="94"/>
+      <c r="N14" s="94"/>
+      <c r="O14" s="94"/>
+      <c r="P14" s="94"/>
+      <c r="Q14" s="94"/>
+      <c r="R14" s="94"/>
+      <c r="S14" s="94"/>
+      <c r="T14" s="94"/>
+      <c r="U14" s="94"/>
+      <c r="V14" s="94"/>
+      <c r="W14" s="94"/>
+      <c r="X14" s="95"/>
     </row>
     <row r="15" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K15" s="87"/>
-      <c r="L15" s="88"/>
-      <c r="M15" s="88"/>
-      <c r="N15" s="88"/>
-      <c r="O15" s="88"/>
-      <c r="P15" s="88"/>
-      <c r="Q15" s="88"/>
-      <c r="R15" s="88"/>
-      <c r="S15" s="88"/>
-      <c r="T15" s="88"/>
-      <c r="U15" s="88"/>
-      <c r="V15" s="88"/>
-      <c r="W15" s="88"/>
-      <c r="X15" s="89"/>
+      <c r="K15" s="96"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="97"/>
+      <c r="O15" s="97"/>
+      <c r="P15" s="97"/>
+      <c r="Q15" s="97"/>
+      <c r="R15" s="97"/>
+      <c r="S15" s="97"/>
+      <c r="T15" s="97"/>
+      <c r="U15" s="97"/>
+      <c r="V15" s="97"/>
+      <c r="W15" s="97"/>
+      <c r="X15" s="98"/>
     </row>
     <row r="18" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K18" s="84" t="s">
+      <c r="K18" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="L18" s="85"/>
-      <c r="M18" s="85"/>
-      <c r="N18" s="85"/>
-      <c r="O18" s="85"/>
-      <c r="P18" s="85"/>
-      <c r="Q18" s="85"/>
-      <c r="R18" s="85"/>
-      <c r="S18" s="85"/>
-      <c r="T18" s="85"/>
-      <c r="U18" s="85"/>
-      <c r="V18" s="85"/>
-      <c r="W18" s="85"/>
-      <c r="X18" s="86"/>
+      <c r="L18" s="94"/>
+      <c r="M18" s="94"/>
+      <c r="N18" s="94"/>
+      <c r="O18" s="94"/>
+      <c r="P18" s="94"/>
+      <c r="Q18" s="94"/>
+      <c r="R18" s="94"/>
+      <c r="S18" s="94"/>
+      <c r="T18" s="94"/>
+      <c r="U18" s="94"/>
+      <c r="V18" s="94"/>
+      <c r="W18" s="94"/>
+      <c r="X18" s="95"/>
     </row>
     <row r="19" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K19" s="87"/>
-      <c r="L19" s="88"/>
-      <c r="M19" s="88"/>
-      <c r="N19" s="88"/>
-      <c r="O19" s="88"/>
-      <c r="P19" s="88"/>
-      <c r="Q19" s="88"/>
-      <c r="R19" s="88"/>
-      <c r="S19" s="88"/>
-      <c r="T19" s="88"/>
-      <c r="U19" s="88"/>
-      <c r="V19" s="88"/>
-      <c r="W19" s="88"/>
-      <c r="X19" s="89"/>
+      <c r="K19" s="96"/>
+      <c r="L19" s="97"/>
+      <c r="M19" s="97"/>
+      <c r="N19" s="97"/>
+      <c r="O19" s="97"/>
+      <c r="P19" s="97"/>
+      <c r="Q19" s="97"/>
+      <c r="R19" s="97"/>
+      <c r="S19" s="97"/>
+      <c r="T19" s="97"/>
+      <c r="U19" s="97"/>
+      <c r="V19" s="97"/>
+      <c r="W19" s="97"/>
+      <c r="X19" s="98"/>
     </row>
     <row r="22" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K22" s="84" t="s">
+      <c r="K22" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="L22" s="85"/>
-      <c r="M22" s="85"/>
-      <c r="N22" s="85"/>
-      <c r="O22" s="85"/>
-      <c r="P22" s="85"/>
-      <c r="Q22" s="85"/>
-      <c r="R22" s="85"/>
-      <c r="S22" s="85"/>
-      <c r="T22" s="85"/>
-      <c r="U22" s="85"/>
-      <c r="V22" s="85"/>
-      <c r="W22" s="85"/>
-      <c r="X22" s="86"/>
+      <c r="L22" s="94"/>
+      <c r="M22" s="94"/>
+      <c r="N22" s="94"/>
+      <c r="O22" s="94"/>
+      <c r="P22" s="94"/>
+      <c r="Q22" s="94"/>
+      <c r="R22" s="94"/>
+      <c r="S22" s="94"/>
+      <c r="T22" s="94"/>
+      <c r="U22" s="94"/>
+      <c r="V22" s="94"/>
+      <c r="W22" s="94"/>
+      <c r="X22" s="95"/>
     </row>
     <row r="23" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K23" s="87"/>
-      <c r="L23" s="88"/>
-      <c r="M23" s="88"/>
-      <c r="N23" s="88"/>
-      <c r="O23" s="88"/>
-      <c r="P23" s="88"/>
-      <c r="Q23" s="88"/>
-      <c r="R23" s="88"/>
-      <c r="S23" s="88"/>
-      <c r="T23" s="88"/>
-      <c r="U23" s="88"/>
-      <c r="V23" s="88"/>
-      <c r="W23" s="88"/>
-      <c r="X23" s="89"/>
+      <c r="K23" s="96"/>
+      <c r="L23" s="97"/>
+      <c r="M23" s="97"/>
+      <c r="N23" s="97"/>
+      <c r="O23" s="97"/>
+      <c r="P23" s="97"/>
+      <c r="Q23" s="97"/>
+      <c r="R23" s="97"/>
+      <c r="S23" s="97"/>
+      <c r="T23" s="97"/>
+      <c r="U23" s="97"/>
+      <c r="V23" s="97"/>
+      <c r="W23" s="97"/>
+      <c r="X23" s="98"/>
     </row>
     <row r="26" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K26" s="84" t="s">
+      <c r="K26" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="L26" s="85"/>
-      <c r="M26" s="85"/>
-      <c r="N26" s="85"/>
-      <c r="O26" s="85"/>
-      <c r="P26" s="85"/>
-      <c r="Q26" s="85"/>
-      <c r="R26" s="85"/>
-      <c r="S26" s="85"/>
-      <c r="T26" s="85"/>
-      <c r="U26" s="85"/>
-      <c r="V26" s="85"/>
-      <c r="W26" s="85"/>
-      <c r="X26" s="86"/>
+      <c r="L26" s="94"/>
+      <c r="M26" s="94"/>
+      <c r="N26" s="94"/>
+      <c r="O26" s="94"/>
+      <c r="P26" s="94"/>
+      <c r="Q26" s="94"/>
+      <c r="R26" s="94"/>
+      <c r="S26" s="94"/>
+      <c r="T26" s="94"/>
+      <c r="U26" s="94"/>
+      <c r="V26" s="94"/>
+      <c r="W26" s="94"/>
+      <c r="X26" s="95"/>
     </row>
     <row r="27" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K27" s="87"/>
-      <c r="L27" s="88"/>
-      <c r="M27" s="88"/>
-      <c r="N27" s="88"/>
-      <c r="O27" s="88"/>
-      <c r="P27" s="88"/>
-      <c r="Q27" s="88"/>
-      <c r="R27" s="88"/>
-      <c r="S27" s="88"/>
-      <c r="T27" s="88"/>
-      <c r="U27" s="88"/>
-      <c r="V27" s="88"/>
-      <c r="W27" s="88"/>
-      <c r="X27" s="89"/>
+      <c r="K27" s="96"/>
+      <c r="L27" s="97"/>
+      <c r="M27" s="97"/>
+      <c r="N27" s="97"/>
+      <c r="O27" s="97"/>
+      <c r="P27" s="97"/>
+      <c r="Q27" s="97"/>
+      <c r="R27" s="97"/>
+      <c r="S27" s="97"/>
+      <c r="T27" s="97"/>
+      <c r="U27" s="97"/>
+      <c r="V27" s="97"/>
+      <c r="W27" s="97"/>
+      <c r="X27" s="98"/>
     </row>
     <row r="30" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K30" s="84" t="s">
+      <c r="K30" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="L30" s="85"/>
-      <c r="M30" s="85"/>
-      <c r="N30" s="85"/>
-      <c r="O30" s="85"/>
-      <c r="P30" s="85"/>
-      <c r="Q30" s="85"/>
-      <c r="R30" s="85"/>
-      <c r="S30" s="85"/>
-      <c r="T30" s="85"/>
-      <c r="U30" s="85"/>
-      <c r="V30" s="85"/>
-      <c r="W30" s="85"/>
-      <c r="X30" s="86"/>
+      <c r="L30" s="94"/>
+      <c r="M30" s="94"/>
+      <c r="N30" s="94"/>
+      <c r="O30" s="94"/>
+      <c r="P30" s="94"/>
+      <c r="Q30" s="94"/>
+      <c r="R30" s="94"/>
+      <c r="S30" s="94"/>
+      <c r="T30" s="94"/>
+      <c r="U30" s="94"/>
+      <c r="V30" s="94"/>
+      <c r="W30" s="94"/>
+      <c r="X30" s="95"/>
     </row>
     <row r="31" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K31" s="87"/>
-      <c r="L31" s="88"/>
-      <c r="M31" s="88"/>
-      <c r="N31" s="88"/>
-      <c r="O31" s="88"/>
-      <c r="P31" s="88"/>
-      <c r="Q31" s="88"/>
-      <c r="R31" s="88"/>
-      <c r="S31" s="88"/>
-      <c r="T31" s="88"/>
-      <c r="U31" s="88"/>
-      <c r="V31" s="88"/>
-      <c r="W31" s="88"/>
-      <c r="X31" s="89"/>
+      <c r="K31" s="96"/>
+      <c r="L31" s="97"/>
+      <c r="M31" s="97"/>
+      <c r="N31" s="97"/>
+      <c r="O31" s="97"/>
+      <c r="P31" s="97"/>
+      <c r="Q31" s="97"/>
+      <c r="R31" s="97"/>
+      <c r="S31" s="97"/>
+      <c r="T31" s="97"/>
+      <c r="U31" s="97"/>
+      <c r="V31" s="97"/>
+      <c r="W31" s="97"/>
+      <c r="X31" s="98"/>
     </row>
     <row r="38" spans="11:11" x14ac:dyDescent="0.4">
       <c r="K38" t="s">
@@ -9513,11 +9668,11 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="108" t="s">
         <v>188</v>
       </c>
-      <c r="B2" s="100"/>
-      <c r="C2" s="101"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="110"/>
       <c r="E2"/>
       <c r="H2"/>
       <c r="I2"/>
@@ -9639,11 +9794,11 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="96" t="s">
+      <c r="A7" s="105" t="s">
         <v>190</v>
       </c>
-      <c r="B7" s="97"/>
-      <c r="C7" s="98"/>
+      <c r="B7" s="106"/>
+      <c r="C7" s="107"/>
       <c r="E7"/>
       <c r="H7"/>
       <c r="I7"/>
@@ -10384,11 +10539,11 @@
       <c r="I34"/>
     </row>
     <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="96" t="s">
+      <c r="A35" s="105" t="s">
         <v>195</v>
       </c>
-      <c r="B35" s="97"/>
-      <c r="C35" s="98"/>
+      <c r="B35" s="106"/>
+      <c r="C35" s="107"/>
       <c r="E35"/>
       <c r="H35"/>
       <c r="I35"/>
@@ -10477,11 +10632,11 @@
       </c>
     </row>
     <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="96" t="s">
+      <c r="A39" s="105" t="s">
         <v>198</v>
       </c>
-      <c r="B39" s="97"/>
-      <c r="C39" s="98"/>
+      <c r="B39" s="106"/>
+      <c r="C39" s="107"/>
       <c r="E39"/>
       <c r="H39"/>
       <c r="I39"/>
@@ -10534,11 +10689,11 @@
       <c r="I41"/>
     </row>
     <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="96" t="s">
+      <c r="A42" s="105" t="s">
         <v>189</v>
       </c>
-      <c r="B42" s="97"/>
-      <c r="C42" s="98"/>
+      <c r="B42" s="106"/>
+      <c r="C42" s="107"/>
       <c r="E42"/>
       <c r="H42"/>
       <c r="I42"/>
@@ -10703,11 +10858,11 @@
       <c r="I48"/>
     </row>
     <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="96" t="s">
+      <c r="A49" s="105" t="s">
         <v>196</v>
       </c>
-      <c r="B49" s="97"/>
-      <c r="C49" s="98"/>
+      <c r="B49" s="106"/>
+      <c r="C49" s="107"/>
       <c r="E49"/>
       <c r="H49"/>
       <c r="I49"/>
@@ -10828,11 +10983,11 @@
       </c>
     </row>
     <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="96" t="s">
+      <c r="A54" s="105" t="s">
         <v>197</v>
       </c>
-      <c r="B54" s="97"/>
-      <c r="C54" s="98"/>
+      <c r="B54" s="106"/>
+      <c r="C54" s="107"/>
       <c r="E54"/>
       <c r="H54" s="19"/>
       <c r="I54"/>
@@ -11451,7 +11606,7 @@
       </c>
     </row>
     <row r="91" spans="1:9" ht="243.75" x14ac:dyDescent="0.4">
-      <c r="F91" s="102" t="s">
+      <c r="F91" s="84" t="s">
         <v>425</v>
       </c>
     </row>
@@ -11483,10 +11638,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6511554B-3B83-477E-8F82-CB1DA06B1302}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -11495,117 +11650,371 @@
     <col min="2" max="2" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="109" t="s">
+    <row r="1" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="91" t="s">
         <v>426</v>
       </c>
-      <c r="B1" s="110" t="s">
+      <c r="B1" s="92" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A2" s="107" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" s="89" t="s">
         <v>427</v>
       </c>
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="90" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A3" s="103" t="s">
+      <c r="C2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" s="85" t="s">
         <v>428</v>
       </c>
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="86" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4" s="103" t="s">
+      <c r="C3" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" s="85" t="s">
         <v>429</v>
       </c>
-      <c r="B4" s="104" t="s">
+      <c r="B4" s="86" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="103" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" s="85" t="s">
         <v>430</v>
       </c>
-      <c r="B5" s="104" t="s">
+      <c r="B5" s="86" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" s="103" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" s="85" t="s">
         <v>431</v>
       </c>
-      <c r="B6" s="104" t="s">
+      <c r="B6" s="86" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7" s="103" t="s">
+      <c r="C6" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" s="85" t="s">
         <v>432</v>
       </c>
-      <c r="B7" s="104" t="s">
+      <c r="B7" s="86" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A8" s="103" t="s">
+      <c r="C7" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" s="85" t="s">
         <v>433</v>
       </c>
-      <c r="B8" s="104" t="s">
+      <c r="B8" s="86" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A9" s="103" t="s">
+      <c r="C8" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" s="85" t="s">
         <v>434</v>
       </c>
-      <c r="B9" s="104" t="s">
+      <c r="B9" s="86" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A10" s="103" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" s="85" t="s">
         <v>435</v>
       </c>
-      <c r="B10" s="104" t="s">
+      <c r="B10" s="86" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A11" s="103" t="s">
+      <c r="C10" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" s="85" t="s">
         <v>440</v>
       </c>
-      <c r="B11" s="104" t="s">
+      <c r="B11" s="86" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A12" s="103" t="s">
+      <c r="C11" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" s="85" t="s">
         <v>436</v>
       </c>
-      <c r="B12" s="104" t="s">
+      <c r="B12" s="86" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="105" t="s">
+      <c r="C12" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="87" t="s">
         <v>437</v>
       </c>
-      <c r="B13" s="106" t="s">
+      <c r="B13" s="88" t="s">
         <v>439</v>
       </c>
+      <c r="C13" t="s">
+        <v>441</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA67DCE-BBF2-410C-9E82-B8F1A39A9A5C}">
+  <dimension ref="B3:Q33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="18.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="C6" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="D7" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="D8" t="s">
+        <v>446</v>
+      </c>
+      <c r="E8" t="s">
+        <v>456</v>
+      </c>
+      <c r="F8" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="D9" t="s">
+        <v>448</v>
+      </c>
+      <c r="E9" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="D10" t="s">
+        <v>449</v>
+      </c>
+      <c r="E10" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="D11" t="s">
+        <v>450</v>
+      </c>
+      <c r="E11" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="D12" t="s">
+        <v>451</v>
+      </c>
+      <c r="E12" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="D13" t="s">
+        <v>453</v>
+      </c>
+      <c r="E13" t="s">
+        <v>458</v>
+      </c>
+      <c r="F13" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="D14" t="s">
+        <v>455</v>
+      </c>
+      <c r="E14" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="D15" t="s">
+        <v>459</v>
+      </c>
+      <c r="E15" t="s">
+        <v>458</v>
+      </c>
+      <c r="F15" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="D16" t="s">
+        <v>460</v>
+      </c>
+      <c r="E16" t="s">
+        <v>458</v>
+      </c>
+      <c r="F16" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.4">
+      <c r="D17" t="s">
+        <v>473</v>
+      </c>
+      <c r="E17" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.4">
+      <c r="D18" t="s">
+        <v>476</v>
+      </c>
+      <c r="E18" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.4">
+      <c r="C23" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="24" spans="3:17" x14ac:dyDescent="0.4">
+      <c r="D24" t="s">
+        <v>466</v>
+      </c>
+      <c r="H24" s="111" t="s">
+        <v>473</v>
+      </c>
+      <c r="I24" s="112" t="s">
+        <v>446</v>
+      </c>
+      <c r="J24" s="112"/>
+      <c r="K24" s="112" t="s">
+        <v>449</v>
+      </c>
+      <c r="L24" s="112"/>
+      <c r="M24" s="111" t="s">
+        <v>451</v>
+      </c>
+      <c r="N24" s="111" t="s">
+        <v>452</v>
+      </c>
+      <c r="O24" s="112" t="s">
+        <v>453</v>
+      </c>
+      <c r="P24" s="112"/>
+      <c r="Q24" s="111" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="25" spans="3:17" x14ac:dyDescent="0.4">
+      <c r="D25" t="s">
+        <v>467</v>
+      </c>
+      <c r="H25" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="26" spans="3:17" x14ac:dyDescent="0.4">
+      <c r="D26" t="s">
+        <v>468</v>
+      </c>
+      <c r="H26" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="27" spans="3:17" x14ac:dyDescent="0.4">
+      <c r="D27" t="s">
+        <v>469</v>
+      </c>
+      <c r="H27" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.4">
+      <c r="D28" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="29" spans="3:17" x14ac:dyDescent="0.4">
+      <c r="D29" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="30" spans="3:17" x14ac:dyDescent="0.4">
+      <c r="D30" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C33" t="s">
+        <v>471</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="O24:P24"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A53464A6-95CF-4320-84CC-75B433BA2AF9}">
   <dimension ref="A1:G27"/>
   <sheetViews>
@@ -12229,7 +12638,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36417535-E656-49C5-B1CE-46E62C58C912}">
   <dimension ref="B3:E34"/>
   <sheetViews>

</xml_diff>

<commit_message>
Tracking multi connection termine!
Pour la suite :
 - Faire fonctionner les fonctions suivantes !
    getDangerousRequests
    getHowLongOnPage
    getMostViewedPageOnPlage
    getLessViewedPageOnPlage
</commit_message>
<xml_diff>
--- a/Cahier des charges/Organisation Projet Nodejs.xlsx
+++ b/Cahier des charges/Organisation Projet Nodejs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\MyEnv\NodeJs\Cahier des charges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDC032C-25C4-4660-A9E7-1EAF467A905A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98341D7B-A2EB-4A7A-BC1F-54C134DE48CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="5" xr2:uid="{D1074EF0-41CD-437C-83BE-5015162961C9}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="584">
   <si>
     <t>Check bin sheet for more informations</t>
     <phoneticPr fontId="1"/>
@@ -5354,6 +5354,14 @@
   </si>
   <si>
     <t>requete avec char spec</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>a faire</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -14542,8 +14550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA67DCE-BBF2-410C-9E82-B8F1A39A9A5C}">
   <dimension ref="A1:U165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -15146,7 +15154,9 @@
       <c r="K23" s="124" t="s">
         <v>451</v>
       </c>
-      <c r="L23" s="122"/>
+      <c r="L23" s="122" t="s">
+        <v>583</v>
+      </c>
       <c r="M23" s="122"/>
       <c r="N23" s="122"/>
       <c r="O23" s="122"/>
@@ -15177,7 +15187,9 @@
       <c r="K24" s="128" t="s">
         <v>451</v>
       </c>
-      <c r="L24" s="126"/>
+      <c r="L24" s="126" t="s">
+        <v>582</v>
+      </c>
       <c r="M24" s="126"/>
       <c r="N24" s="126"/>
       <c r="O24" s="126"/>
@@ -15208,7 +15220,9 @@
       <c r="K25" s="134" t="s">
         <v>451</v>
       </c>
-      <c r="L25" s="132"/>
+      <c r="L25" s="132" t="s">
+        <v>582</v>
+      </c>
       <c r="M25" s="132"/>
       <c r="N25" s="132"/>
       <c r="O25" s="132"/>
@@ -15237,7 +15251,9 @@
       <c r="K26" s="112" t="s">
         <v>455</v>
       </c>
-      <c r="L26" s="107"/>
+      <c r="L26" s="107" t="s">
+        <v>583</v>
+      </c>
       <c r="M26" s="107"/>
       <c r="N26" s="107"/>
       <c r="O26" s="107"/>
@@ -15268,7 +15284,9 @@
       <c r="K27" s="112" t="s">
         <v>451</v>
       </c>
-      <c r="L27" s="107"/>
+      <c r="L27" s="107" t="s">
+        <v>583</v>
+      </c>
       <c r="M27" s="107"/>
       <c r="N27" s="107"/>
       <c r="O27" s="107"/>
@@ -15299,7 +15317,9 @@
       <c r="K28" s="112" t="s">
         <v>451</v>
       </c>
-      <c r="L28" s="107"/>
+      <c r="L28" s="107" t="s">
+        <v>583</v>
+      </c>
       <c r="M28" s="107"/>
       <c r="N28" s="107"/>
       <c r="O28" s="107"/>

</xml_diff>

<commit_message>
continuer le info page
</commit_message>
<xml_diff>
--- a/Cahier des charges/Organisation Projet Nodejs.xlsx
+++ b/Cahier des charges/Organisation Projet Nodejs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\MyEnv\NodeJs\Cahier des charges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71B6490-5B45-4381-B704-ACB5CBF13120}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA71DB5-8F22-4D1C-94E8-BE5F8CAF1546}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="5" xr2:uid="{D1074EF0-41CD-437C-83BE-5015162961C9}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="585">
   <si>
     <t>Check bin sheet for more informations</t>
     <phoneticPr fontId="1"/>
@@ -2810,26 +2810,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Combien ya d'erreur sur le site</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Combien de User en meme temps</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Un utilisateur reste combien de temps en moyenne sur une page</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>quelle est la page la plus visite</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>quelle est la page la moins visite</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>quels utilisateurs peuvent etre dangereux</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -2842,59 +2826,15 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>xxx/error</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>xxx/numuser</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>activite par pays</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>POST</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>activite d'un user</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xxx/activity/country</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xxx/activity/user</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>activite d'une page</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>{"country" : "jp", "periode" : { "from" : "2019-05-30", "to" : "2019-05-31" } }</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>{"user_id" : "Npokfdn2Skg29sDqpJ", "periode" : { "from" : "2019-05-30", "to" : "2019-05-31" } }</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>xxx/page?sort=1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xxx/page?sort=0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>{"path" : "www.test.monsite.com/JOO", "periode" : { "from" : "2019-05-30", "to" : "2019-05-31" } }</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xxx/activity/page</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -5470,6 +5410,55 @@
     <rPh sb="6" eb="8">
       <t>ベンキョウ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>classement page</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>info page 詳細</t>
+    <rPh sb="10" eb="12">
+      <t>ショウサイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>par nombre de vu
+par nombre de requete dangereuses
+par nombre de multico
+par most viewed by user
+par pays
+par error
+par plus longtemps vu</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>quel appareil utilise</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>provenance</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>unique visitors</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>avg visit duration</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>changer couleurs lorsque promotion</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>using cookies</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>a faire k</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5806,7 +5795,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -6284,30 +6273,6 @@
       <left style="medium">
         <color theme="0"/>
       </left>
-      <right style="medium">
-        <color theme="0"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="0"/>
-      </left>
-      <right style="medium">
-        <color theme="0"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="0"/>
-      </left>
       <right/>
       <top style="medium">
         <color theme="0"/>
@@ -6350,7 +6315,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -6687,12 +6652,6 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -6714,46 +6673,16 @@
     <xf numFmtId="0" fontId="37" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6810,8 +6739,50 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -11599,8 +11570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471BD040-1E5E-4739-AB8B-4F419BB83EB3}">
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I133" sqref="I133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -12161,283 +12132,283 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77345D74-9AC5-419C-A473-B6ACCC99F7CE}">
   <dimension ref="K2:X39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q35" sqref="Q35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="2" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K2" s="135" t="s">
+      <c r="K2" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="136"/>
-      <c r="M2" s="136"/>
-      <c r="N2" s="136"/>
-      <c r="O2" s="136"/>
-      <c r="P2" s="136"/>
-      <c r="Q2" s="136"/>
-      <c r="R2" s="136"/>
-      <c r="S2" s="136"/>
-      <c r="T2" s="136"/>
-      <c r="U2" s="136"/>
-      <c r="V2" s="136"/>
-      <c r="W2" s="136"/>
-      <c r="X2" s="137"/>
+      <c r="L2" s="124"/>
+      <c r="M2" s="124"/>
+      <c r="N2" s="124"/>
+      <c r="O2" s="124"/>
+      <c r="P2" s="124"/>
+      <c r="Q2" s="124"/>
+      <c r="R2" s="124"/>
+      <c r="S2" s="124"/>
+      <c r="T2" s="124"/>
+      <c r="U2" s="124"/>
+      <c r="V2" s="124"/>
+      <c r="W2" s="124"/>
+      <c r="X2" s="125"/>
     </row>
     <row r="3" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K3" s="138"/>
-      <c r="L3" s="139"/>
-      <c r="M3" s="139"/>
-      <c r="N3" s="139"/>
-      <c r="O3" s="139"/>
-      <c r="P3" s="139"/>
-      <c r="Q3" s="139"/>
-      <c r="R3" s="139"/>
-      <c r="S3" s="139"/>
-      <c r="T3" s="139"/>
-      <c r="U3" s="139"/>
-      <c r="V3" s="139"/>
-      <c r="W3" s="139"/>
-      <c r="X3" s="140"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="127"/>
+      <c r="M3" s="127"/>
+      <c r="N3" s="127"/>
+      <c r="O3" s="127"/>
+      <c r="P3" s="127"/>
+      <c r="Q3" s="127"/>
+      <c r="R3" s="127"/>
+      <c r="S3" s="127"/>
+      <c r="T3" s="127"/>
+      <c r="U3" s="127"/>
+      <c r="V3" s="127"/>
+      <c r="W3" s="127"/>
+      <c r="X3" s="128"/>
     </row>
     <row r="6" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K6" s="135" t="s">
+      <c r="K6" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="136"/>
-      <c r="M6" s="136"/>
-      <c r="N6" s="136"/>
-      <c r="O6" s="136"/>
-      <c r="P6" s="136"/>
-      <c r="Q6" s="136"/>
-      <c r="R6" s="136"/>
-      <c r="S6" s="136"/>
-      <c r="T6" s="136"/>
-      <c r="U6" s="136"/>
-      <c r="V6" s="136"/>
-      <c r="W6" s="136"/>
-      <c r="X6" s="137"/>
+      <c r="L6" s="124"/>
+      <c r="M6" s="124"/>
+      <c r="N6" s="124"/>
+      <c r="O6" s="124"/>
+      <c r="P6" s="124"/>
+      <c r="Q6" s="124"/>
+      <c r="R6" s="124"/>
+      <c r="S6" s="124"/>
+      <c r="T6" s="124"/>
+      <c r="U6" s="124"/>
+      <c r="V6" s="124"/>
+      <c r="W6" s="124"/>
+      <c r="X6" s="125"/>
     </row>
     <row r="7" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K7" s="138"/>
-      <c r="L7" s="139"/>
-      <c r="M7" s="139"/>
-      <c r="N7" s="139"/>
-      <c r="O7" s="139"/>
-      <c r="P7" s="139"/>
-      <c r="Q7" s="139"/>
-      <c r="R7" s="139"/>
-      <c r="S7" s="139"/>
-      <c r="T7" s="139"/>
-      <c r="U7" s="139"/>
-      <c r="V7" s="139"/>
-      <c r="W7" s="139"/>
-      <c r="X7" s="140"/>
+      <c r="K7" s="126"/>
+      <c r="L7" s="127"/>
+      <c r="M7" s="127"/>
+      <c r="N7" s="127"/>
+      <c r="O7" s="127"/>
+      <c r="P7" s="127"/>
+      <c r="Q7" s="127"/>
+      <c r="R7" s="127"/>
+      <c r="S7" s="127"/>
+      <c r="T7" s="127"/>
+      <c r="U7" s="127"/>
+      <c r="V7" s="127"/>
+      <c r="W7" s="127"/>
+      <c r="X7" s="128"/>
     </row>
     <row r="10" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K10" s="141" t="s">
+      <c r="K10" s="129" t="s">
         <v>1</v>
       </c>
-      <c r="L10" s="142"/>
-      <c r="M10" s="142"/>
-      <c r="N10" s="142"/>
-      <c r="O10" s="142"/>
-      <c r="P10" s="142"/>
-      <c r="Q10" s="142"/>
-      <c r="R10" s="142"/>
-      <c r="S10" s="142"/>
-      <c r="T10" s="142"/>
-      <c r="U10" s="142"/>
-      <c r="V10" s="142"/>
-      <c r="W10" s="142"/>
-      <c r="X10" s="143"/>
+      <c r="L10" s="130"/>
+      <c r="M10" s="130"/>
+      <c r="N10" s="130"/>
+      <c r="O10" s="130"/>
+      <c r="P10" s="130"/>
+      <c r="Q10" s="130"/>
+      <c r="R10" s="130"/>
+      <c r="S10" s="130"/>
+      <c r="T10" s="130"/>
+      <c r="U10" s="130"/>
+      <c r="V10" s="130"/>
+      <c r="W10" s="130"/>
+      <c r="X10" s="131"/>
     </row>
     <row r="11" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K11" s="144"/>
-      <c r="L11" s="145"/>
-      <c r="M11" s="145"/>
-      <c r="N11" s="145"/>
-      <c r="O11" s="145"/>
-      <c r="P11" s="145"/>
-      <c r="Q11" s="145"/>
-      <c r="R11" s="145"/>
-      <c r="S11" s="145"/>
-      <c r="T11" s="145"/>
-      <c r="U11" s="145"/>
-      <c r="V11" s="145"/>
-      <c r="W11" s="145"/>
-      <c r="X11" s="146"/>
+      <c r="K11" s="132"/>
+      <c r="L11" s="133"/>
+      <c r="M11" s="133"/>
+      <c r="N11" s="133"/>
+      <c r="O11" s="133"/>
+      <c r="P11" s="133"/>
+      <c r="Q11" s="133"/>
+      <c r="R11" s="133"/>
+      <c r="S11" s="133"/>
+      <c r="T11" s="133"/>
+      <c r="U11" s="133"/>
+      <c r="V11" s="133"/>
+      <c r="W11" s="133"/>
+      <c r="X11" s="134"/>
     </row>
     <row r="14" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K14" s="135" t="s">
+      <c r="K14" s="123" t="s">
         <v>3</v>
       </c>
-      <c r="L14" s="136"/>
-      <c r="M14" s="136"/>
-      <c r="N14" s="136"/>
-      <c r="O14" s="136"/>
-      <c r="P14" s="136"/>
-      <c r="Q14" s="136"/>
-      <c r="R14" s="136"/>
-      <c r="S14" s="136"/>
-      <c r="T14" s="136"/>
-      <c r="U14" s="136"/>
-      <c r="V14" s="136"/>
-      <c r="W14" s="136"/>
-      <c r="X14" s="137"/>
+      <c r="L14" s="124"/>
+      <c r="M14" s="124"/>
+      <c r="N14" s="124"/>
+      <c r="O14" s="124"/>
+      <c r="P14" s="124"/>
+      <c r="Q14" s="124"/>
+      <c r="R14" s="124"/>
+      <c r="S14" s="124"/>
+      <c r="T14" s="124"/>
+      <c r="U14" s="124"/>
+      <c r="V14" s="124"/>
+      <c r="W14" s="124"/>
+      <c r="X14" s="125"/>
     </row>
     <row r="15" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K15" s="138"/>
-      <c r="L15" s="139"/>
-      <c r="M15" s="139"/>
-      <c r="N15" s="139"/>
-      <c r="O15" s="139"/>
-      <c r="P15" s="139"/>
-      <c r="Q15" s="139"/>
-      <c r="R15" s="139"/>
-      <c r="S15" s="139"/>
-      <c r="T15" s="139"/>
-      <c r="U15" s="139"/>
-      <c r="V15" s="139"/>
-      <c r="W15" s="139"/>
-      <c r="X15" s="140"/>
+      <c r="K15" s="126"/>
+      <c r="L15" s="127"/>
+      <c r="M15" s="127"/>
+      <c r="N15" s="127"/>
+      <c r="O15" s="127"/>
+      <c r="P15" s="127"/>
+      <c r="Q15" s="127"/>
+      <c r="R15" s="127"/>
+      <c r="S15" s="127"/>
+      <c r="T15" s="127"/>
+      <c r="U15" s="127"/>
+      <c r="V15" s="127"/>
+      <c r="W15" s="127"/>
+      <c r="X15" s="128"/>
     </row>
     <row r="18" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K18" s="135" t="s">
+      <c r="K18" s="123" t="s">
         <v>5</v>
       </c>
-      <c r="L18" s="136"/>
-      <c r="M18" s="136"/>
-      <c r="N18" s="136"/>
-      <c r="O18" s="136"/>
-      <c r="P18" s="136"/>
-      <c r="Q18" s="136"/>
-      <c r="R18" s="136"/>
-      <c r="S18" s="136"/>
-      <c r="T18" s="136"/>
-      <c r="U18" s="136"/>
-      <c r="V18" s="136"/>
-      <c r="W18" s="136"/>
-      <c r="X18" s="137"/>
+      <c r="L18" s="124"/>
+      <c r="M18" s="124"/>
+      <c r="N18" s="124"/>
+      <c r="O18" s="124"/>
+      <c r="P18" s="124"/>
+      <c r="Q18" s="124"/>
+      <c r="R18" s="124"/>
+      <c r="S18" s="124"/>
+      <c r="T18" s="124"/>
+      <c r="U18" s="124"/>
+      <c r="V18" s="124"/>
+      <c r="W18" s="124"/>
+      <c r="X18" s="125"/>
     </row>
     <row r="19" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K19" s="138"/>
-      <c r="L19" s="139"/>
-      <c r="M19" s="139"/>
-      <c r="N19" s="139"/>
-      <c r="O19" s="139"/>
-      <c r="P19" s="139"/>
-      <c r="Q19" s="139"/>
-      <c r="R19" s="139"/>
-      <c r="S19" s="139"/>
-      <c r="T19" s="139"/>
-      <c r="U19" s="139"/>
-      <c r="V19" s="139"/>
-      <c r="W19" s="139"/>
-      <c r="X19" s="140"/>
+      <c r="K19" s="126"/>
+      <c r="L19" s="127"/>
+      <c r="M19" s="127"/>
+      <c r="N19" s="127"/>
+      <c r="O19" s="127"/>
+      <c r="P19" s="127"/>
+      <c r="Q19" s="127"/>
+      <c r="R19" s="127"/>
+      <c r="S19" s="127"/>
+      <c r="T19" s="127"/>
+      <c r="U19" s="127"/>
+      <c r="V19" s="127"/>
+      <c r="W19" s="127"/>
+      <c r="X19" s="128"/>
     </row>
     <row r="22" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K22" s="135" t="s">
+      <c r="K22" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="L22" s="136"/>
-      <c r="M22" s="136"/>
-      <c r="N22" s="136"/>
-      <c r="O22" s="136"/>
-      <c r="P22" s="136"/>
-      <c r="Q22" s="136"/>
-      <c r="R22" s="136"/>
-      <c r="S22" s="136"/>
-      <c r="T22" s="136"/>
-      <c r="U22" s="136"/>
-      <c r="V22" s="136"/>
-      <c r="W22" s="136"/>
-      <c r="X22" s="137"/>
+      <c r="L22" s="124"/>
+      <c r="M22" s="124"/>
+      <c r="N22" s="124"/>
+      <c r="O22" s="124"/>
+      <c r="P22" s="124"/>
+      <c r="Q22" s="124"/>
+      <c r="R22" s="124"/>
+      <c r="S22" s="124"/>
+      <c r="T22" s="124"/>
+      <c r="U22" s="124"/>
+      <c r="V22" s="124"/>
+      <c r="W22" s="124"/>
+      <c r="X22" s="125"/>
     </row>
     <row r="23" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K23" s="138"/>
-      <c r="L23" s="139"/>
-      <c r="M23" s="139"/>
-      <c r="N23" s="139"/>
-      <c r="O23" s="139"/>
-      <c r="P23" s="139"/>
-      <c r="Q23" s="139"/>
-      <c r="R23" s="139"/>
-      <c r="S23" s="139"/>
-      <c r="T23" s="139"/>
-      <c r="U23" s="139"/>
-      <c r="V23" s="139"/>
-      <c r="W23" s="139"/>
-      <c r="X23" s="140"/>
+      <c r="K23" s="126"/>
+      <c r="L23" s="127"/>
+      <c r="M23" s="127"/>
+      <c r="N23" s="127"/>
+      <c r="O23" s="127"/>
+      <c r="P23" s="127"/>
+      <c r="Q23" s="127"/>
+      <c r="R23" s="127"/>
+      <c r="S23" s="127"/>
+      <c r="T23" s="127"/>
+      <c r="U23" s="127"/>
+      <c r="V23" s="127"/>
+      <c r="W23" s="127"/>
+      <c r="X23" s="128"/>
     </row>
     <row r="26" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K26" s="135" t="s">
+      <c r="K26" s="123" t="s">
         <v>7</v>
       </c>
-      <c r="L26" s="136"/>
-      <c r="M26" s="136"/>
-      <c r="N26" s="136"/>
-      <c r="O26" s="136"/>
-      <c r="P26" s="136"/>
-      <c r="Q26" s="136"/>
-      <c r="R26" s="136"/>
-      <c r="S26" s="136"/>
-      <c r="T26" s="136"/>
-      <c r="U26" s="136"/>
-      <c r="V26" s="136"/>
-      <c r="W26" s="136"/>
-      <c r="X26" s="137"/>
+      <c r="L26" s="124"/>
+      <c r="M26" s="124"/>
+      <c r="N26" s="124"/>
+      <c r="O26" s="124"/>
+      <c r="P26" s="124"/>
+      <c r="Q26" s="124"/>
+      <c r="R26" s="124"/>
+      <c r="S26" s="124"/>
+      <c r="T26" s="124"/>
+      <c r="U26" s="124"/>
+      <c r="V26" s="124"/>
+      <c r="W26" s="124"/>
+      <c r="X26" s="125"/>
     </row>
     <row r="27" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K27" s="138"/>
-      <c r="L27" s="139"/>
-      <c r="M27" s="139"/>
-      <c r="N27" s="139"/>
-      <c r="O27" s="139"/>
-      <c r="P27" s="139"/>
-      <c r="Q27" s="139"/>
-      <c r="R27" s="139"/>
-      <c r="S27" s="139"/>
-      <c r="T27" s="139"/>
-      <c r="U27" s="139"/>
-      <c r="V27" s="139"/>
-      <c r="W27" s="139"/>
-      <c r="X27" s="140"/>
+      <c r="K27" s="126"/>
+      <c r="L27" s="127"/>
+      <c r="M27" s="127"/>
+      <c r="N27" s="127"/>
+      <c r="O27" s="127"/>
+      <c r="P27" s="127"/>
+      <c r="Q27" s="127"/>
+      <c r="R27" s="127"/>
+      <c r="S27" s="127"/>
+      <c r="T27" s="127"/>
+      <c r="U27" s="127"/>
+      <c r="V27" s="127"/>
+      <c r="W27" s="127"/>
+      <c r="X27" s="128"/>
     </row>
     <row r="30" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K30" s="135" t="s">
+      <c r="K30" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="L30" s="136"/>
-      <c r="M30" s="136"/>
-      <c r="N30" s="136"/>
-      <c r="O30" s="136"/>
-      <c r="P30" s="136"/>
-      <c r="Q30" s="136"/>
-      <c r="R30" s="136"/>
-      <c r="S30" s="136"/>
-      <c r="T30" s="136"/>
-      <c r="U30" s="136"/>
-      <c r="V30" s="136"/>
-      <c r="W30" s="136"/>
-      <c r="X30" s="137"/>
+      <c r="L30" s="124"/>
+      <c r="M30" s="124"/>
+      <c r="N30" s="124"/>
+      <c r="O30" s="124"/>
+      <c r="P30" s="124"/>
+      <c r="Q30" s="124"/>
+      <c r="R30" s="124"/>
+      <c r="S30" s="124"/>
+      <c r="T30" s="124"/>
+      <c r="U30" s="124"/>
+      <c r="V30" s="124"/>
+      <c r="W30" s="124"/>
+      <c r="X30" s="125"/>
     </row>
     <row r="31" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K31" s="138"/>
-      <c r="L31" s="139"/>
-      <c r="M31" s="139"/>
-      <c r="N31" s="139"/>
-      <c r="O31" s="139"/>
-      <c r="P31" s="139"/>
-      <c r="Q31" s="139"/>
-      <c r="R31" s="139"/>
-      <c r="S31" s="139"/>
-      <c r="T31" s="139"/>
-      <c r="U31" s="139"/>
-      <c r="V31" s="139"/>
-      <c r="W31" s="139"/>
-      <c r="X31" s="140"/>
+      <c r="K31" s="126"/>
+      <c r="L31" s="127"/>
+      <c r="M31" s="127"/>
+      <c r="N31" s="127"/>
+      <c r="O31" s="127"/>
+      <c r="P31" s="127"/>
+      <c r="Q31" s="127"/>
+      <c r="R31" s="127"/>
+      <c r="S31" s="127"/>
+      <c r="T31" s="127"/>
+      <c r="U31" s="127"/>
+      <c r="V31" s="127"/>
+      <c r="W31" s="127"/>
+      <c r="X31" s="128"/>
     </row>
     <row r="38" spans="11:11" x14ac:dyDescent="0.4">
       <c r="K38" t="s">
@@ -12472,7 +12443,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -12537,11 +12508,11 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="138" t="s">
         <v>188</v>
       </c>
-      <c r="B2" s="151"/>
-      <c r="C2" s="152"/>
+      <c r="B2" s="139"/>
+      <c r="C2" s="140"/>
       <c r="E2"/>
       <c r="H2"/>
       <c r="I2"/>
@@ -12663,11 +12634,11 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="147" t="s">
+      <c r="A7" s="135" t="s">
         <v>190</v>
       </c>
-      <c r="B7" s="148"/>
-      <c r="C7" s="149"/>
+      <c r="B7" s="136"/>
+      <c r="C7" s="137"/>
       <c r="E7"/>
       <c r="H7"/>
       <c r="I7"/>
@@ -13408,11 +13379,11 @@
       <c r="I34"/>
     </row>
     <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="147" t="s">
+      <c r="A35" s="135" t="s">
         <v>195</v>
       </c>
-      <c r="B35" s="148"/>
-      <c r="C35" s="149"/>
+      <c r="B35" s="136"/>
+      <c r="C35" s="137"/>
       <c r="E35"/>
       <c r="H35"/>
       <c r="I35"/>
@@ -13501,11 +13472,11 @@
       </c>
     </row>
     <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="147" t="s">
+      <c r="A39" s="135" t="s">
         <v>198</v>
       </c>
-      <c r="B39" s="148"/>
-      <c r="C39" s="149"/>
+      <c r="B39" s="136"/>
+      <c r="C39" s="137"/>
       <c r="E39"/>
       <c r="H39"/>
       <c r="I39"/>
@@ -13558,11 +13529,11 @@
       <c r="I41"/>
     </row>
     <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="147" t="s">
+      <c r="A42" s="135" t="s">
         <v>189</v>
       </c>
-      <c r="B42" s="148"/>
-      <c r="C42" s="149"/>
+      <c r="B42" s="136"/>
+      <c r="C42" s="137"/>
       <c r="E42"/>
       <c r="H42"/>
       <c r="I42"/>
@@ -13727,11 +13698,11 @@
       <c r="I48"/>
     </row>
     <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="147" t="s">
+      <c r="A49" s="135" t="s">
         <v>196</v>
       </c>
-      <c r="B49" s="148"/>
-      <c r="C49" s="149"/>
+      <c r="B49" s="136"/>
+      <c r="C49" s="137"/>
       <c r="E49"/>
       <c r="H49"/>
       <c r="I49"/>
@@ -13852,11 +13823,11 @@
       </c>
     </row>
     <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="147" t="s">
+      <c r="A54" s="135" t="s">
         <v>197</v>
       </c>
-      <c r="B54" s="148"/>
-      <c r="C54" s="149"/>
+      <c r="B54" s="136"/>
+      <c r="C54" s="137"/>
       <c r="E54"/>
       <c r="H54" s="19"/>
       <c r="I54"/>
@@ -14509,7 +14480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6511554B-3B83-477E-8F82-CB1DA06B1302}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -14659,10 +14630,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA67DCE-BBF2-410C-9E82-B8F1A39A9A5C}">
-  <dimension ref="A1:U189"/>
+  <dimension ref="A1:U192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K171" sqref="K171"/>
+    <sheetView tabSelected="1" topLeftCell="E16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26:U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -14722,13 +14693,13 @@
     <row r="3" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="94"/>
       <c r="B3" s="95" t="s">
-        <v>467</v>
+        <v>452</v>
       </c>
       <c r="C3" s="96"/>
       <c r="D3" s="96"/>
-      <c r="E3" s="114"/>
+      <c r="E3" s="112"/>
       <c r="F3" s="95" t="s">
-        <v>487</v>
+        <v>472</v>
       </c>
       <c r="G3" s="96"/>
       <c r="H3" s="96"/>
@@ -14748,14 +14719,14 @@
     </row>
     <row r="4" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="94"/>
-      <c r="B4" s="115" t="s">
-        <v>469</v>
+      <c r="B4" s="113" t="s">
+        <v>454</v>
       </c>
       <c r="C4" s="107"/>
       <c r="D4" s="107"/>
       <c r="E4" s="101"/>
-      <c r="F4" s="115" t="s">
-        <v>469</v>
+      <c r="F4" s="113" t="s">
+        <v>454</v>
       </c>
       <c r="G4" s="107"/>
       <c r="H4" s="107"/>
@@ -14775,14 +14746,14 @@
     </row>
     <row r="5" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="94"/>
-      <c r="B5" s="115" t="s">
-        <v>488</v>
+      <c r="B5" s="113" t="s">
+        <v>473</v>
       </c>
       <c r="C5" s="107"/>
       <c r="D5" s="107"/>
       <c r="E5" s="101"/>
-      <c r="F5" s="115" t="s">
-        <v>488</v>
+      <c r="F5" s="113" t="s">
+        <v>473</v>
       </c>
       <c r="G5" s="107"/>
       <c r="H5" s="107"/>
@@ -14802,14 +14773,14 @@
     </row>
     <row r="6" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="94"/>
-      <c r="B6" s="115" t="s">
-        <v>489</v>
+      <c r="B6" s="113" t="s">
+        <v>474</v>
       </c>
       <c r="C6" s="107"/>
       <c r="D6" s="107"/>
       <c r="E6" s="101"/>
-      <c r="F6" s="115" t="s">
-        <v>489</v>
+      <c r="F6" s="113" t="s">
+        <v>474</v>
       </c>
       <c r="G6" s="107"/>
       <c r="H6" s="107"/>
@@ -14829,14 +14800,14 @@
     </row>
     <row r="7" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="94"/>
-      <c r="B7" s="115" t="s">
-        <v>490</v>
+      <c r="B7" s="113" t="s">
+        <v>475</v>
       </c>
       <c r="C7" s="107"/>
       <c r="D7" s="107"/>
       <c r="E7" s="101"/>
-      <c r="F7" s="115" t="s">
-        <v>490</v>
+      <c r="F7" s="113" t="s">
+        <v>475</v>
       </c>
       <c r="G7" s="107"/>
       <c r="H7" s="107"/>
@@ -14856,14 +14827,14 @@
     </row>
     <row r="8" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="94"/>
-      <c r="B8" s="115" t="s">
-        <v>491</v>
+      <c r="B8" s="113" t="s">
+        <v>476</v>
       </c>
       <c r="C8" s="107"/>
       <c r="D8" s="107"/>
       <c r="E8" s="101"/>
-      <c r="F8" s="115" t="s">
-        <v>499</v>
+      <c r="F8" s="113" t="s">
+        <v>484</v>
       </c>
       <c r="G8" s="107"/>
       <c r="H8" s="107"/>
@@ -14883,14 +14854,14 @@
     </row>
     <row r="9" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="94"/>
-      <c r="B9" s="115" t="s">
-        <v>492</v>
+      <c r="B9" s="113" t="s">
+        <v>477</v>
       </c>
       <c r="C9" s="107"/>
       <c r="D9" s="107"/>
       <c r="E9" s="101"/>
-      <c r="F9" s="115" t="s">
-        <v>500</v>
+      <c r="F9" s="113" t="s">
+        <v>485</v>
       </c>
       <c r="G9" s="107"/>
       <c r="H9" s="107"/>
@@ -14910,14 +14881,14 @@
     </row>
     <row r="10" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A10" s="94"/>
-      <c r="B10" s="115" t="s">
-        <v>493</v>
+      <c r="B10" s="113" t="s">
+        <v>478</v>
       </c>
       <c r="C10" s="107"/>
       <c r="D10" s="107"/>
       <c r="E10" s="101"/>
-      <c r="F10" s="115" t="s">
-        <v>501</v>
+      <c r="F10" s="113" t="s">
+        <v>486</v>
       </c>
       <c r="G10" s="107"/>
       <c r="H10" s="107"/>
@@ -14937,14 +14908,14 @@
     </row>
     <row r="11" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A11" s="94"/>
-      <c r="B11" s="115" t="s">
-        <v>494</v>
+      <c r="B11" s="113" t="s">
+        <v>479</v>
       </c>
       <c r="C11" s="107"/>
       <c r="D11" s="107"/>
       <c r="E11" s="101"/>
-      <c r="F11" s="115" t="s">
-        <v>502</v>
+      <c r="F11" s="113" t="s">
+        <v>487</v>
       </c>
       <c r="G11" s="107"/>
       <c r="H11" s="107"/>
@@ -14964,14 +14935,14 @@
     </row>
     <row r="12" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A12" s="94"/>
-      <c r="B12" s="115" t="s">
-        <v>484</v>
+      <c r="B12" s="113" t="s">
+        <v>469</v>
       </c>
       <c r="C12" s="107"/>
       <c r="D12" s="107"/>
       <c r="E12" s="101"/>
-      <c r="F12" s="115" t="s">
-        <v>503</v>
+      <c r="F12" s="113" t="s">
+        <v>488</v>
       </c>
       <c r="G12" s="107"/>
       <c r="H12" s="107"/>
@@ -14991,14 +14962,14 @@
     </row>
     <row r="13" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="94"/>
-      <c r="B13" s="115" t="s">
-        <v>495</v>
+      <c r="B13" s="113" t="s">
+        <v>480</v>
       </c>
       <c r="C13" s="107"/>
       <c r="D13" s="107"/>
       <c r="E13" s="101"/>
-      <c r="F13" s="115" t="s">
-        <v>497</v>
+      <c r="F13" s="113" t="s">
+        <v>482</v>
       </c>
       <c r="G13" s="107"/>
       <c r="H13" s="107"/>
@@ -15018,14 +14989,14 @@
     </row>
     <row r="14" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="94"/>
-      <c r="B14" s="115" t="s">
-        <v>496</v>
+      <c r="B14" s="113" t="s">
+        <v>481</v>
       </c>
       <c r="C14" s="107"/>
       <c r="D14" s="107"/>
       <c r="E14" s="101"/>
-      <c r="F14" s="115" t="s">
-        <v>504</v>
+      <c r="F14" s="113" t="s">
+        <v>489</v>
       </c>
       <c r="G14" s="107"/>
       <c r="H14" s="107"/>
@@ -15045,14 +15016,14 @@
     </row>
     <row r="15" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A15" s="94"/>
-      <c r="B15" s="115" t="s">
-        <v>497</v>
+      <c r="B15" s="113" t="s">
+        <v>482</v>
       </c>
       <c r="C15" s="107"/>
       <c r="D15" s="107"/>
       <c r="E15" s="101"/>
-      <c r="F15" s="115" t="s">
-        <v>505</v>
+      <c r="F15" s="113" t="s">
+        <v>490</v>
       </c>
       <c r="G15" s="107"/>
       <c r="H15" s="107"/>
@@ -15072,14 +15043,14 @@
     </row>
     <row r="16" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A16" s="94"/>
-      <c r="B16" s="115" t="s">
-        <v>498</v>
+      <c r="B16" s="113" t="s">
+        <v>483</v>
       </c>
       <c r="C16" s="107"/>
       <c r="D16" s="107"/>
       <c r="E16" s="101"/>
-      <c r="F16" s="115" t="s">
-        <v>506</v>
+      <c r="F16" s="113" t="s">
+        <v>491</v>
       </c>
       <c r="G16" s="107"/>
       <c r="H16" s="107"/>
@@ -15099,14 +15070,14 @@
     </row>
     <row r="17" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A17" s="94"/>
-      <c r="B17" s="115" t="s">
-        <v>468</v>
+      <c r="B17" s="113" t="s">
+        <v>453</v>
       </c>
       <c r="C17" s="107"/>
       <c r="D17" s="107"/>
       <c r="E17" s="101"/>
-      <c r="F17" s="115" t="s">
-        <v>497</v>
+      <c r="F17" s="113" t="s">
+        <v>482</v>
       </c>
       <c r="G17" s="107"/>
       <c r="H17" s="107"/>
@@ -15130,8 +15101,8 @@
       <c r="C18" s="107"/>
       <c r="D18" s="107"/>
       <c r="E18" s="101"/>
-      <c r="F18" s="115" t="s">
-        <v>498</v>
+      <c r="F18" s="113" t="s">
+        <v>483</v>
       </c>
       <c r="G18" s="107"/>
       <c r="H18" s="107"/>
@@ -15155,8 +15126,8 @@
       <c r="C19" s="110"/>
       <c r="D19" s="110"/>
       <c r="E19" s="105"/>
-      <c r="F19" s="116" t="s">
-        <v>468</v>
+      <c r="F19" s="114" t="s">
+        <v>453</v>
       </c>
       <c r="G19" s="110"/>
       <c r="H19" s="110"/>
@@ -15245,329 +15216,297 @@
       <c r="T22" s="94"/>
       <c r="U22" s="94"/>
     </row>
-    <row r="23" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:21" s="93" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="94"/>
-      <c r="B23" s="121">
+      <c r="B23" s="141">
         <v>1</v>
       </c>
-      <c r="C23" s="121" t="s">
+      <c r="C23" s="144" t="s">
+        <v>445</v>
+      </c>
+      <c r="D23" s="145"/>
+      <c r="E23" s="145"/>
+      <c r="F23" s="145"/>
+      <c r="G23" s="145"/>
+      <c r="H23" s="146"/>
+      <c r="I23" s="144" t="s">
+        <v>446</v>
+      </c>
+      <c r="J23" s="146"/>
+      <c r="K23" s="147" t="s">
+        <v>447</v>
+      </c>
+      <c r="L23" s="144" t="s">
+        <v>568</v>
+      </c>
+      <c r="M23" s="145"/>
+      <c r="N23" s="145"/>
+      <c r="O23" s="145"/>
+      <c r="P23" s="145"/>
+      <c r="Q23" s="145"/>
+      <c r="R23" s="145"/>
+      <c r="S23" s="145"/>
+      <c r="T23" s="145"/>
+      <c r="U23" s="146"/>
+    </row>
+    <row r="24" spans="1:21" s="93" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="94"/>
+      <c r="B24" s="141">
+        <v>2</v>
+      </c>
+      <c r="C24" s="144" t="s">
+        <v>443</v>
+      </c>
+      <c r="D24" s="145"/>
+      <c r="E24" s="145"/>
+      <c r="F24" s="145"/>
+      <c r="G24" s="145"/>
+      <c r="H24" s="146"/>
+      <c r="I24" s="144" t="s">
+        <v>451</v>
+      </c>
+      <c r="J24" s="146"/>
+      <c r="K24" s="147" t="s">
+        <v>447</v>
+      </c>
+      <c r="L24" s="144" t="s">
+        <v>567</v>
+      </c>
+      <c r="M24" s="145"/>
+      <c r="N24" s="145"/>
+      <c r="O24" s="145"/>
+      <c r="P24" s="145"/>
+      <c r="Q24" s="145"/>
+      <c r="R24" s="145"/>
+      <c r="S24" s="145"/>
+      <c r="T24" s="145"/>
+      <c r="U24" s="146"/>
+    </row>
+    <row r="25" spans="1:21" s="93" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="94"/>
+      <c r="B25" s="141">
+        <v>3</v>
+      </c>
+      <c r="C25" s="144" t="s">
+        <v>444</v>
+      </c>
+      <c r="D25" s="145"/>
+      <c r="E25" s="145"/>
+      <c r="F25" s="145"/>
+      <c r="G25" s="145"/>
+      <c r="H25" s="146"/>
+      <c r="I25" s="144" t="s">
+        <v>448</v>
+      </c>
+      <c r="J25" s="146"/>
+      <c r="K25" s="148" t="s">
+        <v>447</v>
+      </c>
+      <c r="L25" s="149" t="s">
+        <v>567</v>
+      </c>
+      <c r="M25" s="150"/>
+      <c r="N25" s="150"/>
+      <c r="O25" s="150"/>
+      <c r="P25" s="150"/>
+      <c r="Q25" s="150"/>
+      <c r="R25" s="150"/>
+      <c r="S25" s="150"/>
+      <c r="T25" s="150"/>
+      <c r="U25" s="151"/>
+    </row>
+    <row r="26" spans="1:21" s="93" customFormat="1" ht="132" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="94"/>
+      <c r="B26" s="142">
+        <v>4</v>
+      </c>
+      <c r="C26" s="152" t="s">
+        <v>575</v>
+      </c>
+      <c r="D26" s="153"/>
+      <c r="E26" s="153"/>
+      <c r="F26" s="153"/>
+      <c r="G26" s="153"/>
+      <c r="H26" s="154"/>
+      <c r="I26" s="152" t="s">
+        <v>450</v>
+      </c>
+      <c r="J26" s="154"/>
+      <c r="K26" s="155" t="s">
+        <v>447</v>
+      </c>
+      <c r="L26" s="143" t="s">
+        <v>577</v>
+      </c>
+      <c r="M26" s="143"/>
+      <c r="N26" s="143"/>
+      <c r="O26" s="143"/>
+      <c r="P26" s="143"/>
+      <c r="Q26" s="143"/>
+      <c r="R26" s="143"/>
+      <c r="S26" s="143"/>
+      <c r="T26" s="143"/>
+      <c r="U26" s="143"/>
+    </row>
+    <row r="27" spans="1:21" s="93" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="94"/>
+      <c r="B27" s="142">
+        <v>5</v>
+      </c>
+      <c r="C27" s="152" t="s">
+        <v>576</v>
+      </c>
+      <c r="D27" s="153"/>
+      <c r="E27" s="153"/>
+      <c r="F27" s="153"/>
+      <c r="G27" s="153"/>
+      <c r="H27" s="154"/>
+      <c r="I27" s="152"/>
+      <c r="J27" s="154"/>
+      <c r="K27" s="155" t="s">
         <v>449</v>
       </c>
-      <c r="D23" s="122"/>
-      <c r="E23" s="122"/>
-      <c r="F23" s="122"/>
-      <c r="G23" s="122"/>
-      <c r="H23" s="123"/>
-      <c r="I23" s="121" t="s">
-        <v>450</v>
-      </c>
-      <c r="J23" s="123"/>
-      <c r="K23" s="124" t="s">
-        <v>451</v>
-      </c>
-      <c r="L23" s="122" t="s">
-        <v>583</v>
-      </c>
-      <c r="M23" s="122"/>
-      <c r="N23" s="122"/>
-      <c r="O23" s="122"/>
-      <c r="P23" s="122"/>
-      <c r="Q23" s="122"/>
-      <c r="R23" s="122"/>
-      <c r="S23" s="122"/>
-      <c r="T23" s="122"/>
-      <c r="U23" s="123"/>
-    </row>
-    <row r="24" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="94"/>
-      <c r="B24" s="125">
-        <v>2</v>
-      </c>
-      <c r="C24" s="125" t="s">
-        <v>443</v>
-      </c>
-      <c r="D24" s="126"/>
-      <c r="E24" s="126"/>
-      <c r="F24" s="126"/>
-      <c r="G24" s="126"/>
-      <c r="H24" s="127"/>
-      <c r="I24" s="125" t="s">
-        <v>466</v>
-      </c>
-      <c r="J24" s="127"/>
-      <c r="K24" s="128" t="s">
-        <v>451</v>
-      </c>
-      <c r="L24" s="126" t="s">
-        <v>582</v>
-      </c>
-      <c r="M24" s="126"/>
-      <c r="N24" s="126"/>
-      <c r="O24" s="126"/>
-      <c r="P24" s="126"/>
-      <c r="Q24" s="126"/>
-      <c r="R24" s="126"/>
-      <c r="S24" s="126"/>
-      <c r="T24" s="126"/>
-      <c r="U24" s="127"/>
-    </row>
-    <row r="25" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="94"/>
-      <c r="B25" s="125">
-        <v>3</v>
-      </c>
-      <c r="C25" s="125" t="s">
-        <v>445</v>
-      </c>
-      <c r="D25" s="132"/>
-      <c r="E25" s="132"/>
-      <c r="F25" s="132"/>
-      <c r="G25" s="132"/>
-      <c r="H25" s="133"/>
-      <c r="I25" s="125" t="s">
-        <v>453</v>
-      </c>
-      <c r="J25" s="133"/>
-      <c r="K25" s="134" t="s">
-        <v>451</v>
-      </c>
-      <c r="L25" s="132" t="s">
-        <v>582</v>
-      </c>
-      <c r="M25" s="132"/>
-      <c r="N25" s="132"/>
-      <c r="O25" s="132"/>
-      <c r="P25" s="132"/>
-      <c r="Q25" s="132"/>
-      <c r="R25" s="132"/>
-      <c r="S25" s="132"/>
-      <c r="T25" s="132"/>
-      <c r="U25" s="133"/>
-    </row>
-    <row r="26" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="94"/>
-      <c r="B26" s="106">
-        <v>4</v>
-      </c>
-      <c r="C26" s="106" t="s">
-        <v>446</v>
-      </c>
-      <c r="D26" s="107"/>
-      <c r="E26" s="107"/>
-      <c r="F26" s="107"/>
-      <c r="G26" s="107"/>
-      <c r="H26" s="108"/>
-      <c r="I26" s="106"/>
-      <c r="J26" s="108"/>
-      <c r="K26" s="112" t="s">
-        <v>455</v>
-      </c>
-      <c r="L26" s="107" t="s">
-        <v>583</v>
-      </c>
-      <c r="M26" s="107"/>
-      <c r="N26" s="107"/>
-      <c r="O26" s="107"/>
-      <c r="P26" s="107"/>
-      <c r="Q26" s="107"/>
-      <c r="R26" s="107"/>
-      <c r="S26" s="107"/>
-      <c r="T26" s="107"/>
-      <c r="U26" s="108"/>
-    </row>
-    <row r="27" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="94"/>
-      <c r="B27" s="106">
-        <v>5</v>
-      </c>
-      <c r="C27" s="106" t="s">
-        <v>447</v>
-      </c>
-      <c r="D27" s="107"/>
-      <c r="E27" s="107"/>
-      <c r="F27" s="107"/>
-      <c r="G27" s="107"/>
-      <c r="H27" s="108"/>
-      <c r="I27" s="106" t="s">
-        <v>462</v>
-      </c>
-      <c r="J27" s="108"/>
-      <c r="K27" s="112" t="s">
-        <v>451</v>
-      </c>
-      <c r="L27" s="107" t="s">
-        <v>583</v>
-      </c>
-      <c r="M27" s="107"/>
-      <c r="N27" s="107"/>
-      <c r="O27" s="107"/>
-      <c r="P27" s="107"/>
-      <c r="Q27" s="107"/>
-      <c r="R27" s="107"/>
-      <c r="S27" s="107"/>
-      <c r="T27" s="107"/>
-      <c r="U27" s="108"/>
+      <c r="L27" s="152" t="s">
+        <v>568</v>
+      </c>
+      <c r="M27" s="153"/>
+      <c r="N27" s="153"/>
+      <c r="O27" s="153"/>
+      <c r="P27" s="153"/>
+      <c r="Q27" s="153"/>
+      <c r="R27" s="153"/>
+      <c r="S27" s="153"/>
+      <c r="T27" s="153"/>
+      <c r="U27" s="154"/>
     </row>
     <row r="28" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A28" s="94"/>
-      <c r="B28" s="106">
-        <v>6</v>
-      </c>
-      <c r="C28" s="106" t="s">
-        <v>448</v>
-      </c>
-      <c r="D28" s="107"/>
-      <c r="E28" s="107"/>
-      <c r="F28" s="107"/>
-      <c r="G28" s="107"/>
-      <c r="H28" s="108"/>
-      <c r="I28" s="106" t="s">
-        <v>463</v>
-      </c>
-      <c r="J28" s="108"/>
-      <c r="K28" s="112" t="s">
-        <v>451</v>
-      </c>
-      <c r="L28" s="107" t="s">
-        <v>583</v>
-      </c>
-      <c r="M28" s="107"/>
-      <c r="N28" s="107"/>
-      <c r="O28" s="107"/>
-      <c r="P28" s="107"/>
-      <c r="Q28" s="107"/>
-      <c r="R28" s="107"/>
-      <c r="S28" s="107"/>
-      <c r="T28" s="107"/>
-      <c r="U28" s="108"/>
+      <c r="B28" s="94"/>
+      <c r="C28" s="94" t="s">
+        <v>578</v>
+      </c>
+      <c r="D28" s="94"/>
+      <c r="E28" s="94"/>
+      <c r="F28" s="94"/>
+      <c r="G28" s="94"/>
+      <c r="H28" s="94"/>
+      <c r="I28" s="94"/>
+      <c r="J28" s="94"/>
+      <c r="K28" s="94"/>
+      <c r="L28" s="94"/>
+      <c r="M28" s="94"/>
+      <c r="N28" s="94"/>
+      <c r="O28" s="94"/>
+      <c r="P28" s="94"/>
+      <c r="Q28" s="94"/>
+      <c r="R28" s="94"/>
+      <c r="S28" s="94"/>
+      <c r="T28" s="94"/>
+      <c r="U28" s="94"/>
     </row>
     <row r="29" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A29" s="94"/>
-      <c r="B29" s="106">
-        <v>7</v>
-      </c>
-      <c r="C29" s="106" t="s">
-        <v>454</v>
-      </c>
-      <c r="D29" s="107"/>
-      <c r="E29" s="107"/>
-      <c r="F29" s="107"/>
-      <c r="G29" s="107"/>
-      <c r="H29" s="108"/>
-      <c r="I29" s="106" t="s">
-        <v>457</v>
-      </c>
-      <c r="J29" s="108"/>
-      <c r="K29" s="112" t="s">
-        <v>455</v>
-      </c>
-      <c r="L29" s="107" t="s">
-        <v>460</v>
-      </c>
-      <c r="M29" s="107"/>
-      <c r="N29" s="107"/>
-      <c r="O29" s="107"/>
-      <c r="P29" s="107"/>
-      <c r="Q29" s="107"/>
-      <c r="R29" s="107"/>
-      <c r="S29" s="107"/>
-      <c r="T29" s="107"/>
-      <c r="U29" s="108"/>
+      <c r="B29" s="94"/>
+      <c r="C29" s="94" t="s">
+        <v>579</v>
+      </c>
+      <c r="D29" s="94"/>
+      <c r="E29" s="94"/>
+      <c r="F29" s="94"/>
+      <c r="G29" s="94"/>
+      <c r="H29" s="94"/>
+      <c r="I29" s="94"/>
+      <c r="J29" s="94"/>
+      <c r="K29" s="94"/>
+      <c r="L29" s="94"/>
+      <c r="M29" s="94"/>
+      <c r="N29" s="94"/>
+      <c r="O29" s="94"/>
+      <c r="P29" s="94"/>
+      <c r="Q29" s="94"/>
+      <c r="R29" s="94"/>
+      <c r="S29" s="94"/>
+      <c r="T29" s="94"/>
+      <c r="U29" s="94"/>
     </row>
     <row r="30" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="94"/>
-      <c r="B30" s="106">
-        <v>8</v>
-      </c>
-      <c r="C30" s="106" t="s">
-        <v>456</v>
-      </c>
-      <c r="D30" s="107"/>
-      <c r="E30" s="107"/>
-      <c r="F30" s="107"/>
-      <c r="G30" s="107"/>
-      <c r="H30" s="108"/>
-      <c r="I30" s="106" t="s">
-        <v>458</v>
-      </c>
-      <c r="J30" s="108"/>
-      <c r="K30" s="112" t="s">
-        <v>455</v>
-      </c>
-      <c r="L30" s="107" t="s">
-        <v>461</v>
-      </c>
-      <c r="M30" s="107"/>
-      <c r="N30" s="107"/>
-      <c r="O30" s="107"/>
-      <c r="P30" s="107"/>
-      <c r="Q30" s="107"/>
-      <c r="R30" s="107"/>
-      <c r="S30" s="107"/>
-      <c r="T30" s="107"/>
-      <c r="U30" s="108"/>
+      <c r="B30" s="94"/>
+      <c r="C30" s="94" t="s">
+        <v>580</v>
+      </c>
+      <c r="D30" s="94" t="s">
+        <v>583</v>
+      </c>
+      <c r="E30" s="94"/>
+      <c r="F30" s="94"/>
+      <c r="G30" s="94"/>
+      <c r="H30" s="94"/>
+      <c r="I30" s="94"/>
+      <c r="J30" s="94"/>
+      <c r="K30" s="94"/>
+      <c r="L30" s="94"/>
+      <c r="M30" s="94"/>
+      <c r="N30" s="94"/>
+      <c r="O30" s="94"/>
+      <c r="P30" s="94"/>
+      <c r="Q30" s="94"/>
+      <c r="R30" s="94"/>
+      <c r="S30" s="94"/>
+      <c r="T30" s="94"/>
+      <c r="U30" s="94"/>
     </row>
     <row r="31" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="94"/>
-      <c r="B31" s="106">
-        <v>9</v>
-      </c>
-      <c r="C31" s="106" t="s">
-        <v>459</v>
-      </c>
-      <c r="D31" s="107"/>
-      <c r="E31" s="107"/>
-      <c r="F31" s="107"/>
-      <c r="G31" s="107"/>
-      <c r="H31" s="108"/>
-      <c r="I31" s="106" t="s">
-        <v>465</v>
-      </c>
-      <c r="J31" s="108"/>
-      <c r="K31" s="112" t="s">
-        <v>455</v>
-      </c>
-      <c r="L31" s="107" t="s">
-        <v>464</v>
-      </c>
-      <c r="M31" s="107"/>
-      <c r="N31" s="107"/>
-      <c r="O31" s="107"/>
-      <c r="P31" s="107"/>
-      <c r="Q31" s="107"/>
-      <c r="R31" s="107"/>
-      <c r="S31" s="107"/>
-      <c r="T31" s="107"/>
-      <c r="U31" s="108"/>
-    </row>
-    <row r="32" spans="1:21" s="93" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="94"/>
+      <c r="C31" s="94" t="s">
+        <v>581</v>
+      </c>
+      <c r="D31" s="94" t="s">
+        <v>584</v>
+      </c>
+      <c r="E31" s="94"/>
+      <c r="F31" s="94"/>
+      <c r="G31" s="94"/>
+      <c r="H31" s="94"/>
+      <c r="I31" s="94"/>
+      <c r="J31" s="94"/>
+      <c r="K31" s="94"/>
+      <c r="L31" s="94"/>
+      <c r="M31" s="94"/>
+      <c r="N31" s="94"/>
+      <c r="O31" s="94"/>
+      <c r="P31" s="94"/>
+      <c r="Q31" s="94"/>
+      <c r="R31" s="94"/>
+      <c r="S31" s="94"/>
+      <c r="T31" s="94"/>
+      <c r="U31" s="94"/>
+    </row>
+    <row r="32" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A32" s="94"/>
-      <c r="B32" s="109"/>
-      <c r="C32" s="109" t="s">
-        <v>444</v>
-      </c>
-      <c r="D32" s="110"/>
-      <c r="E32" s="110"/>
-      <c r="F32" s="110"/>
-      <c r="G32" s="110"/>
-      <c r="H32" s="111"/>
-      <c r="I32" s="109" t="s">
-        <v>452</v>
-      </c>
-      <c r="J32" s="111"/>
-      <c r="K32" s="113" t="s">
-        <v>451</v>
-      </c>
-      <c r="L32" s="110"/>
-      <c r="M32" s="110"/>
-      <c r="N32" s="110"/>
-      <c r="O32" s="110"/>
-      <c r="P32" s="110"/>
-      <c r="Q32" s="110"/>
-      <c r="R32" s="110"/>
-      <c r="S32" s="110"/>
-      <c r="T32" s="110"/>
-      <c r="U32" s="111"/>
+      <c r="B32" s="94"/>
+      <c r="C32" s="94" t="s">
+        <v>582</v>
+      </c>
+      <c r="D32" s="94"/>
+      <c r="E32" s="94"/>
+      <c r="F32" s="94"/>
+      <c r="G32" s="94"/>
+      <c r="H32" s="94"/>
+      <c r="I32" s="94"/>
+      <c r="J32" s="94"/>
+      <c r="K32" s="94"/>
+      <c r="L32" s="94"/>
+      <c r="M32" s="94"/>
+      <c r="N32" s="94"/>
+      <c r="O32" s="94"/>
+      <c r="P32" s="94"/>
+      <c r="Q32" s="94"/>
+      <c r="R32" s="94"/>
+      <c r="S32" s="94"/>
+      <c r="T32" s="94"/>
+      <c r="U32" s="94"/>
     </row>
     <row r="33" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A33" s="94"/>
@@ -15615,7 +15554,7 @@
       <c r="T34" s="94"/>
       <c r="U34" s="94"/>
     </row>
-    <row r="35" spans="1:21" s="93" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A35" s="94"/>
       <c r="B35" s="94"/>
       <c r="C35" s="94"/>
@@ -15638,14 +15577,10 @@
       <c r="T35" s="94"/>
       <c r="U35" s="94"/>
     </row>
-    <row r="36" spans="1:21" s="93" customFormat="1" ht="33.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="94"/>
-      <c r="B36" s="117">
-        <v>1</v>
-      </c>
-      <c r="C36" s="119" t="s">
-        <v>520</v>
-      </c>
+      <c r="B36" s="94"/>
+      <c r="C36" s="94"/>
       <c r="D36" s="94"/>
       <c r="E36" s="94"/>
       <c r="F36" s="94"/>
@@ -15667,22 +15602,18 @@
     </row>
     <row r="37" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A37" s="94"/>
-      <c r="B37" s="95" t="s">
-        <v>507</v>
-      </c>
-      <c r="C37" s="96"/>
-      <c r="D37" s="96"/>
-      <c r="E37" s="96"/>
-      <c r="F37" s="96"/>
-      <c r="G37" s="96"/>
-      <c r="H37" s="96"/>
-      <c r="I37" s="96"/>
-      <c r="J37" s="97"/>
+      <c r="B37" s="94"/>
+      <c r="C37" s="94"/>
+      <c r="D37" s="94"/>
+      <c r="E37" s="94"/>
+      <c r="F37" s="94"/>
+      <c r="G37" s="94"/>
+      <c r="H37" s="94"/>
+      <c r="I37" s="94"/>
+      <c r="J37" s="94"/>
       <c r="K37" s="94"/>
       <c r="L37" s="94"/>
-      <c r="M37" s="94" t="s">
-        <v>577</v>
-      </c>
+      <c r="M37" s="94"/>
       <c r="N37" s="94"/>
       <c r="O37" s="94"/>
       <c r="P37" s="94"/>
@@ -15692,24 +15623,20 @@
       <c r="T37" s="94"/>
       <c r="U37" s="94"/>
     </row>
-    <row r="38" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:21" s="93" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A38" s="94"/>
-      <c r="B38" s="98"/>
-      <c r="C38" s="99" t="s">
-        <v>469</v>
-      </c>
-      <c r="D38" s="100"/>
-      <c r="E38" s="100"/>
-      <c r="F38" s="100"/>
-      <c r="G38" s="100"/>
-      <c r="H38" s="100"/>
-      <c r="I38" s="100"/>
-      <c r="J38" s="101"/>
+      <c r="B38" s="94"/>
+      <c r="C38" s="94"/>
+      <c r="D38" s="94"/>
+      <c r="E38" s="94"/>
+      <c r="F38" s="94"/>
+      <c r="G38" s="94"/>
+      <c r="H38" s="94"/>
+      <c r="I38" s="94"/>
+      <c r="J38" s="94"/>
       <c r="K38" s="94"/>
       <c r="L38" s="94"/>
-      <c r="M38" s="94" t="s">
-        <v>578</v>
-      </c>
+      <c r="M38" s="94"/>
       <c r="N38" s="94"/>
       <c r="O38" s="94"/>
       <c r="P38" s="94"/>
@@ -15719,23 +15646,24 @@
       <c r="T38" s="94"/>
       <c r="U38" s="94"/>
     </row>
-    <row r="39" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:21" s="93" customFormat="1" ht="33.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A39" s="94"/>
-      <c r="B39" s="98"/>
-      <c r="C39" s="99" t="s">
-        <v>470</v>
-      </c>
-      <c r="D39" s="100"/>
-      <c r="E39" s="100"/>
-      <c r="F39" s="100"/>
-      <c r="G39" s="100"/>
-      <c r="H39" s="100"/>
-      <c r="I39" s="100"/>
-      <c r="J39" s="101"/>
+      <c r="B39" s="115">
+        <v>1</v>
+      </c>
+      <c r="C39" s="117" t="s">
+        <v>505</v>
+      </c>
+      <c r="D39" s="94"/>
+      <c r="E39" s="94"/>
+      <c r="F39" s="94"/>
+      <c r="G39" s="94"/>
+      <c r="H39" s="94"/>
+      <c r="I39" s="94"/>
+      <c r="J39" s="94"/>
+      <c r="K39" s="94"/>
       <c r="L39" s="94"/>
-      <c r="M39" s="94" t="s">
-        <v>579</v>
-      </c>
+      <c r="M39" s="94"/>
       <c r="N39" s="94"/>
       <c r="O39" s="94"/>
       <c r="P39" s="94"/>
@@ -15746,25 +15674,37 @@
       <c r="U39" s="94"/>
     </row>
     <row r="40" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="98"/>
-      <c r="C40" s="99" t="s">
-        <v>471</v>
-      </c>
-      <c r="D40" s="100"/>
-      <c r="E40" s="100"/>
-      <c r="F40" s="100"/>
-      <c r="G40" s="100"/>
-      <c r="H40" s="100"/>
-      <c r="I40" s="100"/>
-      <c r="J40" s="101"/>
-      <c r="M40" s="93" t="s">
-        <v>580</v>
-      </c>
+      <c r="A40" s="94"/>
+      <c r="B40" s="95" t="s">
+        <v>492</v>
+      </c>
+      <c r="C40" s="96"/>
+      <c r="D40" s="96"/>
+      <c r="E40" s="96"/>
+      <c r="F40" s="96"/>
+      <c r="G40" s="96"/>
+      <c r="H40" s="96"/>
+      <c r="I40" s="96"/>
+      <c r="J40" s="97"/>
+      <c r="K40" s="94"/>
+      <c r="L40" s="94"/>
+      <c r="M40" s="94" t="s">
+        <v>562</v>
+      </c>
+      <c r="N40" s="94"/>
+      <c r="O40" s="94"/>
+      <c r="P40" s="94"/>
+      <c r="Q40" s="94"/>
+      <c r="R40" s="94"/>
+      <c r="S40" s="94"/>
+      <c r="T40" s="94"/>
+      <c r="U40" s="94"/>
     </row>
     <row r="41" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="94"/>
       <c r="B41" s="98"/>
       <c r="C41" s="99" t="s">
-        <v>472</v>
+        <v>454</v>
       </c>
       <c r="D41" s="100"/>
       <c r="E41" s="100"/>
@@ -15773,14 +15713,25 @@
       <c r="H41" s="100"/>
       <c r="I41" s="100"/>
       <c r="J41" s="101"/>
-      <c r="M41" s="93" t="s">
-        <v>581</v>
-      </c>
+      <c r="K41" s="94"/>
+      <c r="L41" s="94"/>
+      <c r="M41" s="94" t="s">
+        <v>563</v>
+      </c>
+      <c r="N41" s="94"/>
+      <c r="O41" s="94"/>
+      <c r="P41" s="94"/>
+      <c r="Q41" s="94"/>
+      <c r="R41" s="94"/>
+      <c r="S41" s="94"/>
+      <c r="T41" s="94"/>
+      <c r="U41" s="94"/>
     </row>
     <row r="42" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="94"/>
       <c r="B42" s="98"/>
       <c r="C42" s="99" t="s">
-        <v>473</v>
+        <v>455</v>
       </c>
       <c r="D42" s="100"/>
       <c r="E42" s="100"/>
@@ -15789,11 +15740,23 @@
       <c r="H42" s="100"/>
       <c r="I42" s="100"/>
       <c r="J42" s="101"/>
+      <c r="L42" s="94"/>
+      <c r="M42" s="94" t="s">
+        <v>564</v>
+      </c>
+      <c r="N42" s="94"/>
+      <c r="O42" s="94"/>
+      <c r="P42" s="94"/>
+      <c r="Q42" s="94"/>
+      <c r="R42" s="94"/>
+      <c r="S42" s="94"/>
+      <c r="T42" s="94"/>
+      <c r="U42" s="94"/>
     </row>
     <row r="43" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B43" s="98"/>
       <c r="C43" s="99" t="s">
-        <v>474</v>
+        <v>456</v>
       </c>
       <c r="D43" s="100"/>
       <c r="E43" s="100"/>
@@ -15802,11 +15765,14 @@
       <c r="H43" s="100"/>
       <c r="I43" s="100"/>
       <c r="J43" s="101"/>
+      <c r="M43" s="93" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="44" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B44" s="98"/>
       <c r="C44" s="99" t="s">
-        <v>475</v>
+        <v>457</v>
       </c>
       <c r="D44" s="100"/>
       <c r="E44" s="100"/>
@@ -15815,11 +15781,14 @@
       <c r="H44" s="100"/>
       <c r="I44" s="100"/>
       <c r="J44" s="101"/>
+      <c r="M44" s="93" t="s">
+        <v>566</v>
+      </c>
     </row>
     <row r="45" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B45" s="98"/>
       <c r="C45" s="99" t="s">
-        <v>476</v>
+        <v>458</v>
       </c>
       <c r="D45" s="100"/>
       <c r="E45" s="100"/>
@@ -15832,7 +15801,7 @@
     <row r="46" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B46" s="98"/>
       <c r="C46" s="99" t="s">
-        <v>477</v>
+        <v>459</v>
       </c>
       <c r="D46" s="100"/>
       <c r="E46" s="100"/>
@@ -15845,7 +15814,7 @@
     <row r="47" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B47" s="98"/>
       <c r="C47" s="99" t="s">
-        <v>478</v>
+        <v>460</v>
       </c>
       <c r="D47" s="100"/>
       <c r="E47" s="100"/>
@@ -15858,7 +15827,7 @@
     <row r="48" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B48" s="98"/>
       <c r="C48" s="99" t="s">
-        <v>479</v>
+        <v>461</v>
       </c>
       <c r="D48" s="100"/>
       <c r="E48" s="100"/>
@@ -15868,10 +15837,10 @@
       <c r="I48" s="100"/>
       <c r="J48" s="101"/>
     </row>
-    <row r="49" spans="1:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B49" s="98"/>
       <c r="C49" s="99" t="s">
-        <v>480</v>
+        <v>462</v>
       </c>
       <c r="D49" s="100"/>
       <c r="E49" s="100"/>
@@ -15881,10 +15850,10 @@
       <c r="I49" s="100"/>
       <c r="J49" s="101"/>
     </row>
-    <row r="50" spans="1:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B50" s="98"/>
       <c r="C50" s="99" t="s">
-        <v>481</v>
+        <v>463</v>
       </c>
       <c r="D50" s="100"/>
       <c r="E50" s="100"/>
@@ -15894,10 +15863,10 @@
       <c r="I50" s="100"/>
       <c r="J50" s="101"/>
     </row>
-    <row r="51" spans="1:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B51" s="98"/>
       <c r="C51" s="99" t="s">
-        <v>476</v>
+        <v>464</v>
       </c>
       <c r="D51" s="100"/>
       <c r="E51" s="100"/>
@@ -15907,10 +15876,10 @@
       <c r="I51" s="100"/>
       <c r="J51" s="101"/>
     </row>
-    <row r="52" spans="1:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="2:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B52" s="98"/>
       <c r="C52" s="99" t="s">
-        <v>477</v>
+        <v>465</v>
       </c>
       <c r="D52" s="100"/>
       <c r="E52" s="100"/>
@@ -15920,10 +15889,10 @@
       <c r="I52" s="100"/>
       <c r="J52" s="101"/>
     </row>
-    <row r="53" spans="1:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="2:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B53" s="98"/>
       <c r="C53" s="99" t="s">
-        <v>478</v>
+        <v>466</v>
       </c>
       <c r="D53" s="100"/>
       <c r="E53" s="100"/>
@@ -15933,10 +15902,10 @@
       <c r="I53" s="100"/>
       <c r="J53" s="101"/>
     </row>
-    <row r="54" spans="1:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="2:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B54" s="98"/>
       <c r="C54" s="99" t="s">
-        <v>479</v>
+        <v>461</v>
       </c>
       <c r="D54" s="100"/>
       <c r="E54" s="100"/>
@@ -15946,10 +15915,10 @@
       <c r="I54" s="100"/>
       <c r="J54" s="101"/>
     </row>
-    <row r="55" spans="1:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B55" s="98"/>
       <c r="C55" s="99" t="s">
-        <v>480</v>
+        <v>462</v>
       </c>
       <c r="D55" s="100"/>
       <c r="E55" s="100"/>
@@ -15959,10 +15928,10 @@
       <c r="I55" s="100"/>
       <c r="J55" s="101"/>
     </row>
-    <row r="56" spans="1:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="2:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B56" s="98"/>
       <c r="C56" s="99" t="s">
-        <v>482</v>
+        <v>463</v>
       </c>
       <c r="D56" s="100"/>
       <c r="E56" s="100"/>
@@ -15972,10 +15941,10 @@
       <c r="I56" s="100"/>
       <c r="J56" s="101"/>
     </row>
-    <row r="57" spans="1:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="2:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B57" s="98"/>
       <c r="C57" s="99" t="s">
-        <v>483</v>
+        <v>464</v>
       </c>
       <c r="D57" s="100"/>
       <c r="E57" s="100"/>
@@ -15985,10 +15954,10 @@
       <c r="I57" s="100"/>
       <c r="J57" s="101"/>
     </row>
-    <row r="58" spans="1:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="2:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B58" s="98"/>
       <c r="C58" s="99" t="s">
-        <v>485</v>
+        <v>465</v>
       </c>
       <c r="D58" s="100"/>
       <c r="E58" s="100"/>
@@ -15998,10 +15967,10 @@
       <c r="I58" s="100"/>
       <c r="J58" s="101"/>
     </row>
-    <row r="59" spans="1:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="2:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B59" s="98"/>
       <c r="C59" s="99" t="s">
-        <v>486</v>
+        <v>467</v>
       </c>
       <c r="D59" s="100"/>
       <c r="E59" s="100"/>
@@ -16011,97 +15980,96 @@
       <c r="I59" s="100"/>
       <c r="J59" s="101"/>
     </row>
-    <row r="60" spans="1:10" s="93" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B60" s="102"/>
-      <c r="C60" s="103" t="s">
+    <row r="60" spans="2:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B60" s="98"/>
+      <c r="C60" s="99" t="s">
         <v>468</v>
       </c>
-      <c r="D60" s="104"/>
-      <c r="E60" s="104"/>
-      <c r="F60" s="104"/>
-      <c r="G60" s="104"/>
-      <c r="H60" s="104"/>
-      <c r="I60" s="104"/>
-      <c r="J60" s="105"/>
-    </row>
-    <row r="61" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B61" s="107"/>
-      <c r="C61" s="118"/>
-      <c r="D61" s="107"/>
-      <c r="E61" s="107"/>
-      <c r="F61" s="107"/>
-      <c r="G61" s="107"/>
-      <c r="H61" s="107"/>
-      <c r="I61" s="107"/>
-      <c r="J61" s="107"/>
-    </row>
-    <row r="62" spans="1:10" ht="33.75" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B62" s="120">
-        <v>2</v>
-      </c>
-      <c r="C62" s="119" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A63" s="107"/>
-      <c r="B63" s="95" t="s">
-        <v>508</v>
-      </c>
-      <c r="C63" s="96"/>
-      <c r="D63" s="96"/>
-      <c r="E63" s="96"/>
-      <c r="F63" s="96"/>
-      <c r="G63" s="96"/>
-      <c r="H63" s="96"/>
-      <c r="I63" s="96"/>
-      <c r="J63" s="97"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A64" s="107"/>
-      <c r="B64" s="106" t="s">
-        <v>510</v>
-      </c>
-      <c r="C64" s="107"/>
+      <c r="D60" s="100"/>
+      <c r="E60" s="100"/>
+      <c r="F60" s="100"/>
+      <c r="G60" s="100"/>
+      <c r="H60" s="100"/>
+      <c r="I60" s="100"/>
+      <c r="J60" s="101"/>
+    </row>
+    <row r="61" spans="2:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B61" s="98"/>
+      <c r="C61" s="99" t="s">
+        <v>470</v>
+      </c>
+      <c r="D61" s="100"/>
+      <c r="E61" s="100"/>
+      <c r="F61" s="100"/>
+      <c r="G61" s="100"/>
+      <c r="H61" s="100"/>
+      <c r="I61" s="100"/>
+      <c r="J61" s="101"/>
+    </row>
+    <row r="62" spans="2:10" s="93" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B62" s="98"/>
+      <c r="C62" s="99" t="s">
+        <v>471</v>
+      </c>
+      <c r="D62" s="100"/>
+      <c r="E62" s="100"/>
+      <c r="F62" s="100"/>
+      <c r="G62" s="100"/>
+      <c r="H62" s="100"/>
+      <c r="I62" s="100"/>
+      <c r="J62" s="101"/>
+    </row>
+    <row r="63" spans="2:10" s="93" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B63" s="102"/>
+      <c r="C63" s="103" t="s">
+        <v>453</v>
+      </c>
+      <c r="D63" s="104"/>
+      <c r="E63" s="104"/>
+      <c r="F63" s="104"/>
+      <c r="G63" s="104"/>
+      <c r="H63" s="104"/>
+      <c r="I63" s="104"/>
+      <c r="J63" s="105"/>
+    </row>
+    <row r="64" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B64" s="107"/>
+      <c r="C64" s="116"/>
       <c r="D64" s="107"/>
       <c r="E64" s="107"/>
       <c r="F64" s="107"/>
       <c r="G64" s="107"/>
       <c r="H64" s="107"/>
       <c r="I64" s="107"/>
-      <c r="J64" s="108"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A65" s="107"/>
-      <c r="B65" s="106"/>
-      <c r="C65" s="107" t="s">
-        <v>512</v>
-      </c>
-      <c r="D65" s="107"/>
-      <c r="E65" s="107"/>
-      <c r="F65" s="107"/>
-      <c r="G65" s="107"/>
-      <c r="H65" s="107"/>
-      <c r="I65" s="107"/>
-      <c r="J65" s="108"/>
+      <c r="J64" s="107"/>
+    </row>
+    <row r="65" spans="1:12" ht="33.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B65" s="118">
+        <v>2</v>
+      </c>
+      <c r="C65" s="117" t="s">
+        <v>509</v>
+      </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A66" s="107"/>
-      <c r="B66" s="106"/>
-      <c r="C66" s="107" t="s">
-        <v>511</v>
-      </c>
-      <c r="D66" s="107"/>
-      <c r="E66" s="107"/>
-      <c r="F66" s="107"/>
-      <c r="G66" s="107"/>
-      <c r="H66" s="107"/>
-      <c r="I66" s="107"/>
-      <c r="J66" s="108"/>
+      <c r="B66" s="95" t="s">
+        <v>493</v>
+      </c>
+      <c r="C66" s="96"/>
+      <c r="D66" s="96"/>
+      <c r="E66" s="96"/>
+      <c r="F66" s="96"/>
+      <c r="G66" s="96"/>
+      <c r="H66" s="96"/>
+      <c r="I66" s="96"/>
+      <c r="J66" s="97"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A67" s="107"/>
-      <c r="B67" s="106"/>
+      <c r="B67" s="106" t="s">
+        <v>495</v>
+      </c>
       <c r="C67" s="107"/>
       <c r="D67" s="107"/>
       <c r="E67" s="107"/>
@@ -16113,10 +16081,10 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A68" s="107"/>
-      <c r="B68" s="106" t="s">
-        <v>515</v>
-      </c>
-      <c r="C68" s="107"/>
+      <c r="B68" s="106"/>
+      <c r="C68" s="107" t="s">
+        <v>497</v>
+      </c>
       <c r="D68" s="107"/>
       <c r="E68" s="107"/>
       <c r="F68" s="107"/>
@@ -16129,7 +16097,7 @@
       <c r="A69" s="107"/>
       <c r="B69" s="106"/>
       <c r="C69" s="107" t="s">
-        <v>516</v>
+        <v>496</v>
       </c>
       <c r="D69" s="107"/>
       <c r="E69" s="107"/>
@@ -16142,9 +16110,7 @@
     <row r="70" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A70" s="107"/>
       <c r="B70" s="106"/>
-      <c r="C70" s="107" t="s">
-        <v>518</v>
-      </c>
+      <c r="C70" s="107"/>
       <c r="D70" s="107"/>
       <c r="E70" s="107"/>
       <c r="F70" s="107"/>
@@ -16155,7 +16121,9 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A71" s="107"/>
-      <c r="B71" s="106"/>
+      <c r="B71" s="106" t="s">
+        <v>500</v>
+      </c>
       <c r="C71" s="107"/>
       <c r="D71" s="107"/>
       <c r="E71" s="107"/>
@@ -16164,18 +16132,13 @@
       <c r="H71" s="107"/>
       <c r="I71" s="107"/>
       <c r="J71" s="108"/>
-      <c r="K71" s="94" t="s">
-        <v>519</v>
-      </c>
-      <c r="L71" s="94" t="s">
-        <v>519</v>
-      </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B72" s="106" t="s">
-        <v>513</v>
-      </c>
-      <c r="C72" s="107"/>
+      <c r="A72" s="107"/>
+      <c r="B72" s="106"/>
+      <c r="C72" s="107" t="s">
+        <v>501</v>
+      </c>
       <c r="D72" s="107"/>
       <c r="E72" s="107"/>
       <c r="F72" s="107"/>
@@ -16185,109 +16148,115 @@
       <c r="J72" s="108"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A73" s="107"/>
       <c r="B73" s="106"/>
       <c r="C73" s="107" t="s">
-        <v>517</v>
+        <v>503</v>
       </c>
       <c r="D73" s="107"/>
       <c r="E73" s="107"/>
       <c r="F73" s="107"/>
       <c r="G73" s="107"/>
       <c r="H73" s="107"/>
-      <c r="I73" s="107" t="s">
-        <v>521</v>
-      </c>
+      <c r="I73" s="107"/>
       <c r="J73" s="108"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A74" s="107"/>
       <c r="B74" s="106"/>
-      <c r="C74" s="107" t="s">
-        <v>509</v>
-      </c>
+      <c r="C74" s="107"/>
       <c r="D74" s="107"/>
       <c r="E74" s="107"/>
       <c r="F74" s="107"/>
       <c r="G74" s="107"/>
       <c r="H74" s="107"/>
-      <c r="I74" s="107" t="s">
-        <v>522</v>
-      </c>
+      <c r="I74" s="107"/>
       <c r="J74" s="108"/>
+      <c r="K74" s="94" t="s">
+        <v>504</v>
+      </c>
       <c r="L74" s="94" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B75" s="109"/>
-      <c r="C75" s="110" t="s">
-        <v>514</v>
-      </c>
-      <c r="D75" s="110"/>
-      <c r="E75" s="110"/>
-      <c r="F75" s="110"/>
-      <c r="G75" s="110"/>
-      <c r="H75" s="110"/>
-      <c r="I75" s="110" t="s">
-        <v>523</v>
-      </c>
-      <c r="J75" s="111" t="s">
-        <v>519</v>
-      </c>
+        <v>504</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B75" s="106" t="s">
+        <v>498</v>
+      </c>
+      <c r="C75" s="107"/>
+      <c r="D75" s="107"/>
+      <c r="E75" s="107"/>
+      <c r="F75" s="107"/>
+      <c r="G75" s="107"/>
+      <c r="H75" s="107"/>
+      <c r="I75" s="107"/>
+      <c r="J75" s="108"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B76" s="95"/>
-      <c r="C76" s="96"/>
-      <c r="D76" s="96"/>
-      <c r="E76" s="96"/>
-      <c r="F76" s="96"/>
-      <c r="G76" s="96"/>
-      <c r="H76" s="96"/>
-      <c r="I76" s="96"/>
-      <c r="J76" s="97"/>
+      <c r="B76" s="106"/>
+      <c r="C76" s="107" t="s">
+        <v>502</v>
+      </c>
+      <c r="D76" s="107"/>
+      <c r="E76" s="107"/>
+      <c r="F76" s="107"/>
+      <c r="G76" s="107"/>
+      <c r="H76" s="107"/>
+      <c r="I76" s="107" t="s">
+        <v>506</v>
+      </c>
+      <c r="J76" s="108"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B77" s="106"/>
-      <c r="C77" s="99" t="s">
-        <v>469</v>
+      <c r="C77" s="107" t="s">
+        <v>494</v>
       </c>
       <c r="D77" s="107"/>
       <c r="E77" s="107"/>
       <c r="F77" s="107"/>
       <c r="G77" s="107"/>
       <c r="H77" s="107"/>
-      <c r="I77" s="107"/>
+      <c r="I77" s="107" t="s">
+        <v>507</v>
+      </c>
       <c r="J77" s="108"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B78" s="106"/>
-      <c r="C78" s="99" t="s">
-        <v>525</v>
-      </c>
-      <c r="D78" s="107"/>
-      <c r="E78" s="107"/>
-      <c r="F78" s="107"/>
-      <c r="G78" s="107"/>
-      <c r="H78" s="107"/>
-      <c r="I78" s="107"/>
-      <c r="J78" s="108"/>
+      <c r="L77" s="94" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B78" s="109"/>
+      <c r="C78" s="110" t="s">
+        <v>499</v>
+      </c>
+      <c r="D78" s="110"/>
+      <c r="E78" s="110"/>
+      <c r="F78" s="110"/>
+      <c r="G78" s="110"/>
+      <c r="H78" s="110"/>
+      <c r="I78" s="110" t="s">
+        <v>508</v>
+      </c>
+      <c r="J78" s="111" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B79" s="106"/>
-      <c r="C79" s="99" t="s">
-        <v>526</v>
-      </c>
-      <c r="D79" s="107"/>
-      <c r="E79" s="107"/>
-      <c r="F79" s="107"/>
-      <c r="G79" s="107"/>
-      <c r="H79" s="107"/>
-      <c r="I79" s="107"/>
-      <c r="J79" s="108"/>
+      <c r="B79" s="95"/>
+      <c r="C79" s="96"/>
+      <c r="D79" s="96"/>
+      <c r="E79" s="96"/>
+      <c r="F79" s="96"/>
+      <c r="G79" s="96"/>
+      <c r="H79" s="96"/>
+      <c r="I79" s="96"/>
+      <c r="J79" s="97"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B80" s="106"/>
       <c r="C80" s="99" t="s">
-        <v>527</v>
+        <v>454</v>
       </c>
       <c r="D80" s="107"/>
       <c r="E80" s="107"/>
@@ -16300,7 +16269,7 @@
     <row r="81" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B81" s="106"/>
       <c r="C81" s="99" t="s">
-        <v>528</v>
+        <v>510</v>
       </c>
       <c r="D81" s="107"/>
       <c r="E81" s="107"/>
@@ -16313,7 +16282,7 @@
     <row r="82" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B82" s="106"/>
       <c r="C82" s="99" t="s">
-        <v>529</v>
+        <v>511</v>
       </c>
       <c r="D82" s="107"/>
       <c r="E82" s="107"/>
@@ -16326,7 +16295,7 @@
     <row r="83" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B83" s="106"/>
       <c r="C83" s="99" t="s">
-        <v>530</v>
+        <v>512</v>
       </c>
       <c r="D83" s="107"/>
       <c r="E83" s="107"/>
@@ -16339,7 +16308,7 @@
     <row r="84" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B84" s="106"/>
       <c r="C84" s="99" t="s">
-        <v>531</v>
+        <v>513</v>
       </c>
       <c r="D84" s="107"/>
       <c r="E84" s="107"/>
@@ -16352,7 +16321,7 @@
     <row r="85" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B85" s="106"/>
       <c r="C85" s="99" t="s">
-        <v>532</v>
+        <v>514</v>
       </c>
       <c r="D85" s="107"/>
       <c r="E85" s="107"/>
@@ -16365,7 +16334,7 @@
     <row r="86" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B86" s="106"/>
       <c r="C86" s="99" t="s">
-        <v>533</v>
+        <v>515</v>
       </c>
       <c r="D86" s="107"/>
       <c r="E86" s="107"/>
@@ -16378,7 +16347,7 @@
     <row r="87" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B87" s="106"/>
       <c r="C87" s="99" t="s">
-        <v>534</v>
+        <v>516</v>
       </c>
       <c r="D87" s="107"/>
       <c r="E87" s="107"/>
@@ -16391,7 +16360,7 @@
     <row r="88" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B88" s="106"/>
       <c r="C88" s="99" t="s">
-        <v>535</v>
+        <v>517</v>
       </c>
       <c r="D88" s="107"/>
       <c r="E88" s="107"/>
@@ -16404,7 +16373,7 @@
     <row r="89" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B89" s="106"/>
       <c r="C89" s="99" t="s">
-        <v>536</v>
+        <v>518</v>
       </c>
       <c r="D89" s="107"/>
       <c r="E89" s="107"/>
@@ -16417,7 +16386,7 @@
     <row r="90" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B90" s="106"/>
       <c r="C90" s="99" t="s">
-        <v>537</v>
+        <v>519</v>
       </c>
       <c r="D90" s="107"/>
       <c r="E90" s="107"/>
@@ -16430,7 +16399,7 @@
     <row r="91" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B91" s="106"/>
       <c r="C91" s="99" t="s">
-        <v>538</v>
+        <v>520</v>
       </c>
       <c r="D91" s="107"/>
       <c r="E91" s="107"/>
@@ -16443,7 +16412,7 @@
     <row r="92" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B92" s="106"/>
       <c r="C92" s="99" t="s">
-        <v>539</v>
+        <v>521</v>
       </c>
       <c r="D92" s="107"/>
       <c r="E92" s="107"/>
@@ -16456,7 +16425,7 @@
     <row r="93" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B93" s="106"/>
       <c r="C93" s="99" t="s">
-        <v>540</v>
+        <v>522</v>
       </c>
       <c r="D93" s="107"/>
       <c r="E93" s="107"/>
@@ -16469,7 +16438,7 @@
     <row r="94" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B94" s="106"/>
       <c r="C94" s="99" t="s">
-        <v>481</v>
+        <v>523</v>
       </c>
       <c r="D94" s="107"/>
       <c r="E94" s="107"/>
@@ -16482,7 +16451,7 @@
     <row r="95" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B95" s="106"/>
       <c r="C95" s="99" t="s">
-        <v>541</v>
+        <v>524</v>
       </c>
       <c r="D95" s="107"/>
       <c r="E95" s="107"/>
@@ -16495,7 +16464,7 @@
     <row r="96" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B96" s="106"/>
       <c r="C96" s="99" t="s">
-        <v>542</v>
+        <v>525</v>
       </c>
       <c r="D96" s="107"/>
       <c r="E96" s="107"/>
@@ -16508,7 +16477,7 @@
     <row r="97" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B97" s="106"/>
       <c r="C97" s="99" t="s">
-        <v>543</v>
+        <v>466</v>
       </c>
       <c r="D97" s="107"/>
       <c r="E97" s="107"/>
@@ -16521,7 +16490,7 @@
     <row r="98" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B98" s="106"/>
       <c r="C98" s="99" t="s">
-        <v>544</v>
+        <v>526</v>
       </c>
       <c r="D98" s="107"/>
       <c r="E98" s="107"/>
@@ -16534,7 +16503,7 @@
     <row r="99" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B99" s="106"/>
       <c r="C99" s="99" t="s">
-        <v>545</v>
+        <v>527</v>
       </c>
       <c r="D99" s="107"/>
       <c r="E99" s="107"/>
@@ -16547,7 +16516,7 @@
     <row r="100" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B100" s="106"/>
       <c r="C100" s="99" t="s">
-        <v>546</v>
+        <v>528</v>
       </c>
       <c r="D100" s="107"/>
       <c r="E100" s="107"/>
@@ -16560,7 +16529,7 @@
     <row r="101" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B101" s="106"/>
       <c r="C101" s="99" t="s">
-        <v>547</v>
+        <v>529</v>
       </c>
       <c r="D101" s="107"/>
       <c r="E101" s="107"/>
@@ -16573,7 +16542,7 @@
     <row r="102" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B102" s="106"/>
       <c r="C102" s="99" t="s">
-        <v>548</v>
+        <v>530</v>
       </c>
       <c r="D102" s="107"/>
       <c r="E102" s="107"/>
@@ -16586,7 +16555,7 @@
     <row r="103" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B103" s="106"/>
       <c r="C103" s="99" t="s">
-        <v>549</v>
+        <v>531</v>
       </c>
       <c r="D103" s="107"/>
       <c r="E103" s="107"/>
@@ -16599,7 +16568,7 @@
     <row r="104" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B104" s="106"/>
       <c r="C104" s="99" t="s">
-        <v>497</v>
+        <v>532</v>
       </c>
       <c r="D104" s="107"/>
       <c r="E104" s="107"/>
@@ -16612,7 +16581,7 @@
     <row r="105" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B105" s="106"/>
       <c r="C105" s="99" t="s">
-        <v>550</v>
+        <v>533</v>
       </c>
       <c r="D105" s="107"/>
       <c r="E105" s="107"/>
@@ -16625,7 +16594,7 @@
     <row r="106" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B106" s="106"/>
       <c r="C106" s="99" t="s">
-        <v>551</v>
+        <v>534</v>
       </c>
       <c r="D106" s="107"/>
       <c r="E106" s="107"/>
@@ -16638,7 +16607,7 @@
     <row r="107" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B107" s="106"/>
       <c r="C107" s="99" t="s">
-        <v>552</v>
+        <v>482</v>
       </c>
       <c r="D107" s="107"/>
       <c r="E107" s="107"/>
@@ -16651,7 +16620,7 @@
     <row r="108" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B108" s="106"/>
       <c r="C108" s="99" t="s">
-        <v>553</v>
+        <v>535</v>
       </c>
       <c r="D108" s="107"/>
       <c r="E108" s="107"/>
@@ -16664,7 +16633,7 @@
     <row r="109" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B109" s="106"/>
       <c r="C109" s="99" t="s">
-        <v>551</v>
+        <v>536</v>
       </c>
       <c r="D109" s="107"/>
       <c r="E109" s="107"/>
@@ -16677,7 +16646,7 @@
     <row r="110" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B110" s="106"/>
       <c r="C110" s="99" t="s">
-        <v>554</v>
+        <v>537</v>
       </c>
       <c r="D110" s="107"/>
       <c r="E110" s="107"/>
@@ -16690,7 +16659,7 @@
     <row r="111" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B111" s="106"/>
       <c r="C111" s="99" t="s">
-        <v>468</v>
+        <v>538</v>
       </c>
       <c r="D111" s="107"/>
       <c r="E111" s="107"/>
@@ -16700,81 +16669,81 @@
       <c r="I111" s="107"/>
       <c r="J111" s="108"/>
     </row>
-    <row r="112" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B112" s="109"/>
-      <c r="C112" s="110"/>
-      <c r="D112" s="110"/>
-      <c r="E112" s="110"/>
-      <c r="F112" s="110"/>
-      <c r="G112" s="110"/>
-      <c r="H112" s="110"/>
-      <c r="I112" s="110"/>
-      <c r="J112" s="111"/>
-    </row>
-    <row r="113" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="114" spans="2:10" ht="33.75" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B114" s="120">
+    <row r="112" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B112" s="106"/>
+      <c r="C112" s="99" t="s">
+        <v>536</v>
+      </c>
+      <c r="D112" s="107"/>
+      <c r="E112" s="107"/>
+      <c r="F112" s="107"/>
+      <c r="G112" s="107"/>
+      <c r="H112" s="107"/>
+      <c r="I112" s="107"/>
+      <c r="J112" s="108"/>
+    </row>
+    <row r="113" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B113" s="106"/>
+      <c r="C113" s="99" t="s">
+        <v>539</v>
+      </c>
+      <c r="D113" s="107"/>
+      <c r="E113" s="107"/>
+      <c r="F113" s="107"/>
+      <c r="G113" s="107"/>
+      <c r="H113" s="107"/>
+      <c r="I113" s="107"/>
+      <c r="J113" s="108"/>
+    </row>
+    <row r="114" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B114" s="106"/>
+      <c r="C114" s="99" t="s">
+        <v>453</v>
+      </c>
+      <c r="D114" s="107"/>
+      <c r="E114" s="107"/>
+      <c r="F114" s="107"/>
+      <c r="G114" s="107"/>
+      <c r="H114" s="107"/>
+      <c r="I114" s="107"/>
+      <c r="J114" s="108"/>
+    </row>
+    <row r="115" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B115" s="109"/>
+      <c r="C115" s="110"/>
+      <c r="D115" s="110"/>
+      <c r="E115" s="110"/>
+      <c r="F115" s="110"/>
+      <c r="G115" s="110"/>
+      <c r="H115" s="110"/>
+      <c r="I115" s="110"/>
+      <c r="J115" s="111"/>
+    </row>
+    <row r="116" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="117" spans="2:10" ht="33.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B117" s="118">
         <v>3</v>
       </c>
-      <c r="C114" s="94" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="115" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B115" s="129" t="s">
-        <v>555</v>
-      </c>
-      <c r="C115" s="130"/>
-      <c r="D115" s="130"/>
-      <c r="E115" s="130"/>
-      <c r="F115" s="130"/>
-      <c r="G115" s="130"/>
-      <c r="H115" s="130"/>
-      <c r="I115" s="130"/>
-      <c r="J115" s="131"/>
-    </row>
-    <row r="116" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B116" s="106" t="s">
-        <v>568</v>
-      </c>
-      <c r="C116" s="107"/>
-      <c r="D116" s="107"/>
-      <c r="E116" s="107"/>
-      <c r="F116" s="107"/>
-      <c r="G116" s="107"/>
-      <c r="H116" s="107"/>
-      <c r="I116" s="107"/>
-      <c r="J116" s="108"/>
-    </row>
-    <row r="117" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B117" s="115" t="s">
-        <v>469</v>
-      </c>
-      <c r="C117" s="107"/>
-      <c r="D117" s="107"/>
-      <c r="E117" s="107"/>
-      <c r="F117" s="107"/>
-      <c r="G117" s="107"/>
-      <c r="H117" s="107"/>
-      <c r="I117" s="107"/>
-      <c r="J117" s="108"/>
-    </row>
-    <row r="118" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B118" s="115" t="s">
-        <v>556</v>
-      </c>
-      <c r="C118" s="107"/>
-      <c r="D118" s="107"/>
-      <c r="E118" s="107"/>
-      <c r="F118" s="107"/>
-      <c r="G118" s="107"/>
-      <c r="H118" s="107"/>
-      <c r="I118" s="107"/>
-      <c r="J118" s="108"/>
+      <c r="C117" s="94" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="118" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B118" s="119" t="s">
+        <v>540</v>
+      </c>
+      <c r="C118" s="120"/>
+      <c r="D118" s="120"/>
+      <c r="E118" s="120"/>
+      <c r="F118" s="120"/>
+      <c r="G118" s="120"/>
+      <c r="H118" s="120"/>
+      <c r="I118" s="120"/>
+      <c r="J118" s="121"/>
     </row>
     <row r="119" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B119" s="115" t="s">
-        <v>557</v>
+      <c r="B119" s="106" t="s">
+        <v>553</v>
       </c>
       <c r="C119" s="107"/>
       <c r="D119" s="107"/>
@@ -16786,8 +16755,8 @@
       <c r="J119" s="108"/>
     </row>
     <row r="120" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B120" s="115" t="s">
-        <v>558</v>
+      <c r="B120" s="113" t="s">
+        <v>454</v>
       </c>
       <c r="C120" s="107"/>
       <c r="D120" s="107"/>
@@ -16799,8 +16768,8 @@
       <c r="J120" s="108"/>
     </row>
     <row r="121" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B121" s="115" t="s">
-        <v>559</v>
+      <c r="B121" s="113" t="s">
+        <v>541</v>
       </c>
       <c r="C121" s="107"/>
       <c r="D121" s="107"/>
@@ -16812,8 +16781,8 @@
       <c r="J121" s="108"/>
     </row>
     <row r="122" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B122" s="115" t="s">
-        <v>560</v>
+      <c r="B122" s="113" t="s">
+        <v>542</v>
       </c>
       <c r="C122" s="107"/>
       <c r="D122" s="107"/>
@@ -16825,8 +16794,8 @@
       <c r="J122" s="108"/>
     </row>
     <row r="123" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B123" s="115" t="s">
-        <v>561</v>
+      <c r="B123" s="113" t="s">
+        <v>543</v>
       </c>
       <c r="C123" s="107"/>
       <c r="D123" s="107"/>
@@ -16838,8 +16807,8 @@
       <c r="J123" s="108"/>
     </row>
     <row r="124" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B124" s="115" t="s">
-        <v>562</v>
+      <c r="B124" s="113" t="s">
+        <v>544</v>
       </c>
       <c r="C124" s="107"/>
       <c r="D124" s="107"/>
@@ -16851,8 +16820,8 @@
       <c r="J124" s="108"/>
     </row>
     <row r="125" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B125" s="115" t="s">
-        <v>497</v>
+      <c r="B125" s="113" t="s">
+        <v>545</v>
       </c>
       <c r="C125" s="107"/>
       <c r="D125" s="107"/>
@@ -16864,8 +16833,8 @@
       <c r="J125" s="108"/>
     </row>
     <row r="126" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B126" s="115" t="s">
-        <v>563</v>
+      <c r="B126" s="113" t="s">
+        <v>546</v>
       </c>
       <c r="C126" s="107"/>
       <c r="D126" s="107"/>
@@ -16877,8 +16846,8 @@
       <c r="J126" s="108"/>
     </row>
     <row r="127" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B127" s="115" t="s">
-        <v>557</v>
+      <c r="B127" s="113" t="s">
+        <v>547</v>
       </c>
       <c r="C127" s="107"/>
       <c r="D127" s="107"/>
@@ -16890,8 +16859,8 @@
       <c r="J127" s="108"/>
     </row>
     <row r="128" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B128" s="115" t="s">
-        <v>558</v>
+      <c r="B128" s="113" t="s">
+        <v>482</v>
       </c>
       <c r="C128" s="107"/>
       <c r="D128" s="107"/>
@@ -16903,8 +16872,8 @@
       <c r="J128" s="108"/>
     </row>
     <row r="129" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B129" s="115" t="s">
-        <v>559</v>
+      <c r="B129" s="113" t="s">
+        <v>548</v>
       </c>
       <c r="C129" s="107"/>
       <c r="D129" s="107"/>
@@ -16916,8 +16885,8 @@
       <c r="J129" s="108"/>
     </row>
     <row r="130" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B130" s="115" t="s">
-        <v>560</v>
+      <c r="B130" s="113" t="s">
+        <v>542</v>
       </c>
       <c r="C130" s="107"/>
       <c r="D130" s="107"/>
@@ -16929,8 +16898,8 @@
       <c r="J130" s="108"/>
     </row>
     <row r="131" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B131" s="115" t="s">
-        <v>561</v>
+      <c r="B131" s="113" t="s">
+        <v>543</v>
       </c>
       <c r="C131" s="107"/>
       <c r="D131" s="107"/>
@@ -16942,8 +16911,8 @@
       <c r="J131" s="108"/>
     </row>
     <row r="132" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B132" s="115" t="s">
-        <v>562</v>
+      <c r="B132" s="113" t="s">
+        <v>544</v>
       </c>
       <c r="C132" s="107"/>
       <c r="D132" s="107"/>
@@ -16955,8 +16924,8 @@
       <c r="J132" s="108"/>
     </row>
     <row r="133" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B133" s="115" t="s">
-        <v>564</v>
+      <c r="B133" s="113" t="s">
+        <v>545</v>
       </c>
       <c r="C133" s="107"/>
       <c r="D133" s="107"/>
@@ -16968,8 +16937,8 @@
       <c r="J133" s="108"/>
     </row>
     <row r="134" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B134" s="115" t="s">
-        <v>565</v>
+      <c r="B134" s="113" t="s">
+        <v>546</v>
       </c>
       <c r="C134" s="107"/>
       <c r="D134" s="107"/>
@@ -16981,8 +16950,8 @@
       <c r="J134" s="108"/>
     </row>
     <row r="135" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B135" s="115" t="s">
-        <v>557</v>
+      <c r="B135" s="113" t="s">
+        <v>547</v>
       </c>
       <c r="C135" s="107"/>
       <c r="D135" s="107"/>
@@ -16994,8 +16963,8 @@
       <c r="J135" s="108"/>
     </row>
     <row r="136" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B136" s="115" t="s">
-        <v>558</v>
+      <c r="B136" s="113" t="s">
+        <v>549</v>
       </c>
       <c r="C136" s="107"/>
       <c r="D136" s="107"/>
@@ -17007,8 +16976,8 @@
       <c r="J136" s="108"/>
     </row>
     <row r="137" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B137" s="115" t="s">
-        <v>559</v>
+      <c r="B137" s="113" t="s">
+        <v>550</v>
       </c>
       <c r="C137" s="107"/>
       <c r="D137" s="107"/>
@@ -17020,8 +16989,8 @@
       <c r="J137" s="108"/>
     </row>
     <row r="138" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B138" s="115" t="s">
-        <v>560</v>
+      <c r="B138" s="113" t="s">
+        <v>542</v>
       </c>
       <c r="C138" s="107"/>
       <c r="D138" s="107"/>
@@ -17033,8 +17002,8 @@
       <c r="J138" s="108"/>
     </row>
     <row r="139" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B139" s="115" t="s">
-        <v>561</v>
+      <c r="B139" s="113" t="s">
+        <v>543</v>
       </c>
       <c r="C139" s="107"/>
       <c r="D139" s="107"/>
@@ -17046,8 +17015,8 @@
       <c r="J139" s="108"/>
     </row>
     <row r="140" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B140" s="115" t="s">
-        <v>562</v>
+      <c r="B140" s="113" t="s">
+        <v>544</v>
       </c>
       <c r="C140" s="107"/>
       <c r="D140" s="107"/>
@@ -17059,8 +17028,8 @@
       <c r="J140" s="108"/>
     </row>
     <row r="141" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B141" s="115" t="s">
-        <v>566</v>
+      <c r="B141" s="113" t="s">
+        <v>545</v>
       </c>
       <c r="C141" s="107"/>
       <c r="D141" s="107"/>
@@ -17071,9 +17040,9 @@
       <c r="I141" s="107"/>
       <c r="J141" s="108"/>
     </row>
-    <row r="142" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B142" s="115" t="s">
-        <v>468</v>
+    <row r="142" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B142" s="113" t="s">
+        <v>546</v>
       </c>
       <c r="C142" s="107"/>
       <c r="D142" s="107"/>
@@ -17085,21 +17054,21 @@
       <c r="J142" s="108"/>
     </row>
     <row r="143" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B143" s="95" t="s">
-        <v>574</v>
-      </c>
-      <c r="C143" s="96"/>
-      <c r="D143" s="96"/>
-      <c r="E143" s="96"/>
-      <c r="F143" s="96"/>
-      <c r="G143" s="96"/>
-      <c r="H143" s="96"/>
-      <c r="I143" s="96"/>
-      <c r="J143" s="97"/>
+      <c r="B143" s="113" t="s">
+        <v>547</v>
+      </c>
+      <c r="C143" s="107"/>
+      <c r="D143" s="107"/>
+      <c r="E143" s="107"/>
+      <c r="F143" s="107"/>
+      <c r="G143" s="107"/>
+      <c r="H143" s="107"/>
+      <c r="I143" s="107"/>
+      <c r="J143" s="108"/>
     </row>
     <row r="144" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B144" s="115" t="s">
-        <v>469</v>
+      <c r="B144" s="113" t="s">
+        <v>551</v>
       </c>
       <c r="C144" s="107"/>
       <c r="D144" s="107"/>
@@ -17110,9 +17079,9 @@
       <c r="I144" s="107"/>
       <c r="J144" s="108"/>
     </row>
-    <row r="145" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B145" s="115" t="s">
-        <v>569</v>
+    <row r="145" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B145" s="113" t="s">
+        <v>453</v>
       </c>
       <c r="C145" s="107"/>
       <c r="D145" s="107"/>
@@ -17124,21 +17093,21 @@
       <c r="J145" s="108"/>
     </row>
     <row r="146" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B146" s="115" t="s">
-        <v>570</v>
-      </c>
-      <c r="C146" s="107"/>
-      <c r="D146" s="107"/>
-      <c r="E146" s="107"/>
-      <c r="F146" s="107"/>
-      <c r="G146" s="107"/>
-      <c r="H146" s="107"/>
-      <c r="I146" s="107"/>
-      <c r="J146" s="108"/>
+      <c r="B146" s="95" t="s">
+        <v>559</v>
+      </c>
+      <c r="C146" s="96"/>
+      <c r="D146" s="96"/>
+      <c r="E146" s="96"/>
+      <c r="F146" s="96"/>
+      <c r="G146" s="96"/>
+      <c r="H146" s="96"/>
+      <c r="I146" s="96"/>
+      <c r="J146" s="97"/>
     </row>
     <row r="147" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B147" s="115" t="s">
-        <v>571</v>
+      <c r="B147" s="113" t="s">
+        <v>454</v>
       </c>
       <c r="C147" s="107"/>
       <c r="D147" s="107"/>
@@ -17150,8 +17119,8 @@
       <c r="J147" s="108"/>
     </row>
     <row r="148" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B148" s="115" t="s">
-        <v>572</v>
+      <c r="B148" s="113" t="s">
+        <v>554</v>
       </c>
       <c r="C148" s="107"/>
       <c r="D148" s="107"/>
@@ -17163,8 +17132,8 @@
       <c r="J148" s="108"/>
     </row>
     <row r="149" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B149" s="115" t="s">
-        <v>573</v>
+      <c r="B149" s="113" t="s">
+        <v>555</v>
       </c>
       <c r="C149" s="107"/>
       <c r="D149" s="107"/>
@@ -17176,8 +17145,8 @@
       <c r="J149" s="108"/>
     </row>
     <row r="150" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B150" s="115" t="s">
-        <v>468</v>
+      <c r="B150" s="113" t="s">
+        <v>556</v>
       </c>
       <c r="C150" s="107"/>
       <c r="D150" s="107"/>
@@ -17188,71 +17157,77 @@
       <c r="I150" s="107"/>
       <c r="J150" s="108"/>
     </row>
-    <row r="151" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B151" s="109"/>
-      <c r="C151" s="110"/>
-      <c r="D151" s="110"/>
-      <c r="E151" s="110"/>
-      <c r="F151" s="110"/>
-      <c r="G151" s="110"/>
-      <c r="H151" s="110"/>
-      <c r="I151" s="110"/>
-      <c r="J151" s="111"/>
-    </row>
-    <row r="152" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="153" spans="2:10" ht="33.75" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B153" s="120">
+    <row r="151" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B151" s="113" t="s">
+        <v>557</v>
+      </c>
+      <c r="C151" s="107"/>
+      <c r="D151" s="107"/>
+      <c r="E151" s="107"/>
+      <c r="F151" s="107"/>
+      <c r="G151" s="107"/>
+      <c r="H151" s="107"/>
+      <c r="I151" s="107"/>
+      <c r="J151" s="108"/>
+    </row>
+    <row r="152" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B152" s="113" t="s">
+        <v>558</v>
+      </c>
+      <c r="C152" s="107"/>
+      <c r="D152" s="107"/>
+      <c r="E152" s="107"/>
+      <c r="F152" s="107"/>
+      <c r="G152" s="107"/>
+      <c r="H152" s="107"/>
+      <c r="I152" s="107"/>
+      <c r="J152" s="108"/>
+    </row>
+    <row r="153" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B153" s="113" t="s">
+        <v>453</v>
+      </c>
+      <c r="C153" s="107"/>
+      <c r="D153" s="107"/>
+      <c r="E153" s="107"/>
+      <c r="F153" s="107"/>
+      <c r="G153" s="107"/>
+      <c r="H153" s="107"/>
+      <c r="I153" s="107"/>
+      <c r="J153" s="108"/>
+    </row>
+    <row r="154" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B154" s="109"/>
+      <c r="C154" s="110"/>
+      <c r="D154" s="110"/>
+      <c r="E154" s="110"/>
+      <c r="F154" s="110"/>
+      <c r="G154" s="110"/>
+      <c r="H154" s="110"/>
+      <c r="I154" s="110"/>
+      <c r="J154" s="111"/>
+    </row>
+    <row r="155" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="156" spans="2:10" ht="33.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B156" s="118">
         <v>4</v>
       </c>
-      <c r="C153" s="94" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="154" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B154" s="95" t="s">
-        <v>575</v>
-      </c>
-      <c r="C154" s="96"/>
-      <c r="D154" s="96"/>
-      <c r="E154" s="96"/>
-      <c r="F154" s="96"/>
-      <c r="G154" s="96"/>
-      <c r="H154" s="96"/>
-      <c r="I154" s="96"/>
-      <c r="J154" s="97"/>
-    </row>
-    <row r="155" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B155" s="106"/>
-      <c r="C155" s="107"/>
-      <c r="D155" s="107"/>
-      <c r="E155" s="107"/>
-      <c r="F155" s="107"/>
-      <c r="G155" s="107"/>
-      <c r="H155" s="107"/>
-      <c r="I155" s="107"/>
-      <c r="J155" s="108"/>
-    </row>
-    <row r="156" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B156" s="106"/>
-      <c r="C156" s="107"/>
-      <c r="D156" s="107"/>
-      <c r="E156" s="107"/>
-      <c r="F156" s="107"/>
-      <c r="G156" s="107"/>
-      <c r="H156" s="107"/>
-      <c r="I156" s="107"/>
-      <c r="J156" s="108"/>
+      <c r="C156" s="94" t="s">
+        <v>561</v>
+      </c>
     </row>
     <row r="157" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B157" s="106"/>
-      <c r="C157" s="107"/>
-      <c r="D157" s="107"/>
-      <c r="E157" s="107"/>
-      <c r="F157" s="107"/>
-      <c r="G157" s="107"/>
-      <c r="H157" s="107"/>
-      <c r="I157" s="107"/>
-      <c r="J157" s="108"/>
+      <c r="B157" s="95" t="s">
+        <v>560</v>
+      </c>
+      <c r="C157" s="96"/>
+      <c r="D157" s="96"/>
+      <c r="E157" s="96"/>
+      <c r="F157" s="96"/>
+      <c r="G157" s="96"/>
+      <c r="H157" s="96"/>
+      <c r="I157" s="96"/>
+      <c r="J157" s="97"/>
     </row>
     <row r="158" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B158" s="106"/>
@@ -17331,51 +17306,101 @@
       <c r="I164" s="107"/>
       <c r="J164" s="108"/>
     </row>
-    <row r="165" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B165" s="109"/>
-      <c r="C165" s="110"/>
-      <c r="D165" s="110"/>
-      <c r="E165" s="110"/>
-      <c r="F165" s="110"/>
-      <c r="G165" s="110"/>
-      <c r="H165" s="110"/>
-      <c r="I165" s="110"/>
-      <c r="J165" s="111"/>
-    </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B180" s="94" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B181" s="94" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B182" s="153" t="s">
-        <v>589</v>
-      </c>
+    <row r="165" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B165" s="106"/>
+      <c r="C165" s="107"/>
+      <c r="D165" s="107"/>
+      <c r="E165" s="107"/>
+      <c r="F165" s="107"/>
+      <c r="G165" s="107"/>
+      <c r="H165" s="107"/>
+      <c r="I165" s="107"/>
+      <c r="J165" s="108"/>
+    </row>
+    <row r="166" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B166" s="106"/>
+      <c r="C166" s="107"/>
+      <c r="D166" s="107"/>
+      <c r="E166" s="107"/>
+      <c r="F166" s="107"/>
+      <c r="G166" s="107"/>
+      <c r="H166" s="107"/>
+      <c r="I166" s="107"/>
+      <c r="J166" s="108"/>
+    </row>
+    <row r="167" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B167" s="106"/>
+      <c r="C167" s="107"/>
+      <c r="D167" s="107"/>
+      <c r="E167" s="107"/>
+      <c r="F167" s="107"/>
+      <c r="G167" s="107"/>
+      <c r="H167" s="107"/>
+      <c r="I167" s="107"/>
+      <c r="J167" s="108"/>
+    </row>
+    <row r="168" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B168" s="109"/>
+      <c r="C168" s="110"/>
+      <c r="D168" s="110"/>
+      <c r="E168" s="110"/>
+      <c r="F168" s="110"/>
+      <c r="G168" s="110"/>
+      <c r="H168" s="110"/>
+      <c r="I168" s="110"/>
+      <c r="J168" s="111"/>
     </row>
     <row r="183" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B183" s="153"/>
+      <c r="B183" s="94" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="184" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B184" s="94" t="s">
+        <v>570</v>
+      </c>
     </row>
     <row r="185" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B185" s="94" t="s">
-        <v>588</v>
-      </c>
+      <c r="B185" s="122" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="186" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B186" s="122"/>
     </row>
     <row r="188" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B188" s="94" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B189" s="94" t="s">
-        <v>587</v>
+        <v>573</v>
+      </c>
+    </row>
+    <row r="191" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B191" s="94" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="192" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B192" s="94" t="s">
+        <v>572</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="L26:U26"/>
+    <mergeCell ref="L23:U23"/>
+    <mergeCell ref="L24:U24"/>
+    <mergeCell ref="L25:U25"/>
+    <mergeCell ref="L27:U27"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="C26:H26"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="C23:H23"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Requete avec REQ/RES LIVE DATA
</commit_message>
<xml_diff>
--- a/Cahier des charges/Organisation Projet Nodejs.xlsx
+++ b/Cahier des charges/Organisation Projet Nodejs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\MyEnv\NodeJs\Cahier des charges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA71DB5-8F22-4D1C-94E8-BE5F8CAF1546}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F36D94-FEFE-4980-96F8-348577B7F1E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="5" xr2:uid="{D1074EF0-41CD-437C-83BE-5015162961C9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="3" xr2:uid="{D1074EF0-41CD-437C-83BE-5015162961C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="591">
   <si>
     <t>Check bin sheet for more informations</t>
     <phoneticPr fontId="1"/>
@@ -5459,6 +5459,30 @@
   </si>
   <si>
     <t>a faire k</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Faire un projet qui genere des chats</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Apprendre les trucs a droite</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Refaire le projet de tracking version ameliorer</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Il faut que je recupere la plupart des infos par request</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Il faut que je supprime les trucs inutiles</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Il faut que le code soit mega simple</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -6685,6 +6709,21 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6739,28 +6778,22 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6772,16 +6805,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -12139,276 +12163,276 @@
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="2" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K2" s="123" t="s">
+      <c r="K2" s="128" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="124"/>
-      <c r="M2" s="124"/>
-      <c r="N2" s="124"/>
-      <c r="O2" s="124"/>
-      <c r="P2" s="124"/>
-      <c r="Q2" s="124"/>
-      <c r="R2" s="124"/>
-      <c r="S2" s="124"/>
-      <c r="T2" s="124"/>
-      <c r="U2" s="124"/>
-      <c r="V2" s="124"/>
-      <c r="W2" s="124"/>
-      <c r="X2" s="125"/>
+      <c r="L2" s="129"/>
+      <c r="M2" s="129"/>
+      <c r="N2" s="129"/>
+      <c r="O2" s="129"/>
+      <c r="P2" s="129"/>
+      <c r="Q2" s="129"/>
+      <c r="R2" s="129"/>
+      <c r="S2" s="129"/>
+      <c r="T2" s="129"/>
+      <c r="U2" s="129"/>
+      <c r="V2" s="129"/>
+      <c r="W2" s="129"/>
+      <c r="X2" s="130"/>
     </row>
     <row r="3" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K3" s="126"/>
-      <c r="L3" s="127"/>
-      <c r="M3" s="127"/>
-      <c r="N3" s="127"/>
-      <c r="O3" s="127"/>
-      <c r="P3" s="127"/>
-      <c r="Q3" s="127"/>
-      <c r="R3" s="127"/>
-      <c r="S3" s="127"/>
-      <c r="T3" s="127"/>
-      <c r="U3" s="127"/>
-      <c r="V3" s="127"/>
-      <c r="W3" s="127"/>
-      <c r="X3" s="128"/>
+      <c r="K3" s="131"/>
+      <c r="L3" s="132"/>
+      <c r="M3" s="132"/>
+      <c r="N3" s="132"/>
+      <c r="O3" s="132"/>
+      <c r="P3" s="132"/>
+      <c r="Q3" s="132"/>
+      <c r="R3" s="132"/>
+      <c r="S3" s="132"/>
+      <c r="T3" s="132"/>
+      <c r="U3" s="132"/>
+      <c r="V3" s="132"/>
+      <c r="W3" s="132"/>
+      <c r="X3" s="133"/>
     </row>
     <row r="6" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K6" s="123" t="s">
+      <c r="K6" s="128" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="124"/>
-      <c r="M6" s="124"/>
-      <c r="N6" s="124"/>
-      <c r="O6" s="124"/>
-      <c r="P6" s="124"/>
-      <c r="Q6" s="124"/>
-      <c r="R6" s="124"/>
-      <c r="S6" s="124"/>
-      <c r="T6" s="124"/>
-      <c r="U6" s="124"/>
-      <c r="V6" s="124"/>
-      <c r="W6" s="124"/>
-      <c r="X6" s="125"/>
+      <c r="L6" s="129"/>
+      <c r="M6" s="129"/>
+      <c r="N6" s="129"/>
+      <c r="O6" s="129"/>
+      <c r="P6" s="129"/>
+      <c r="Q6" s="129"/>
+      <c r="R6" s="129"/>
+      <c r="S6" s="129"/>
+      <c r="T6" s="129"/>
+      <c r="U6" s="129"/>
+      <c r="V6" s="129"/>
+      <c r="W6" s="129"/>
+      <c r="X6" s="130"/>
     </row>
     <row r="7" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K7" s="126"/>
-      <c r="L7" s="127"/>
-      <c r="M7" s="127"/>
-      <c r="N7" s="127"/>
-      <c r="O7" s="127"/>
-      <c r="P7" s="127"/>
-      <c r="Q7" s="127"/>
-      <c r="R7" s="127"/>
-      <c r="S7" s="127"/>
-      <c r="T7" s="127"/>
-      <c r="U7" s="127"/>
-      <c r="V7" s="127"/>
-      <c r="W7" s="127"/>
-      <c r="X7" s="128"/>
+      <c r="K7" s="131"/>
+      <c r="L7" s="132"/>
+      <c r="M7" s="132"/>
+      <c r="N7" s="132"/>
+      <c r="O7" s="132"/>
+      <c r="P7" s="132"/>
+      <c r="Q7" s="132"/>
+      <c r="R7" s="132"/>
+      <c r="S7" s="132"/>
+      <c r="T7" s="132"/>
+      <c r="U7" s="132"/>
+      <c r="V7" s="132"/>
+      <c r="W7" s="132"/>
+      <c r="X7" s="133"/>
     </row>
     <row r="10" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K10" s="129" t="s">
+      <c r="K10" s="134" t="s">
         <v>1</v>
       </c>
-      <c r="L10" s="130"/>
-      <c r="M10" s="130"/>
-      <c r="N10" s="130"/>
-      <c r="O10" s="130"/>
-      <c r="P10" s="130"/>
-      <c r="Q10" s="130"/>
-      <c r="R10" s="130"/>
-      <c r="S10" s="130"/>
-      <c r="T10" s="130"/>
-      <c r="U10" s="130"/>
-      <c r="V10" s="130"/>
-      <c r="W10" s="130"/>
-      <c r="X10" s="131"/>
+      <c r="L10" s="135"/>
+      <c r="M10" s="135"/>
+      <c r="N10" s="135"/>
+      <c r="O10" s="135"/>
+      <c r="P10" s="135"/>
+      <c r="Q10" s="135"/>
+      <c r="R10" s="135"/>
+      <c r="S10" s="135"/>
+      <c r="T10" s="135"/>
+      <c r="U10" s="135"/>
+      <c r="V10" s="135"/>
+      <c r="W10" s="135"/>
+      <c r="X10" s="136"/>
     </row>
     <row r="11" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K11" s="132"/>
-      <c r="L11" s="133"/>
-      <c r="M11" s="133"/>
-      <c r="N11" s="133"/>
-      <c r="O11" s="133"/>
-      <c r="P11" s="133"/>
-      <c r="Q11" s="133"/>
-      <c r="R11" s="133"/>
-      <c r="S11" s="133"/>
-      <c r="T11" s="133"/>
-      <c r="U11" s="133"/>
-      <c r="V11" s="133"/>
-      <c r="W11" s="133"/>
-      <c r="X11" s="134"/>
+      <c r="K11" s="137"/>
+      <c r="L11" s="138"/>
+      <c r="M11" s="138"/>
+      <c r="N11" s="138"/>
+      <c r="O11" s="138"/>
+      <c r="P11" s="138"/>
+      <c r="Q11" s="138"/>
+      <c r="R11" s="138"/>
+      <c r="S11" s="138"/>
+      <c r="T11" s="138"/>
+      <c r="U11" s="138"/>
+      <c r="V11" s="138"/>
+      <c r="W11" s="138"/>
+      <c r="X11" s="139"/>
     </row>
     <row r="14" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K14" s="123" t="s">
+      <c r="K14" s="128" t="s">
         <v>3</v>
       </c>
-      <c r="L14" s="124"/>
-      <c r="M14" s="124"/>
-      <c r="N14" s="124"/>
-      <c r="O14" s="124"/>
-      <c r="P14" s="124"/>
-      <c r="Q14" s="124"/>
-      <c r="R14" s="124"/>
-      <c r="S14" s="124"/>
-      <c r="T14" s="124"/>
-      <c r="U14" s="124"/>
-      <c r="V14" s="124"/>
-      <c r="W14" s="124"/>
-      <c r="X14" s="125"/>
+      <c r="L14" s="129"/>
+      <c r="M14" s="129"/>
+      <c r="N14" s="129"/>
+      <c r="O14" s="129"/>
+      <c r="P14" s="129"/>
+      <c r="Q14" s="129"/>
+      <c r="R14" s="129"/>
+      <c r="S14" s="129"/>
+      <c r="T14" s="129"/>
+      <c r="U14" s="129"/>
+      <c r="V14" s="129"/>
+      <c r="W14" s="129"/>
+      <c r="X14" s="130"/>
     </row>
     <row r="15" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K15" s="126"/>
-      <c r="L15" s="127"/>
-      <c r="M15" s="127"/>
-      <c r="N15" s="127"/>
-      <c r="O15" s="127"/>
-      <c r="P15" s="127"/>
-      <c r="Q15" s="127"/>
-      <c r="R15" s="127"/>
-      <c r="S15" s="127"/>
-      <c r="T15" s="127"/>
-      <c r="U15" s="127"/>
-      <c r="V15" s="127"/>
-      <c r="W15" s="127"/>
-      <c r="X15" s="128"/>
+      <c r="K15" s="131"/>
+      <c r="L15" s="132"/>
+      <c r="M15" s="132"/>
+      <c r="N15" s="132"/>
+      <c r="O15" s="132"/>
+      <c r="P15" s="132"/>
+      <c r="Q15" s="132"/>
+      <c r="R15" s="132"/>
+      <c r="S15" s="132"/>
+      <c r="T15" s="132"/>
+      <c r="U15" s="132"/>
+      <c r="V15" s="132"/>
+      <c r="W15" s="132"/>
+      <c r="X15" s="133"/>
     </row>
     <row r="18" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K18" s="123" t="s">
+      <c r="K18" s="128" t="s">
         <v>5</v>
       </c>
-      <c r="L18" s="124"/>
-      <c r="M18" s="124"/>
-      <c r="N18" s="124"/>
-      <c r="O18" s="124"/>
-      <c r="P18" s="124"/>
-      <c r="Q18" s="124"/>
-      <c r="R18" s="124"/>
-      <c r="S18" s="124"/>
-      <c r="T18" s="124"/>
-      <c r="U18" s="124"/>
-      <c r="V18" s="124"/>
-      <c r="W18" s="124"/>
-      <c r="X18" s="125"/>
+      <c r="L18" s="129"/>
+      <c r="M18" s="129"/>
+      <c r="N18" s="129"/>
+      <c r="O18" s="129"/>
+      <c r="P18" s="129"/>
+      <c r="Q18" s="129"/>
+      <c r="R18" s="129"/>
+      <c r="S18" s="129"/>
+      <c r="T18" s="129"/>
+      <c r="U18" s="129"/>
+      <c r="V18" s="129"/>
+      <c r="W18" s="129"/>
+      <c r="X18" s="130"/>
     </row>
     <row r="19" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K19" s="126"/>
-      <c r="L19" s="127"/>
-      <c r="M19" s="127"/>
-      <c r="N19" s="127"/>
-      <c r="O19" s="127"/>
-      <c r="P19" s="127"/>
-      <c r="Q19" s="127"/>
-      <c r="R19" s="127"/>
-      <c r="S19" s="127"/>
-      <c r="T19" s="127"/>
-      <c r="U19" s="127"/>
-      <c r="V19" s="127"/>
-      <c r="W19" s="127"/>
-      <c r="X19" s="128"/>
+      <c r="K19" s="131"/>
+      <c r="L19" s="132"/>
+      <c r="M19" s="132"/>
+      <c r="N19" s="132"/>
+      <c r="O19" s="132"/>
+      <c r="P19" s="132"/>
+      <c r="Q19" s="132"/>
+      <c r="R19" s="132"/>
+      <c r="S19" s="132"/>
+      <c r="T19" s="132"/>
+      <c r="U19" s="132"/>
+      <c r="V19" s="132"/>
+      <c r="W19" s="132"/>
+      <c r="X19" s="133"/>
     </row>
     <row r="22" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K22" s="123" t="s">
+      <c r="K22" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="L22" s="124"/>
-      <c r="M22" s="124"/>
-      <c r="N22" s="124"/>
-      <c r="O22" s="124"/>
-      <c r="P22" s="124"/>
-      <c r="Q22" s="124"/>
-      <c r="R22" s="124"/>
-      <c r="S22" s="124"/>
-      <c r="T22" s="124"/>
-      <c r="U22" s="124"/>
-      <c r="V22" s="124"/>
-      <c r="W22" s="124"/>
-      <c r="X22" s="125"/>
+      <c r="L22" s="129"/>
+      <c r="M22" s="129"/>
+      <c r="N22" s="129"/>
+      <c r="O22" s="129"/>
+      <c r="P22" s="129"/>
+      <c r="Q22" s="129"/>
+      <c r="R22" s="129"/>
+      <c r="S22" s="129"/>
+      <c r="T22" s="129"/>
+      <c r="U22" s="129"/>
+      <c r="V22" s="129"/>
+      <c r="W22" s="129"/>
+      <c r="X22" s="130"/>
     </row>
     <row r="23" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K23" s="126"/>
-      <c r="L23" s="127"/>
-      <c r="M23" s="127"/>
-      <c r="N23" s="127"/>
-      <c r="O23" s="127"/>
-      <c r="P23" s="127"/>
-      <c r="Q23" s="127"/>
-      <c r="R23" s="127"/>
-      <c r="S23" s="127"/>
-      <c r="T23" s="127"/>
-      <c r="U23" s="127"/>
-      <c r="V23" s="127"/>
-      <c r="W23" s="127"/>
-      <c r="X23" s="128"/>
+      <c r="K23" s="131"/>
+      <c r="L23" s="132"/>
+      <c r="M23" s="132"/>
+      <c r="N23" s="132"/>
+      <c r="O23" s="132"/>
+      <c r="P23" s="132"/>
+      <c r="Q23" s="132"/>
+      <c r="R23" s="132"/>
+      <c r="S23" s="132"/>
+      <c r="T23" s="132"/>
+      <c r="U23" s="132"/>
+      <c r="V23" s="132"/>
+      <c r="W23" s="132"/>
+      <c r="X23" s="133"/>
     </row>
     <row r="26" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K26" s="123" t="s">
+      <c r="K26" s="128" t="s">
         <v>7</v>
       </c>
-      <c r="L26" s="124"/>
-      <c r="M26" s="124"/>
-      <c r="N26" s="124"/>
-      <c r="O26" s="124"/>
-      <c r="P26" s="124"/>
-      <c r="Q26" s="124"/>
-      <c r="R26" s="124"/>
-      <c r="S26" s="124"/>
-      <c r="T26" s="124"/>
-      <c r="U26" s="124"/>
-      <c r="V26" s="124"/>
-      <c r="W26" s="124"/>
-      <c r="X26" s="125"/>
+      <c r="L26" s="129"/>
+      <c r="M26" s="129"/>
+      <c r="N26" s="129"/>
+      <c r="O26" s="129"/>
+      <c r="P26" s="129"/>
+      <c r="Q26" s="129"/>
+      <c r="R26" s="129"/>
+      <c r="S26" s="129"/>
+      <c r="T26" s="129"/>
+      <c r="U26" s="129"/>
+      <c r="V26" s="129"/>
+      <c r="W26" s="129"/>
+      <c r="X26" s="130"/>
     </row>
     <row r="27" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K27" s="126"/>
-      <c r="L27" s="127"/>
-      <c r="M27" s="127"/>
-      <c r="N27" s="127"/>
-      <c r="O27" s="127"/>
-      <c r="P27" s="127"/>
-      <c r="Q27" s="127"/>
-      <c r="R27" s="127"/>
-      <c r="S27" s="127"/>
-      <c r="T27" s="127"/>
-      <c r="U27" s="127"/>
-      <c r="V27" s="127"/>
-      <c r="W27" s="127"/>
-      <c r="X27" s="128"/>
+      <c r="K27" s="131"/>
+      <c r="L27" s="132"/>
+      <c r="M27" s="132"/>
+      <c r="N27" s="132"/>
+      <c r="O27" s="132"/>
+      <c r="P27" s="132"/>
+      <c r="Q27" s="132"/>
+      <c r="R27" s="132"/>
+      <c r="S27" s="132"/>
+      <c r="T27" s="132"/>
+      <c r="U27" s="132"/>
+      <c r="V27" s="132"/>
+      <c r="W27" s="132"/>
+      <c r="X27" s="133"/>
     </row>
     <row r="30" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K30" s="123" t="s">
+      <c r="K30" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="L30" s="124"/>
-      <c r="M30" s="124"/>
-      <c r="N30" s="124"/>
-      <c r="O30" s="124"/>
-      <c r="P30" s="124"/>
-      <c r="Q30" s="124"/>
-      <c r="R30" s="124"/>
-      <c r="S30" s="124"/>
-      <c r="T30" s="124"/>
-      <c r="U30" s="124"/>
-      <c r="V30" s="124"/>
-      <c r="W30" s="124"/>
-      <c r="X30" s="125"/>
+      <c r="L30" s="129"/>
+      <c r="M30" s="129"/>
+      <c r="N30" s="129"/>
+      <c r="O30" s="129"/>
+      <c r="P30" s="129"/>
+      <c r="Q30" s="129"/>
+      <c r="R30" s="129"/>
+      <c r="S30" s="129"/>
+      <c r="T30" s="129"/>
+      <c r="U30" s="129"/>
+      <c r="V30" s="129"/>
+      <c r="W30" s="129"/>
+      <c r="X30" s="130"/>
     </row>
     <row r="31" spans="11:24" x14ac:dyDescent="0.4">
-      <c r="K31" s="126"/>
-      <c r="L31" s="127"/>
-      <c r="M31" s="127"/>
-      <c r="N31" s="127"/>
-      <c r="O31" s="127"/>
-      <c r="P31" s="127"/>
-      <c r="Q31" s="127"/>
-      <c r="R31" s="127"/>
-      <c r="S31" s="127"/>
-      <c r="T31" s="127"/>
-      <c r="U31" s="127"/>
-      <c r="V31" s="127"/>
-      <c r="W31" s="127"/>
-      <c r="X31" s="128"/>
+      <c r="K31" s="131"/>
+      <c r="L31" s="132"/>
+      <c r="M31" s="132"/>
+      <c r="N31" s="132"/>
+      <c r="O31" s="132"/>
+      <c r="P31" s="132"/>
+      <c r="Q31" s="132"/>
+      <c r="R31" s="132"/>
+      <c r="S31" s="132"/>
+      <c r="T31" s="132"/>
+      <c r="U31" s="132"/>
+      <c r="V31" s="132"/>
+      <c r="W31" s="132"/>
+      <c r="X31" s="133"/>
     </row>
     <row r="38" spans="11:11" x14ac:dyDescent="0.4">
       <c r="K38" t="s">
@@ -12462,10 +12486,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1494C983-D6B3-4A8C-AA9C-1AD533947069}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:N91"/>
+  <dimension ref="A1:N126"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="F91" sqref="F91"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -12508,11 +12532,11 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="138" t="s">
+      <c r="A2" s="143" t="s">
         <v>188</v>
       </c>
-      <c r="B2" s="139"/>
-      <c r="C2" s="140"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="145"/>
       <c r="E2"/>
       <c r="H2"/>
       <c r="I2"/>
@@ -12634,11 +12658,11 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="135" t="s">
+      <c r="A7" s="140" t="s">
         <v>190</v>
       </c>
-      <c r="B7" s="136"/>
-      <c r="C7" s="137"/>
+      <c r="B7" s="141"/>
+      <c r="C7" s="142"/>
       <c r="E7"/>
       <c r="H7"/>
       <c r="I7"/>
@@ -13379,11 +13403,11 @@
       <c r="I34"/>
     </row>
     <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="135" t="s">
+      <c r="A35" s="140" t="s">
         <v>195</v>
       </c>
-      <c r="B35" s="136"/>
-      <c r="C35" s="137"/>
+      <c r="B35" s="141"/>
+      <c r="C35" s="142"/>
       <c r="E35"/>
       <c r="H35"/>
       <c r="I35"/>
@@ -13472,11 +13496,11 @@
       </c>
     </row>
     <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="135" t="s">
+      <c r="A39" s="140" t="s">
         <v>198</v>
       </c>
-      <c r="B39" s="136"/>
-      <c r="C39" s="137"/>
+      <c r="B39" s="141"/>
+      <c r="C39" s="142"/>
       <c r="E39"/>
       <c r="H39"/>
       <c r="I39"/>
@@ -13529,11 +13553,11 @@
       <c r="I41"/>
     </row>
     <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="135" t="s">
+      <c r="A42" s="140" t="s">
         <v>189</v>
       </c>
-      <c r="B42" s="136"/>
-      <c r="C42" s="137"/>
+      <c r="B42" s="141"/>
+      <c r="C42" s="142"/>
       <c r="E42"/>
       <c r="H42"/>
       <c r="I42"/>
@@ -13698,11 +13722,11 @@
       <c r="I48"/>
     </row>
     <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="135" t="s">
+      <c r="A49" s="140" t="s">
         <v>196</v>
       </c>
-      <c r="B49" s="136"/>
-      <c r="C49" s="137"/>
+      <c r="B49" s="141"/>
+      <c r="C49" s="142"/>
       <c r="E49"/>
       <c r="H49"/>
       <c r="I49"/>
@@ -13823,11 +13847,11 @@
       </c>
     </row>
     <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="135" t="s">
+      <c r="A54" s="140" t="s">
         <v>197</v>
       </c>
-      <c r="B54" s="136"/>
-      <c r="C54" s="137"/>
+      <c r="B54" s="141"/>
+      <c r="C54" s="142"/>
       <c r="E54"/>
       <c r="H54" s="19"/>
       <c r="I54"/>
@@ -14448,6 +14472,120 @@
     <row r="91" spans="1:9" ht="243.75" x14ac:dyDescent="0.4">
       <c r="F91" s="84" t="s">
         <v>425</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B108" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C108" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B109" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C109" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B110" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="C110" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="111" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B111" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="C111" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B112" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="C112" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B113" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="C113" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B114" s="30" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B115" s="30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B116" s="30" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B117" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B118" s="30" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B119" s="30" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B120" s="30" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B121" s="30" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B122" s="30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B123" s="30" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B124" s="30" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B125" s="30" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B126" s="30" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -14632,7 +14770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA67DCE-BBF2-410C-9E82-B8F1A39A9A5C}">
   <dimension ref="A1:U192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="E7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L26" sqref="L26:U26"/>
     </sheetView>
   </sheetViews>
@@ -15218,166 +15356,166 @@
     </row>
     <row r="23" spans="1:21" s="93" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="94"/>
-      <c r="B23" s="141">
+      <c r="B23" s="123">
         <v>1</v>
       </c>
-      <c r="C23" s="144" t="s">
+      <c r="C23" s="148" t="s">
         <v>445</v>
       </c>
-      <c r="D23" s="145"/>
-      <c r="E23" s="145"/>
-      <c r="F23" s="145"/>
-      <c r="G23" s="145"/>
-      <c r="H23" s="146"/>
-      <c r="I23" s="144" t="s">
+      <c r="D23" s="151"/>
+      <c r="E23" s="151"/>
+      <c r="F23" s="151"/>
+      <c r="G23" s="151"/>
+      <c r="H23" s="149"/>
+      <c r="I23" s="148" t="s">
         <v>446</v>
       </c>
-      <c r="J23" s="146"/>
-      <c r="K23" s="147" t="s">
+      <c r="J23" s="149"/>
+      <c r="K23" s="125" t="s">
         <v>447</v>
       </c>
-      <c r="L23" s="144" t="s">
+      <c r="L23" s="148" t="s">
         <v>568</v>
       </c>
-      <c r="M23" s="145"/>
-      <c r="N23" s="145"/>
-      <c r="O23" s="145"/>
-      <c r="P23" s="145"/>
-      <c r="Q23" s="145"/>
-      <c r="R23" s="145"/>
-      <c r="S23" s="145"/>
-      <c r="T23" s="145"/>
-      <c r="U23" s="146"/>
+      <c r="M23" s="151"/>
+      <c r="N23" s="151"/>
+      <c r="O23" s="151"/>
+      <c r="P23" s="151"/>
+      <c r="Q23" s="151"/>
+      <c r="R23" s="151"/>
+      <c r="S23" s="151"/>
+      <c r="T23" s="151"/>
+      <c r="U23" s="149"/>
     </row>
     <row r="24" spans="1:21" s="93" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="94"/>
-      <c r="B24" s="141">
+      <c r="B24" s="123">
         <v>2</v>
       </c>
-      <c r="C24" s="144" t="s">
+      <c r="C24" s="148" t="s">
         <v>443</v>
       </c>
-      <c r="D24" s="145"/>
-      <c r="E24" s="145"/>
-      <c r="F24" s="145"/>
-      <c r="G24" s="145"/>
-      <c r="H24" s="146"/>
-      <c r="I24" s="144" t="s">
+      <c r="D24" s="151"/>
+      <c r="E24" s="151"/>
+      <c r="F24" s="151"/>
+      <c r="G24" s="151"/>
+      <c r="H24" s="149"/>
+      <c r="I24" s="148" t="s">
         <v>451</v>
       </c>
-      <c r="J24" s="146"/>
-      <c r="K24" s="147" t="s">
+      <c r="J24" s="149"/>
+      <c r="K24" s="125" t="s">
         <v>447</v>
       </c>
-      <c r="L24" s="144" t="s">
+      <c r="L24" s="148" t="s">
         <v>567</v>
       </c>
-      <c r="M24" s="145"/>
-      <c r="N24" s="145"/>
-      <c r="O24" s="145"/>
-      <c r="P24" s="145"/>
-      <c r="Q24" s="145"/>
-      <c r="R24" s="145"/>
-      <c r="S24" s="145"/>
-      <c r="T24" s="145"/>
-      <c r="U24" s="146"/>
+      <c r="M24" s="151"/>
+      <c r="N24" s="151"/>
+      <c r="O24" s="151"/>
+      <c r="P24" s="151"/>
+      <c r="Q24" s="151"/>
+      <c r="R24" s="151"/>
+      <c r="S24" s="151"/>
+      <c r="T24" s="151"/>
+      <c r="U24" s="149"/>
     </row>
     <row r="25" spans="1:21" s="93" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="94"/>
-      <c r="B25" s="141">
+      <c r="B25" s="123">
         <v>3</v>
       </c>
-      <c r="C25" s="144" t="s">
+      <c r="C25" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="D25" s="145"/>
-      <c r="E25" s="145"/>
-      <c r="F25" s="145"/>
-      <c r="G25" s="145"/>
-      <c r="H25" s="146"/>
-      <c r="I25" s="144" t="s">
+      <c r="D25" s="151"/>
+      <c r="E25" s="151"/>
+      <c r="F25" s="151"/>
+      <c r="G25" s="151"/>
+      <c r="H25" s="149"/>
+      <c r="I25" s="148" t="s">
         <v>448</v>
       </c>
-      <c r="J25" s="146"/>
-      <c r="K25" s="148" t="s">
+      <c r="J25" s="149"/>
+      <c r="K25" s="126" t="s">
         <v>447</v>
       </c>
-      <c r="L25" s="149" t="s">
+      <c r="L25" s="152" t="s">
         <v>567</v>
       </c>
-      <c r="M25" s="150"/>
-      <c r="N25" s="150"/>
-      <c r="O25" s="150"/>
-      <c r="P25" s="150"/>
-      <c r="Q25" s="150"/>
-      <c r="R25" s="150"/>
-      <c r="S25" s="150"/>
-      <c r="T25" s="150"/>
-      <c r="U25" s="151"/>
+      <c r="M25" s="153"/>
+      <c r="N25" s="153"/>
+      <c r="O25" s="153"/>
+      <c r="P25" s="153"/>
+      <c r="Q25" s="153"/>
+      <c r="R25" s="153"/>
+      <c r="S25" s="153"/>
+      <c r="T25" s="153"/>
+      <c r="U25" s="154"/>
     </row>
     <row r="26" spans="1:21" s="93" customFormat="1" ht="132" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A26" s="94"/>
-      <c r="B26" s="142">
+      <c r="B26" s="124">
         <v>4</v>
       </c>
-      <c r="C26" s="152" t="s">
+      <c r="C26" s="146" t="s">
         <v>575</v>
       </c>
-      <c r="D26" s="153"/>
-      <c r="E26" s="153"/>
-      <c r="F26" s="153"/>
-      <c r="G26" s="153"/>
-      <c r="H26" s="154"/>
-      <c r="I26" s="152" t="s">
+      <c r="D26" s="155"/>
+      <c r="E26" s="155"/>
+      <c r="F26" s="155"/>
+      <c r="G26" s="155"/>
+      <c r="H26" s="147"/>
+      <c r="I26" s="146" t="s">
         <v>450</v>
       </c>
-      <c r="J26" s="154"/>
-      <c r="K26" s="155" t="s">
+      <c r="J26" s="147"/>
+      <c r="K26" s="127" t="s">
         <v>447</v>
       </c>
-      <c r="L26" s="143" t="s">
+      <c r="L26" s="150" t="s">
         <v>577</v>
       </c>
-      <c r="M26" s="143"/>
-      <c r="N26" s="143"/>
-      <c r="O26" s="143"/>
-      <c r="P26" s="143"/>
-      <c r="Q26" s="143"/>
-      <c r="R26" s="143"/>
-      <c r="S26" s="143"/>
-      <c r="T26" s="143"/>
-      <c r="U26" s="143"/>
+      <c r="M26" s="150"/>
+      <c r="N26" s="150"/>
+      <c r="O26" s="150"/>
+      <c r="P26" s="150"/>
+      <c r="Q26" s="150"/>
+      <c r="R26" s="150"/>
+      <c r="S26" s="150"/>
+      <c r="T26" s="150"/>
+      <c r="U26" s="150"/>
     </row>
     <row r="27" spans="1:21" s="93" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A27" s="94"/>
-      <c r="B27" s="142">
+      <c r="B27" s="124">
         <v>5</v>
       </c>
-      <c r="C27" s="152" t="s">
+      <c r="C27" s="146" t="s">
         <v>576</v>
       </c>
-      <c r="D27" s="153"/>
-      <c r="E27" s="153"/>
-      <c r="F27" s="153"/>
-      <c r="G27" s="153"/>
-      <c r="H27" s="154"/>
-      <c r="I27" s="152"/>
-      <c r="J27" s="154"/>
-      <c r="K27" s="155" t="s">
+      <c r="D27" s="155"/>
+      <c r="E27" s="155"/>
+      <c r="F27" s="155"/>
+      <c r="G27" s="155"/>
+      <c r="H27" s="147"/>
+      <c r="I27" s="146"/>
+      <c r="J27" s="147"/>
+      <c r="K27" s="127" t="s">
         <v>449</v>
       </c>
-      <c r="L27" s="152" t="s">
+      <c r="L27" s="146" t="s">
         <v>568</v>
       </c>
-      <c r="M27" s="153"/>
-      <c r="N27" s="153"/>
-      <c r="O27" s="153"/>
-      <c r="P27" s="153"/>
-      <c r="Q27" s="153"/>
-      <c r="R27" s="153"/>
-      <c r="S27" s="153"/>
-      <c r="T27" s="153"/>
-      <c r="U27" s="154"/>
+      <c r="M27" s="155"/>
+      <c r="N27" s="155"/>
+      <c r="O27" s="155"/>
+      <c r="P27" s="155"/>
+      <c r="Q27" s="155"/>
+      <c r="R27" s="155"/>
+      <c r="S27" s="155"/>
+      <c r="T27" s="155"/>
+      <c r="U27" s="147"/>
     </row>
     <row r="28" spans="1:21" s="93" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A28" s="94"/>
@@ -17385,21 +17523,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="C26:H26"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="L26:U26"/>
+    <mergeCell ref="L23:U23"/>
+    <mergeCell ref="L24:U24"/>
+    <mergeCell ref="L25:U25"/>
+    <mergeCell ref="L27:U27"/>
     <mergeCell ref="I27:J27"/>
     <mergeCell ref="I26:J26"/>
     <mergeCell ref="I23:J23"/>
     <mergeCell ref="I24:J24"/>
     <mergeCell ref="I25:J25"/>
-    <mergeCell ref="L26:U26"/>
-    <mergeCell ref="L23:U23"/>
-    <mergeCell ref="L24:U24"/>
-    <mergeCell ref="L25:U25"/>
-    <mergeCell ref="L27:U27"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="C26:H26"/>
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="C23:H23"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>